<commit_message>
Re-arranging & getting rid of old, unneeded files
</commit_message>
<xml_diff>
--- a/data/hake_input_yr24.xlsx
+++ b/data/hake_input_yr24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68571D3-9234-284D-AB63-9219E8E87590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4629EAC2-421D-1049-9B33-B4BBECF2B485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40960" yWindow="7700" windowWidth="34180" windowHeight="33360" firstSheet="4" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40960" yWindow="7700" windowWidth="34180" windowHeight="33360" firstSheet="4" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -26070,8 +26070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30463,7 +30463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S53" sqref="S53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Better organization for the project
</commit_message>
<xml_diff>
--- a/data/hake_input_yr24.xlsx
+++ b/data/hake_input_yr24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4629EAC2-421D-1049-9B33-B4BBECF2B485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F5BD62-9F41-F94B-B255-FC4C73D467D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40960" yWindow="7700" windowWidth="34180" windowHeight="33360" firstSheet="4" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2540" yWindow="15440" windowWidth="28280" windowHeight="24560" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="403">
   <si>
     <t>Number</t>
   </si>
@@ -26070,7 +26070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
@@ -33665,7 +33665,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33726,11 +33726,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>1318040</v>
       </c>
       <c r="I2">
-        <v>0.33478599999999997</v>
+        <v>0.351296</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -33813,11 +33813,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>1569148</v>
+      <c r="H5" s="2">
+        <v>1569150</v>
       </c>
       <c r="I5">
-        <v>0.29488599999999998</v>
+        <v>0.31139600000000001</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -33904,7 +33904,7 @@
         <v>861744</v>
       </c>
       <c r="I8">
-        <v>0.35088599999999998</v>
+        <v>0.367396</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -33958,11 +33958,11 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10">
-        <v>2137528</v>
+      <c r="H10" s="2">
+        <v>2137530</v>
       </c>
       <c r="I10">
-        <v>0.31078600000000001</v>
+        <v>0.32729599999999998</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -34016,11 +34016,11 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12">
-        <v>1376099</v>
+      <c r="H12" s="2">
+        <v>1376100</v>
       </c>
       <c r="I12">
-        <v>0.31048599999999998</v>
+        <v>0.32699600000000001</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -34078,7 +34078,7 @@
         <v>942721</v>
       </c>
       <c r="I14">
-        <v>0.32268599999999997</v>
+        <v>0.339196</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -34132,11 +34132,11 @@
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="H16">
-        <v>1502273</v>
+      <c r="H16" s="2">
+        <v>1502270</v>
       </c>
       <c r="I16">
-        <v>0.344586</v>
+        <v>0.36109599999999997</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -34194,7 +34194,7 @@
         <v>674617</v>
       </c>
       <c r="I18">
-        <v>0.36218600000000001</v>
+        <v>0.37869599999999998</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -34219,11 +34219,11 @@
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="H19">
-        <v>1279421</v>
+      <c r="H19" s="2">
+        <v>1279420</v>
       </c>
       <c r="I19">
-        <v>0.31358599999999998</v>
+        <v>0.330096</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -34248,11 +34248,11 @@
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="H20">
-        <v>1929235</v>
+      <c r="H20" s="2">
+        <v>1929240</v>
       </c>
       <c r="I20">
-        <v>0.310886</v>
+        <v>0.32739600000000002</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -34306,11 +34306,11 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="H22">
-        <v>2155853</v>
+      <c r="H22" s="2">
+        <v>2155850</v>
       </c>
       <c r="I22">
-        <v>0.32978600000000002</v>
+        <v>0.34629599999999999</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -34364,11 +34364,11 @@
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="H24">
-        <v>1417811</v>
+      <c r="H24" s="2">
+        <v>1417810</v>
       </c>
       <c r="I24">
-        <v>0.31208599999999997</v>
+        <v>0.328596</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -34422,11 +34422,11 @@
       <c r="G26">
         <v>1</v>
       </c>
-      <c r="H26">
-        <v>1722611</v>
+      <c r="H26" s="2">
+        <v>1718030</v>
       </c>
       <c r="I26">
-        <v>0.31078600000000001</v>
+        <v>0.32739600000000002</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -34451,6 +34451,12 @@
       <c r="G27">
         <v>1</v>
       </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -34474,6 +34480,12 @@
       <c r="G28">
         <v>1</v>
       </c>
+      <c r="H28" s="2">
+        <v>1524640</v>
+      </c>
+      <c r="I28">
+        <v>0.38739600000000002</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -34497,6 +34509,12 @@
       <c r="G29">
         <v>1</v>
       </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -34519,6 +34537,12 @@
       </c>
       <c r="G30">
         <v>1</v>
+      </c>
+      <c r="H30">
+        <v>907095</v>
+      </c>
+      <c r="I30">
+        <v>0.35149599999999998</v>
       </c>
     </row>
   </sheetData>
@@ -36453,10 +36477,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:DU54"/>
+  <dimension ref="A1:DU65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Y29" sqref="Y29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37767,7 +37791,7 @@
     </row>
     <row r="15" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -37782,63 +37806,63 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>1980</v>
+        <v>2021</v>
       </c>
       <c r="G15">
         <v>7</v>
       </c>
       <c r="H15">
-        <v>221</v>
+        <v>65</v>
       </c>
       <c r="I15">
-        <v>0.14799999999999999</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>0.54400000000000004</v>
+        <v>8.0256699999999999</v>
       </c>
       <c r="K15">
-        <v>30.087</v>
+        <v>5.7798699999999998</v>
       </c>
       <c r="L15">
-        <v>1.855</v>
+        <v>14.042299999999999</v>
       </c>
       <c r="M15">
-        <v>4.4880000000000004</v>
+        <v>28.2364</v>
       </c>
       <c r="N15">
-        <v>8.1649999999999991</v>
+        <v>3.4929000000000001</v>
       </c>
       <c r="O15">
-        <v>11.227</v>
+        <v>20.904499999999999</v>
       </c>
       <c r="P15">
-        <v>5.0119999999999996</v>
+        <v>3.0621399999999999</v>
       </c>
       <c r="Q15">
-        <v>8.9410000000000007</v>
+        <v>2.0468000000000002</v>
       </c>
       <c r="R15">
-        <v>11.076000000000001</v>
+        <v>1.9549000000000001</v>
       </c>
       <c r="S15">
-        <v>9.4600000000000009</v>
+        <v>9.9208499999999997</v>
       </c>
       <c r="T15">
-        <v>2.6280000000000001</v>
+        <v>1.4997199999999999</v>
       </c>
       <c r="U15">
-        <v>3.7850000000000001</v>
+        <v>0.31104100000000001</v>
       </c>
       <c r="V15">
-        <v>1.516</v>
+        <v>0.21940899999999999</v>
       </c>
       <c r="W15">
-        <v>1.0680000000000001</v>
+        <v>0.50351900000000005</v>
       </c>
     </row>
     <row r="16" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -37853,58 +37877,58 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>1981</v>
+        <v>2023</v>
       </c>
       <c r="G16">
         <v>7</v>
       </c>
       <c r="H16">
-        <v>154</v>
+        <v>64</v>
       </c>
       <c r="I16">
-        <v>19.492999999999999</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>4.03</v>
+        <v>50.580199999999998</v>
       </c>
       <c r="K16">
-        <v>1.403</v>
+        <v>24.6599</v>
       </c>
       <c r="L16">
-        <v>26.725999999999999</v>
+        <v>1.0310999999999999</v>
       </c>
       <c r="M16">
-        <v>3.9009999999999998</v>
+        <v>1.1721999999999999</v>
       </c>
       <c r="N16">
-        <v>5.548</v>
+        <v>2.9196</v>
       </c>
       <c r="O16">
-        <v>3.3759999999999999</v>
+        <v>8.0851000000000006</v>
       </c>
       <c r="P16">
-        <v>14.675000000000001</v>
+        <v>0.88080000000000003</v>
       </c>
       <c r="Q16">
-        <v>3.7690000000000001</v>
+        <v>5.3788999999999998</v>
       </c>
       <c r="R16">
-        <v>3.1949999999999998</v>
+        <v>0.76929999999999998</v>
       </c>
       <c r="S16">
-        <v>10.185</v>
+        <v>0.58309999999999995</v>
       </c>
       <c r="T16">
-        <v>2.3130000000000002</v>
+        <v>0.66979999999999995</v>
       </c>
       <c r="U16">
-        <v>0.504</v>
+        <v>2.2987000000000002</v>
       </c>
       <c r="V16">
-        <v>0.16300000000000001</v>
+        <v>0.40839999999999999</v>
       </c>
       <c r="W16">
-        <v>0.72</v>
+        <v>0.56279999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -37924,58 +37948,58 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>1982</v>
+        <v>1975</v>
       </c>
       <c r="G17">
         <v>7</v>
       </c>
       <c r="H17">
-        <v>170</v>
+        <v>13</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>4.6079999999999997</v>
       </c>
       <c r="J17">
-        <v>32.049999999999997</v>
+        <v>33.845999999999997</v>
       </c>
       <c r="K17">
-        <v>3.5209999999999999</v>
+        <v>7.4320000000000004</v>
       </c>
       <c r="L17">
-        <v>0.48599999999999999</v>
+        <v>1.248</v>
       </c>
       <c r="M17">
-        <v>27.347000000000001</v>
+        <v>25.396999999999998</v>
       </c>
       <c r="N17">
-        <v>1.526</v>
+        <v>5.5460000000000003</v>
       </c>
       <c r="O17">
-        <v>3.68</v>
+        <v>8.0310000000000006</v>
       </c>
       <c r="P17">
-        <v>3.8940000000000001</v>
+        <v>10.537000000000001</v>
       </c>
       <c r="Q17">
-        <v>11.763999999999999</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="R17">
-        <v>3.2679999999999998</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="S17">
-        <v>3.6110000000000002</v>
+        <v>0.871</v>
       </c>
       <c r="T17">
-        <v>7.6449999999999996</v>
+        <v>0.45100000000000001</v>
       </c>
       <c r="U17">
-        <v>0.24099999999999999</v>
+        <v>0</v>
       </c>
       <c r="V17">
-        <v>0.30199999999999999</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="W17">
-        <v>0.66400000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
@@ -37995,58 +38019,58 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>1983</v>
+        <v>1976</v>
       </c>
       <c r="G18">
         <v>7</v>
       </c>
       <c r="H18">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1.337</v>
       </c>
       <c r="K18">
-        <v>34.143999999999998</v>
+        <v>14.474</v>
       </c>
       <c r="L18">
-        <v>3.9969999999999999</v>
+        <v>6.742</v>
       </c>
       <c r="M18">
-        <v>1.825</v>
+        <v>4.0970000000000004</v>
       </c>
       <c r="N18">
-        <v>23.457999999999998</v>
+        <v>24.582000000000001</v>
       </c>
       <c r="O18">
-        <v>5.1260000000000003</v>
+        <v>9.766</v>
       </c>
       <c r="P18">
-        <v>5.6470000000000002</v>
+        <v>8.8989999999999991</v>
       </c>
       <c r="Q18">
-        <v>5.3</v>
+        <v>12.099</v>
       </c>
       <c r="R18">
-        <v>9.3829999999999991</v>
+        <v>5.431</v>
       </c>
       <c r="S18">
-        <v>3.91</v>
+        <v>4.3029999999999999</v>
       </c>
       <c r="T18">
-        <v>3.1280000000000001</v>
+        <v>4.0750000000000002</v>
       </c>
       <c r="U18">
-        <v>2.2589999999999999</v>
+        <v>1.0680000000000001</v>
       </c>
       <c r="V18">
-        <v>1.1299999999999999</v>
+        <v>2.355</v>
       </c>
       <c r="W18">
-        <v>0.69499999999999995</v>
+        <v>0.68700000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
@@ -38066,58 +38090,58 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1984</v>
+        <v>1977</v>
       </c>
       <c r="G19">
         <v>7</v>
       </c>
       <c r="H19">
-        <v>123</v>
+        <v>320</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>8.4480000000000004</v>
       </c>
       <c r="K19">
-        <v>1.393</v>
+        <v>3.6829999999999998</v>
       </c>
       <c r="L19">
-        <v>61.904000000000003</v>
+        <v>27.472999999999999</v>
       </c>
       <c r="M19">
-        <v>3.625</v>
+        <v>3.5939999999999999</v>
       </c>
       <c r="N19">
-        <v>3.8490000000000002</v>
+        <v>9.1059999999999999</v>
       </c>
       <c r="O19">
-        <v>16.777999999999999</v>
+        <v>22.681999999999999</v>
       </c>
       <c r="P19">
-        <v>2.8530000000000002</v>
+        <v>7.5990000000000002</v>
       </c>
       <c r="Q19">
-        <v>1.5089999999999999</v>
+        <v>6.5439999999999996</v>
       </c>
       <c r="R19">
-        <v>1.2390000000000001</v>
+        <v>4.016</v>
       </c>
       <c r="S19">
-        <v>3.3420000000000001</v>
+        <v>3.55</v>
       </c>
       <c r="T19">
-        <v>0.92300000000000004</v>
+        <v>2.3079999999999998</v>
       </c>
       <c r="U19">
-        <v>0.58599999999999997</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="V19">
-        <v>1.4390000000000001</v>
+        <v>0.308</v>
       </c>
       <c r="W19">
-        <v>0.56100000000000005</v>
+        <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
@@ -38137,58 +38161,58 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>1985</v>
+        <v>1978</v>
       </c>
       <c r="G20">
         <v>7</v>
       </c>
       <c r="H20">
-        <v>57</v>
+        <v>341</v>
       </c>
       <c r="I20">
-        <v>0.92500000000000004</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="J20">
-        <v>0.111</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="K20">
-        <v>0.34799999999999998</v>
+        <v>6.5110000000000001</v>
       </c>
       <c r="L20">
-        <v>7.2409999999999997</v>
+        <v>6.31</v>
       </c>
       <c r="M20">
-        <v>66.754999999999995</v>
+        <v>26.416</v>
       </c>
       <c r="N20">
-        <v>8.407</v>
+        <v>6.0910000000000002</v>
       </c>
       <c r="O20">
-        <v>5.6050000000000004</v>
+        <v>8.8680000000000003</v>
       </c>
       <c r="P20">
-        <v>7.1059999999999999</v>
+        <v>21.504999999999999</v>
       </c>
       <c r="Q20">
-        <v>2.0419999999999998</v>
+        <v>9.7759999999999998</v>
       </c>
       <c r="R20">
-        <v>0.53</v>
+        <v>4.7110000000000003</v>
       </c>
       <c r="S20">
-        <v>0.65400000000000003</v>
+        <v>4.68</v>
       </c>
       <c r="T20">
-        <v>0.246</v>
+        <v>2.339</v>
       </c>
       <c r="U20">
-        <v>0</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="V20">
-        <v>0</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="W20">
-        <v>3.2000000000000001E-2</v>
+        <v>0.33700000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
@@ -38208,58 +38232,58 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>1986</v>
+        <v>1979</v>
       </c>
       <c r="G21">
         <v>7</v>
       </c>
       <c r="H21">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21">
-        <v>15.343999999999999</v>
+        <v>6.492</v>
       </c>
       <c r="K21">
-        <v>5.3849999999999998</v>
+        <v>10.241</v>
       </c>
       <c r="L21">
-        <v>0.52700000000000002</v>
+        <v>9.3819999999999997</v>
       </c>
       <c r="M21">
-        <v>0.76100000000000001</v>
+        <v>5.7210000000000001</v>
       </c>
       <c r="N21">
-        <v>43.634</v>
+        <v>17.666</v>
       </c>
       <c r="O21">
-        <v>6.8970000000000002</v>
+        <v>10.256</v>
       </c>
       <c r="P21">
-        <v>8.1530000000000005</v>
+        <v>17.37</v>
       </c>
       <c r="Q21">
-        <v>8.26</v>
+        <v>12.762</v>
       </c>
       <c r="R21">
-        <v>2.1890000000000001</v>
+        <v>4.18</v>
       </c>
       <c r="S21">
-        <v>2.8170000000000002</v>
+        <v>2.8759999999999999</v>
       </c>
       <c r="T21">
-        <v>1.8340000000000001</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="U21">
-        <v>3.1339999999999999</v>
+        <v>1.645</v>
       </c>
       <c r="V21">
-        <v>0.45700000000000002</v>
+        <v>0</v>
       </c>
       <c r="W21">
-        <v>0.60899999999999999</v>
+        <v>0.44500000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
@@ -38279,58 +38303,58 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>1987</v>
+        <v>1980</v>
       </c>
       <c r="G22">
         <v>7</v>
       </c>
       <c r="H22">
-        <v>56</v>
+        <v>221</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="K22">
-        <v>29.582999999999998</v>
+        <v>30.087</v>
       </c>
       <c r="L22">
-        <v>2.9039999999999999</v>
+        <v>1.855</v>
       </c>
       <c r="M22">
-        <v>0.13500000000000001</v>
+        <v>4.4880000000000004</v>
       </c>
       <c r="N22">
-        <v>1.0129999999999999</v>
+        <v>8.1649999999999991</v>
       </c>
       <c r="O22">
-        <v>53.26</v>
+        <v>11.227</v>
       </c>
       <c r="P22">
-        <v>0.40400000000000003</v>
+        <v>5.0119999999999996</v>
       </c>
       <c r="Q22">
-        <v>1.25</v>
+        <v>8.9410000000000007</v>
       </c>
       <c r="R22">
-        <v>7.0910000000000002</v>
+        <v>11.076000000000001</v>
       </c>
       <c r="S22">
-        <v>0</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="T22">
-        <v>0.74399999999999999</v>
+        <v>2.6280000000000001</v>
       </c>
       <c r="U22">
-        <v>1.859</v>
+        <v>3.7850000000000001</v>
       </c>
       <c r="V22">
-        <v>1.7569999999999999</v>
+        <v>1.516</v>
       </c>
       <c r="W22">
-        <v>0</v>
+        <v>1.0680000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
@@ -38350,58 +38374,58 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>1988</v>
+        <v>1981</v>
       </c>
       <c r="G23">
         <v>7</v>
       </c>
       <c r="H23">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>19.492999999999999</v>
       </c>
       <c r="J23">
-        <v>0.65300000000000002</v>
+        <v>4.03</v>
       </c>
       <c r="K23">
-        <v>6.6000000000000003E-2</v>
+        <v>1.403</v>
       </c>
       <c r="L23">
-        <v>32.276000000000003</v>
+        <v>26.725999999999999</v>
       </c>
       <c r="M23">
-        <v>0.98</v>
+        <v>3.9009999999999998</v>
       </c>
       <c r="N23">
-        <v>1.45</v>
+        <v>5.548</v>
       </c>
       <c r="O23">
-        <v>0.66400000000000003</v>
+        <v>3.3759999999999999</v>
       </c>
       <c r="P23">
-        <v>46.045999999999999</v>
+        <v>14.675000000000001</v>
       </c>
       <c r="Q23">
-        <v>1.351</v>
+        <v>3.7690000000000001</v>
       </c>
       <c r="R23">
-        <v>0.83899999999999997</v>
+        <v>3.1949999999999998</v>
       </c>
       <c r="S23">
-        <v>10.483000000000001</v>
+        <v>10.185</v>
       </c>
       <c r="T23">
-        <v>0.78900000000000003</v>
+        <v>2.3130000000000002</v>
       </c>
       <c r="U23">
-        <v>5.3999999999999999E-2</v>
+        <v>0.504</v>
       </c>
       <c r="V23">
-        <v>6.5000000000000002E-2</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="W23">
-        <v>4.2830000000000004</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
@@ -38421,58 +38445,58 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>1989</v>
+        <v>1982</v>
       </c>
       <c r="G24">
         <v>7</v>
       </c>
       <c r="H24">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>5.6159999999999997</v>
+        <v>32.049999999999997</v>
       </c>
       <c r="K24">
-        <v>2.431</v>
+        <v>3.5209999999999999</v>
       </c>
       <c r="L24">
-        <v>0.28799999999999998</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="M24">
-        <v>50.206000000000003</v>
+        <v>27.347000000000001</v>
       </c>
       <c r="N24">
-        <v>1.2569999999999999</v>
+        <v>1.526</v>
       </c>
       <c r="O24">
-        <v>0.29199999999999998</v>
+        <v>3.68</v>
       </c>
       <c r="P24">
-        <v>8.4000000000000005E-2</v>
+        <v>3.8940000000000001</v>
       </c>
       <c r="Q24">
-        <v>35.192</v>
+        <v>11.763999999999999</v>
       </c>
       <c r="R24">
-        <v>1.802</v>
+        <v>3.2679999999999998</v>
       </c>
       <c r="S24">
-        <v>0.39500000000000002</v>
+        <v>3.6110000000000002</v>
       </c>
       <c r="T24">
-        <v>2.3159999999999998</v>
+        <v>7.6449999999999996</v>
       </c>
       <c r="U24">
-        <v>8.4000000000000005E-2</v>
+        <v>0.24099999999999999</v>
       </c>
       <c r="V24">
-        <v>0</v>
+        <v>0.30199999999999999</v>
       </c>
       <c r="W24">
-        <v>3.6999999999999998E-2</v>
+        <v>0.66400000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
@@ -38492,58 +38516,58 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>1990</v>
+        <v>1983</v>
       </c>
       <c r="G25">
         <v>7</v>
       </c>
       <c r="H25">
-        <v>163</v>
+        <v>117</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
-        <v>5.194</v>
+        <v>0</v>
       </c>
       <c r="K25">
-        <v>20.56</v>
+        <v>34.143999999999998</v>
       </c>
       <c r="L25">
-        <v>1.885</v>
+        <v>3.9969999999999999</v>
       </c>
       <c r="M25">
-        <v>0.59199999999999997</v>
+        <v>1.825</v>
       </c>
       <c r="N25">
-        <v>31.347999999999999</v>
+        <v>23.457999999999998</v>
       </c>
       <c r="O25">
-        <v>0.51200000000000001</v>
+        <v>5.1260000000000003</v>
       </c>
       <c r="P25">
-        <v>0.2</v>
+        <v>5.6470000000000002</v>
       </c>
       <c r="Q25">
-        <v>4.2000000000000003E-2</v>
+        <v>5.3</v>
       </c>
       <c r="R25">
-        <v>31.901</v>
+        <v>9.3829999999999991</v>
       </c>
       <c r="S25">
-        <v>0.29599999999999999</v>
+        <v>3.91</v>
       </c>
       <c r="T25">
-        <v>6.7000000000000004E-2</v>
+        <v>3.1280000000000001</v>
       </c>
       <c r="U25">
-        <v>6.4109999999999996</v>
+        <v>2.2589999999999999</v>
       </c>
       <c r="V25">
-        <v>0</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W25">
-        <v>0.99199999999999999</v>
+        <v>0.69499999999999995</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -38563,58 +38587,58 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>1991</v>
+        <v>1984</v>
       </c>
       <c r="G26">
         <v>7</v>
       </c>
       <c r="H26">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26">
-        <v>3.464</v>
+        <v>0</v>
       </c>
       <c r="K26">
-        <v>20.372</v>
+        <v>1.393</v>
       </c>
       <c r="L26">
-        <v>19.632000000000001</v>
+        <v>61.904000000000003</v>
       </c>
       <c r="M26">
-        <v>2.5219999999999998</v>
+        <v>3.625</v>
       </c>
       <c r="N26">
-        <v>0.79</v>
+        <v>3.8490000000000002</v>
       </c>
       <c r="O26">
-        <v>28.26</v>
+        <v>16.777999999999999</v>
       </c>
       <c r="P26">
-        <v>1.177</v>
+        <v>2.8530000000000002</v>
       </c>
       <c r="Q26">
-        <v>0.14499999999999999</v>
+        <v>1.5089999999999999</v>
       </c>
       <c r="R26">
-        <v>0.18099999999999999</v>
+        <v>1.2390000000000001</v>
       </c>
       <c r="S26">
-        <v>18.687999999999999</v>
+        <v>3.3420000000000001</v>
       </c>
       <c r="T26">
-        <v>0.42299999999999999</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="U26">
-        <v>0</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="V26">
-        <v>3.6059999999999999</v>
+        <v>1.4390000000000001</v>
       </c>
       <c r="W26">
-        <v>0.74099999999999999</v>
+        <v>0.56100000000000005</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
@@ -38634,58 +38658,58 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>1992</v>
+        <v>1985</v>
       </c>
       <c r="G27">
         <v>7</v>
       </c>
       <c r="H27">
-        <v>243</v>
+        <v>57</v>
       </c>
       <c r="I27">
-        <v>0.46100000000000002</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="J27">
-        <v>4.2380000000000004</v>
+        <v>0.111</v>
       </c>
       <c r="K27">
-        <v>4.3040000000000003</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="L27">
-        <v>13.053000000000001</v>
+        <v>7.2409999999999997</v>
       </c>
       <c r="M27">
-        <v>18.594000000000001</v>
+        <v>66.754999999999995</v>
       </c>
       <c r="N27">
-        <v>2.2709999999999999</v>
+        <v>8.407</v>
       </c>
       <c r="O27">
-        <v>1.0429999999999999</v>
+        <v>5.6050000000000004</v>
       </c>
       <c r="P27">
-        <v>33.926000000000002</v>
+        <v>7.1059999999999999</v>
       </c>
       <c r="Q27">
-        <v>0.76700000000000002</v>
+        <v>2.0419999999999998</v>
       </c>
       <c r="R27">
-        <v>7.8E-2</v>
+        <v>0.53</v>
       </c>
       <c r="S27">
-        <v>0.34</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="T27">
-        <v>18.05</v>
+        <v>0.246</v>
       </c>
       <c r="U27">
-        <v>0.41299999999999998</v>
+        <v>0</v>
       </c>
       <c r="V27">
-        <v>3.6999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="W27">
-        <v>2.4260000000000002</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
@@ -38705,58 +38729,58 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>1993</v>
+        <v>1986</v>
       </c>
       <c r="G28">
         <v>7</v>
       </c>
       <c r="H28">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="I28">
         <v>0</v>
       </c>
       <c r="J28">
-        <v>1.0509999999999999</v>
+        <v>15.343999999999999</v>
       </c>
       <c r="K28">
-        <v>23.24</v>
+        <v>5.3849999999999998</v>
       </c>
       <c r="L28">
-        <v>3.26</v>
+        <v>0.52700000000000002</v>
       </c>
       <c r="M28">
-        <v>12.98</v>
+        <v>0.76100000000000001</v>
       </c>
       <c r="N28">
-        <v>15.667</v>
+        <v>43.634</v>
       </c>
       <c r="O28">
-        <v>1.5</v>
+        <v>6.8970000000000002</v>
       </c>
       <c r="P28">
-        <v>0.81</v>
+        <v>8.1530000000000005</v>
       </c>
       <c r="Q28">
-        <v>27.422000000000001</v>
+        <v>8.26</v>
       </c>
       <c r="R28">
-        <v>0.67400000000000004</v>
+        <v>2.1890000000000001</v>
       </c>
       <c r="S28">
-        <v>8.8999999999999996E-2</v>
+        <v>2.8170000000000002</v>
       </c>
       <c r="T28">
-        <v>0.12</v>
+        <v>1.8340000000000001</v>
       </c>
       <c r="U28">
-        <v>12.004</v>
+        <v>3.1339999999999999</v>
       </c>
       <c r="V28">
-        <v>5.3999999999999999E-2</v>
+        <v>0.45700000000000002</v>
       </c>
       <c r="W28">
-        <v>1.129</v>
+        <v>0.60899999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
@@ -38776,58 +38800,58 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1994</v>
+        <v>1987</v>
       </c>
       <c r="G29">
         <v>7</v>
       </c>
       <c r="H29">
-        <v>235</v>
+        <v>56</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
       <c r="J29">
-        <v>3.6999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="K29">
-        <v>2.8319999999999999</v>
+        <v>29.582999999999998</v>
       </c>
       <c r="L29">
-        <v>21.39</v>
+        <v>2.9039999999999999</v>
       </c>
       <c r="M29">
-        <v>1.2649999999999999</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="N29">
-        <v>12.628</v>
+        <v>1.0129999999999999</v>
       </c>
       <c r="O29">
-        <v>18.687000000000001</v>
+        <v>53.26</v>
       </c>
       <c r="P29">
-        <v>1.571</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="Q29">
-        <v>0.57299999999999995</v>
+        <v>1.25</v>
       </c>
       <c r="R29">
-        <v>29.905999999999999</v>
+        <v>7.0910000000000002</v>
       </c>
       <c r="S29">
-        <v>0.26200000000000001</v>
+        <v>0</v>
       </c>
       <c r="T29">
-        <v>0.28199999999999997</v>
+        <v>0.74399999999999999</v>
       </c>
       <c r="U29">
-        <v>2.1999999999999999E-2</v>
+        <v>1.859</v>
       </c>
       <c r="V29">
-        <v>9.6340000000000003</v>
+        <v>1.7569999999999999</v>
       </c>
       <c r="W29">
-        <v>0.90900000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
@@ -38847,58 +38871,58 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>1995</v>
+        <v>1988</v>
       </c>
       <c r="G30">
         <v>7</v>
       </c>
       <c r="H30">
-        <v>147</v>
+        <v>84</v>
       </c>
       <c r="I30">
-        <v>0.61899999999999999</v>
+        <v>0</v>
       </c>
       <c r="J30">
-        <v>1.2809999999999999</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="K30">
-        <v>0.46800000000000003</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="L30">
-        <v>6.3079999999999998</v>
+        <v>32.276000000000003</v>
       </c>
       <c r="M30">
-        <v>28.966999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="N30">
-        <v>1.1519999999999999</v>
+        <v>1.45</v>
       </c>
       <c r="O30">
-        <v>8.0530000000000008</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="P30">
-        <v>20.268999999999998</v>
+        <v>46.045999999999999</v>
       </c>
       <c r="Q30">
-        <v>1.577</v>
+        <v>1.351</v>
       </c>
       <c r="R30">
-        <v>0.222</v>
+        <v>0.83899999999999997</v>
       </c>
       <c r="S30">
-        <v>22.423999999999999</v>
+        <v>10.483000000000001</v>
       </c>
       <c r="T30">
-        <v>0.435</v>
+        <v>0.78900000000000003</v>
       </c>
       <c r="U30">
-        <v>0.45100000000000001</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="V30">
-        <v>3.6999999999999998E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="W30">
-        <v>7.7350000000000003</v>
+        <v>4.2830000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
@@ -38918,58 +38942,58 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="G31">
         <v>7</v>
       </c>
       <c r="H31">
-        <v>186</v>
+        <v>80</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31">
-        <v>18.282</v>
+        <v>5.6159999999999997</v>
       </c>
       <c r="K31">
-        <v>16.242000000000001</v>
+        <v>2.431</v>
       </c>
       <c r="L31">
-        <v>1.506</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="M31">
-        <v>7.742</v>
+        <v>50.206000000000003</v>
       </c>
       <c r="N31">
-        <v>18.138999999999999</v>
+        <v>1.2569999999999999</v>
       </c>
       <c r="O31">
-        <v>1.002</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="P31">
-        <v>4.9089999999999998</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="Q31">
-        <v>10.981</v>
+        <v>35.192</v>
       </c>
       <c r="R31">
-        <v>0.57599999999999996</v>
+        <v>1.802</v>
       </c>
       <c r="S31">
-        <v>0.34699999999999998</v>
+        <v>0.39500000000000002</v>
       </c>
       <c r="T31">
-        <v>15.717000000000001</v>
+        <v>2.3159999999999998</v>
       </c>
       <c r="U31">
-        <v>8.9999999999999993E-3</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="V31">
-        <v>0.108</v>
+        <v>0</v>
       </c>
       <c r="W31">
-        <v>4.4390000000000001</v>
+        <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
@@ -38989,58 +39013,58 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>1997</v>
+        <v>1990</v>
       </c>
       <c r="G32">
         <v>7</v>
       </c>
       <c r="H32">
-        <v>220</v>
+        <v>163</v>
       </c>
       <c r="I32">
         <v>0</v>
       </c>
       <c r="J32">
-        <v>0.73699999999999999</v>
+        <v>5.194</v>
       </c>
       <c r="K32">
-        <v>29.474</v>
+        <v>20.56</v>
       </c>
       <c r="L32">
-        <v>24.952000000000002</v>
+        <v>1.885</v>
       </c>
       <c r="M32">
-        <v>1.4690000000000001</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="N32">
-        <v>7.8390000000000004</v>
+        <v>31.347999999999999</v>
       </c>
       <c r="O32">
-        <v>12.488</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="P32">
-        <v>1.798</v>
+        <v>0.2</v>
       </c>
       <c r="Q32">
-        <v>3.9780000000000002</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="R32">
-        <v>6.6710000000000003</v>
+        <v>31.901</v>
       </c>
       <c r="S32">
-        <v>1.284</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="T32">
-        <v>0.216</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="U32">
-        <v>6.08</v>
+        <v>6.4109999999999996</v>
       </c>
       <c r="V32">
-        <v>0.73299999999999998</v>
+        <v>0</v>
       </c>
       <c r="W32">
-        <v>2.282</v>
+        <v>0.99199999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
@@ -39060,58 +39084,58 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>1998</v>
+        <v>1991</v>
       </c>
       <c r="G33">
         <v>7</v>
       </c>
       <c r="H33">
-        <v>243</v>
+        <v>160</v>
       </c>
       <c r="I33">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>4.7789999999999999</v>
+        <v>3.464</v>
       </c>
       <c r="K33">
-        <v>20.335000000000001</v>
+        <v>20.372</v>
       </c>
       <c r="L33">
-        <v>20.294</v>
+        <v>19.632000000000001</v>
       </c>
       <c r="M33">
-        <v>26.596</v>
+        <v>2.5219999999999998</v>
       </c>
       <c r="N33">
-        <v>2.8679999999999999</v>
+        <v>0.79</v>
       </c>
       <c r="O33">
-        <v>5.4059999999999997</v>
+        <v>28.26</v>
       </c>
       <c r="P33">
-        <v>9.3119999999999994</v>
+        <v>1.177</v>
       </c>
       <c r="Q33">
-        <v>0.91700000000000004</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="R33">
-        <v>1.5609999999999999</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="S33">
-        <v>3.9009999999999998</v>
+        <v>18.687999999999999</v>
       </c>
       <c r="T33">
-        <v>0.35299999999999998</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="U33">
-        <v>9.1999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="V33">
-        <v>2.9420000000000002</v>
+        <v>3.6059999999999999</v>
       </c>
       <c r="W33">
-        <v>0.628</v>
+        <v>0.74099999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
@@ -39131,58 +39155,58 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>1999</v>
+        <v>1992</v>
       </c>
       <c r="G34">
         <v>7</v>
       </c>
       <c r="H34">
-        <v>509</v>
+        <v>243</v>
       </c>
       <c r="I34">
-        <v>6.2E-2</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="J34">
-        <v>10.244</v>
+        <v>4.2380000000000004</v>
       </c>
       <c r="K34">
-        <v>20.364000000000001</v>
+        <v>4.3040000000000003</v>
       </c>
       <c r="L34">
-        <v>17.981999999999999</v>
+        <v>13.053000000000001</v>
       </c>
       <c r="M34">
-        <v>20.062000000000001</v>
+        <v>18.594000000000001</v>
       </c>
       <c r="N34">
-        <v>13.198</v>
+        <v>2.2709999999999999</v>
       </c>
       <c r="O34">
-        <v>2.6880000000000002</v>
+        <v>1.0429999999999999</v>
       </c>
       <c r="P34">
-        <v>3.93</v>
+        <v>33.926000000000002</v>
       </c>
       <c r="Q34">
-        <v>4.008</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="R34">
-        <v>0.98899999999999999</v>
+        <v>7.8E-2</v>
       </c>
       <c r="S34">
-        <v>1.542</v>
+        <v>0.34</v>
       </c>
       <c r="T34">
-        <v>2.14</v>
+        <v>18.05</v>
       </c>
       <c r="U34">
-        <v>0.39200000000000002</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="V34">
-        <v>0.33400000000000002</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="W34">
-        <v>2.0659999999999998</v>
+        <v>2.4260000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
@@ -39202,58 +39226,58 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>2000</v>
+        <v>1993</v>
       </c>
       <c r="G35">
         <v>7</v>
       </c>
       <c r="H35">
-        <v>530</v>
+        <v>172</v>
       </c>
       <c r="I35">
-        <v>0.996</v>
+        <v>0</v>
       </c>
       <c r="J35">
-        <v>4.218</v>
+        <v>1.0509999999999999</v>
       </c>
       <c r="K35">
-        <v>10.935</v>
+        <v>23.24</v>
       </c>
       <c r="L35">
-        <v>14.285</v>
+        <v>3.26</v>
       </c>
       <c r="M35">
-        <v>12.88</v>
+        <v>12.98</v>
       </c>
       <c r="N35">
-        <v>21.062999999999999</v>
+        <v>15.667</v>
       </c>
       <c r="O35">
-        <v>13.115</v>
+        <v>1.5</v>
       </c>
       <c r="P35">
-        <v>6.548</v>
+        <v>0.81</v>
       </c>
       <c r="Q35">
-        <v>4.6479999999999997</v>
+        <v>27.422000000000001</v>
       </c>
       <c r="R35">
-        <v>2.5089999999999999</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="S35">
-        <v>2.0699999999999998</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="T35">
-        <v>2.306</v>
+        <v>0.12</v>
       </c>
       <c r="U35">
-        <v>1.292</v>
+        <v>12.004</v>
       </c>
       <c r="V35">
-        <v>0.72</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="W35">
-        <v>2.4140000000000001</v>
+        <v>1.129</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
@@ -39273,58 +39297,58 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>2001</v>
+        <v>1994</v>
       </c>
       <c r="G36">
         <v>7</v>
       </c>
       <c r="H36">
-        <v>540</v>
+        <v>235</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
       <c r="J36">
-        <v>17.338000000000001</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="K36">
-        <v>16.247</v>
+        <v>2.8319999999999999</v>
       </c>
       <c r="L36">
-        <v>14.25</v>
+        <v>21.39</v>
       </c>
       <c r="M36">
-        <v>15.685</v>
+        <v>1.2649999999999999</v>
       </c>
       <c r="N36">
-        <v>8.5589999999999993</v>
+        <v>12.628</v>
       </c>
       <c r="O36">
-        <v>12.101000000000001</v>
+        <v>18.687000000000001</v>
       </c>
       <c r="P36">
-        <v>5.9889999999999999</v>
+        <v>1.571</v>
       </c>
       <c r="Q36">
-        <v>1.778</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="R36">
-        <v>2.2320000000000002</v>
+        <v>29.905999999999999</v>
       </c>
       <c r="S36">
-        <v>1.81</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="T36">
-        <v>0.69799999999999995</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="U36">
-        <v>1.421</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="V36">
-        <v>0.68500000000000005</v>
+        <v>9.6340000000000003</v>
       </c>
       <c r="W36">
-        <v>1.2090000000000001</v>
+        <v>0.90900000000000003</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
@@ -39344,58 +39368,58 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="G37">
         <v>7</v>
       </c>
       <c r="H37">
-        <v>449</v>
+        <v>147</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="J37">
-        <v>3.3000000000000002E-2</v>
+        <v>1.2809999999999999</v>
       </c>
       <c r="K37">
-        <v>50.642000000000003</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="L37">
-        <v>14.933999999999999</v>
+        <v>6.3079999999999998</v>
       </c>
       <c r="M37">
-        <v>9.6869999999999994</v>
+        <v>28.966999999999999</v>
       </c>
       <c r="N37">
-        <v>5.7190000000000003</v>
+        <v>1.1519999999999999</v>
       </c>
       <c r="O37">
-        <v>4.4379999999999997</v>
+        <v>8.0530000000000008</v>
       </c>
       <c r="P37">
-        <v>6.58</v>
+        <v>20.268999999999998</v>
       </c>
       <c r="Q37">
-        <v>3.5459999999999998</v>
+        <v>1.577</v>
       </c>
       <c r="R37">
-        <v>0.871</v>
+        <v>0.222</v>
       </c>
       <c r="S37">
-        <v>0.84499999999999997</v>
+        <v>22.423999999999999</v>
       </c>
       <c r="T37">
-        <v>1.036</v>
+        <v>0.435</v>
       </c>
       <c r="U37">
-        <v>0.24199999999999999</v>
+        <v>0.45100000000000001</v>
       </c>
       <c r="V37">
-        <v>0.47499999999999998</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="W37">
-        <v>0.95299999999999996</v>
+        <v>7.7350000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
@@ -39415,58 +39439,58 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>2003</v>
+        <v>1996</v>
       </c>
       <c r="G38">
         <v>7</v>
       </c>
       <c r="H38">
-        <v>456</v>
+        <v>186</v>
       </c>
       <c r="I38">
         <v>0</v>
       </c>
       <c r="J38">
-        <v>0.105</v>
+        <v>18.282</v>
       </c>
       <c r="K38">
-        <v>1.3939999999999999</v>
+        <v>16.242000000000001</v>
       </c>
       <c r="L38">
-        <v>67.790999999999997</v>
+        <v>1.506</v>
       </c>
       <c r="M38">
-        <v>11.664</v>
+        <v>7.742</v>
       </c>
       <c r="N38">
-        <v>3.3519999999999999</v>
+        <v>18.138999999999999</v>
       </c>
       <c r="O38">
-        <v>5.0090000000000003</v>
+        <v>1.002</v>
       </c>
       <c r="P38">
-        <v>3.2029999999999998</v>
+        <v>4.9089999999999998</v>
       </c>
       <c r="Q38">
-        <v>3.153</v>
+        <v>10.981</v>
       </c>
       <c r="R38">
-        <v>2.1190000000000002</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="S38">
-        <v>0.879</v>
+        <v>0.34699999999999998</v>
       </c>
       <c r="T38">
-        <v>0.438</v>
+        <v>15.717000000000001</v>
       </c>
       <c r="U38">
-        <v>0.53600000000000003</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="V38">
-        <v>0.126</v>
+        <v>0.108</v>
       </c>
       <c r="W38">
-        <v>0.23200000000000001</v>
+        <v>4.4390000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
@@ -39486,58 +39510,58 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>2004</v>
+        <v>1997</v>
       </c>
       <c r="G39">
         <v>7</v>
       </c>
       <c r="H39">
-        <v>501</v>
+        <v>220</v>
       </c>
       <c r="I39">
         <v>0</v>
       </c>
       <c r="J39">
-        <v>2.1999999999999999E-2</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="K39">
-        <v>5.343</v>
+        <v>29.474</v>
       </c>
       <c r="L39">
-        <v>6.1260000000000003</v>
+        <v>24.952000000000002</v>
       </c>
       <c r="M39">
-        <v>68.293000000000006</v>
+        <v>1.4690000000000001</v>
       </c>
       <c r="N39">
-        <v>8.1150000000000002</v>
+        <v>7.8390000000000004</v>
       </c>
       <c r="O39">
-        <v>2.1779999999999999</v>
+        <v>12.488</v>
       </c>
       <c r="P39">
-        <v>4.133</v>
+        <v>1.798</v>
       </c>
       <c r="Q39">
-        <v>2.5059999999999998</v>
+        <v>3.9780000000000002</v>
       </c>
       <c r="R39">
-        <v>1.27</v>
+        <v>6.6710000000000003</v>
       </c>
       <c r="S39">
-        <v>1.073</v>
+        <v>1.284</v>
       </c>
       <c r="T39">
-        <v>0.34599999999999997</v>
+        <v>0.216</v>
       </c>
       <c r="U39">
-        <v>0.26800000000000002</v>
+        <v>6.08</v>
       </c>
       <c r="V39">
-        <v>0.158</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="W39">
-        <v>0.17</v>
+        <v>2.282</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
@@ -39557,58 +39581,58 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>2005</v>
+        <v>1998</v>
       </c>
       <c r="G40">
         <v>7</v>
       </c>
       <c r="H40">
-        <v>613</v>
+        <v>243</v>
       </c>
       <c r="I40">
-        <v>1.7999999999999999E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="J40">
-        <v>0.56899999999999995</v>
+        <v>4.7789999999999999</v>
       </c>
       <c r="K40">
-        <v>0.46400000000000002</v>
+        <v>20.335000000000001</v>
       </c>
       <c r="L40">
-        <v>6.5609999999999999</v>
+        <v>20.294</v>
       </c>
       <c r="M40">
-        <v>5.3810000000000002</v>
+        <v>26.596</v>
       </c>
       <c r="N40">
-        <v>68.722999999999999</v>
+        <v>2.8679999999999999</v>
       </c>
       <c r="O40">
-        <v>7.9539999999999997</v>
+        <v>5.4059999999999997</v>
       </c>
       <c r="P40">
-        <v>2.359</v>
+        <v>9.3119999999999994</v>
       </c>
       <c r="Q40">
-        <v>2.9079999999999999</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="R40">
-        <v>2.2080000000000002</v>
+        <v>1.5609999999999999</v>
       </c>
       <c r="S40">
-        <v>1.177</v>
+        <v>3.9009999999999998</v>
       </c>
       <c r="T40">
-        <v>1.091</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="U40">
-        <v>0.25</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="V40">
-        <v>0.09</v>
+        <v>2.9420000000000002</v>
       </c>
       <c r="W40">
-        <v>0.248</v>
+        <v>0.628</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
@@ -39628,58 +39652,58 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>2006</v>
+        <v>1999</v>
       </c>
       <c r="G41">
         <v>7</v>
       </c>
       <c r="H41">
-        <v>720</v>
+        <v>509</v>
       </c>
       <c r="I41">
-        <v>0.32600000000000001</v>
+        <v>6.2E-2</v>
       </c>
       <c r="J41">
-        <v>2.8079999999999998</v>
+        <v>10.244</v>
       </c>
       <c r="K41">
-        <v>10.444000000000001</v>
+        <v>20.364000000000001</v>
       </c>
       <c r="L41">
-        <v>1.673</v>
+        <v>17.981999999999999</v>
       </c>
       <c r="M41">
-        <v>8.5670000000000002</v>
+        <v>20.062000000000001</v>
       </c>
       <c r="N41">
-        <v>4.8789999999999996</v>
+        <v>13.198</v>
       </c>
       <c r="O41">
-        <v>59.036999999999999</v>
+        <v>2.6880000000000002</v>
       </c>
       <c r="P41">
-        <v>5.2759999999999998</v>
+        <v>3.93</v>
       </c>
       <c r="Q41">
-        <v>1.716</v>
+        <v>4.008</v>
       </c>
       <c r="R41">
-        <v>2.3759999999999999</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="S41">
-        <v>1.1339999999999999</v>
+        <v>1.542</v>
       </c>
       <c r="T41">
-        <v>1.0149999999999999</v>
+        <v>2.14</v>
       </c>
       <c r="U41">
-        <v>0.42599999999999999</v>
+        <v>0.39200000000000002</v>
       </c>
       <c r="V41">
-        <v>0.13600000000000001</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="W41">
-        <v>0.188</v>
+        <v>2.0659999999999998</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
@@ -39699,58 +39723,58 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>2007</v>
+        <v>2000</v>
       </c>
       <c r="G42">
         <v>7</v>
       </c>
       <c r="H42">
-        <v>629</v>
+        <v>530</v>
       </c>
       <c r="I42">
-        <v>0.77500000000000002</v>
+        <v>0.996</v>
       </c>
       <c r="J42">
-        <v>11.522</v>
+        <v>4.218</v>
       </c>
       <c r="K42">
-        <v>3.8069999999999999</v>
+        <v>10.935</v>
       </c>
       <c r="L42">
-        <v>15.696999999999999</v>
+        <v>14.285</v>
       </c>
       <c r="M42">
-        <v>1.589</v>
+        <v>12.88</v>
       </c>
       <c r="N42">
-        <v>6.8869999999999996</v>
+        <v>21.062999999999999</v>
       </c>
       <c r="O42">
-        <v>3.8109999999999999</v>
+        <v>13.115</v>
       </c>
       <c r="P42">
-        <v>43.947000000000003</v>
+        <v>6.548</v>
       </c>
       <c r="Q42">
-        <v>5.08</v>
+        <v>4.6479999999999997</v>
       </c>
       <c r="R42">
-        <v>1.7130000000000001</v>
+        <v>2.5089999999999999</v>
       </c>
       <c r="S42">
-        <v>2.2029999999999998</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="T42">
-        <v>1.661</v>
+        <v>2.306</v>
       </c>
       <c r="U42">
-        <v>0.48199999999999998</v>
+        <v>1.292</v>
       </c>
       <c r="V42">
-        <v>0.187</v>
+        <v>0.72</v>
       </c>
       <c r="W42">
-        <v>0.63900000000000001</v>
+        <v>2.4140000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
@@ -39770,58 +39794,58 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>2008</v>
+        <v>2001</v>
       </c>
       <c r="G43">
         <v>7</v>
       </c>
       <c r="H43">
-        <v>794</v>
+        <v>540</v>
       </c>
       <c r="I43">
-        <v>0.75679821000000003</v>
+        <v>0</v>
       </c>
       <c r="J43">
-        <v>9.7950929999999996</v>
+        <v>17.338000000000001</v>
       </c>
       <c r="K43">
-        <v>30.526859999999999</v>
+        <v>16.247</v>
       </c>
       <c r="L43">
-        <v>2.40239</v>
+        <v>14.25</v>
       </c>
       <c r="M43">
-        <v>14.41985</v>
+        <v>15.685</v>
       </c>
       <c r="N43">
-        <v>1.02719</v>
+        <v>8.5589999999999993</v>
       </c>
       <c r="O43">
-        <v>3.6315300000000001</v>
+        <v>12.101000000000001</v>
       </c>
       <c r="P43">
-        <v>3.1684999999999999</v>
+        <v>5.9889999999999999</v>
       </c>
       <c r="Q43">
-        <v>28.092041999999999</v>
+        <v>1.778</v>
       </c>
       <c r="R43">
-        <v>3.0540949999999998</v>
+        <v>2.2320000000000002</v>
       </c>
       <c r="S43">
-        <v>1.148803</v>
+        <v>1.81</v>
       </c>
       <c r="T43">
-        <v>0.73478200000000005</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="U43">
-        <v>0.49574800000000002</v>
+        <v>1.421</v>
       </c>
       <c r="V43">
-        <v>0.3143184</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="W43">
-        <v>0.432008</v>
+        <v>1.2090000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
@@ -39841,58 +39865,58 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <v>2009</v>
+        <v>2002</v>
       </c>
       <c r="G44">
         <v>7</v>
       </c>
       <c r="H44">
-        <v>685</v>
+        <v>449</v>
       </c>
       <c r="I44">
-        <v>0.64311483999999997</v>
+        <v>0</v>
       </c>
       <c r="J44">
-        <v>0.52659699999999998</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="K44">
-        <v>29.653030000000001</v>
+        <v>50.642000000000003</v>
       </c>
       <c r="L44">
-        <v>27.187539999999998</v>
+        <v>14.933999999999999</v>
       </c>
       <c r="M44">
-        <v>3.4567199999999998</v>
+        <v>9.6869999999999994</v>
       </c>
       <c r="N44">
-        <v>11.00914</v>
+        <v>5.7190000000000003</v>
       </c>
       <c r="O44">
-        <v>1.34707</v>
+        <v>4.4379999999999997</v>
       </c>
       <c r="P44">
-        <v>2.3982679999999998</v>
+        <v>6.58</v>
       </c>
       <c r="Q44">
-        <v>2.3471519999999999</v>
+        <v>3.5459999999999998</v>
       </c>
       <c r="R44">
-        <v>16.688388</v>
+        <v>0.871</v>
       </c>
       <c r="S44">
-        <v>2.5758040000000002</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="T44">
-        <v>0.92379599999999995</v>
+        <v>1.036</v>
       </c>
       <c r="U44">
-        <v>0.62511939999999999</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="V44">
-        <v>0.29063519999999998</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="W44">
-        <v>0.32762350000000001</v>
+        <v>0.95299999999999996</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
@@ -39912,58 +39936,58 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>2010</v>
+        <v>2003</v>
       </c>
       <c r="G45">
         <v>7</v>
       </c>
       <c r="H45">
-        <v>874</v>
+        <v>456</v>
       </c>
       <c r="I45">
-        <v>2.8652650000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="J45">
-        <v>25.609874000000001</v>
+        <v>0.105</v>
       </c>
       <c r="K45">
-        <v>3.37629</v>
+        <v>1.3939999999999999</v>
       </c>
       <c r="L45">
-        <v>35.094929999999998</v>
+        <v>67.790999999999997</v>
       </c>
       <c r="M45">
-        <v>21.349329999999998</v>
+        <v>11.664</v>
       </c>
       <c r="N45">
-        <v>2.30165</v>
+        <v>3.3519999999999999</v>
       </c>
       <c r="O45">
-        <v>2.9434</v>
+        <v>5.0090000000000003</v>
       </c>
       <c r="P45">
-        <v>0.43138399999999999</v>
+        <v>3.2029999999999998</v>
       </c>
       <c r="Q45">
-        <v>0.57658200000000004</v>
+        <v>3.153</v>
       </c>
       <c r="R45">
-        <v>0.96884599999999998</v>
+        <v>2.1190000000000002</v>
       </c>
       <c r="S45">
-        <v>5.8603730000000001</v>
+        <v>0.879</v>
       </c>
       <c r="T45">
-        <v>0.90585000000000004</v>
+        <v>0.438</v>
       </c>
       <c r="U45">
-        <v>0.28973520000000003</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="V45">
-        <v>0.10446900000000001</v>
+        <v>0.126</v>
       </c>
       <c r="W45">
-        <v>0.15863340000000001</v>
+        <v>0.23200000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
@@ -39983,58 +40007,58 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>2011</v>
+        <v>2004</v>
       </c>
       <c r="G46">
         <v>7</v>
       </c>
       <c r="H46">
-        <v>1079</v>
+        <v>501</v>
       </c>
       <c r="I46">
-        <v>2.7723253300000001</v>
+        <v>0</v>
       </c>
       <c r="J46">
-        <v>8.934132</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K46">
-        <v>70.269260000000003</v>
+        <v>5.343</v>
       </c>
       <c r="L46">
-        <v>2.72756</v>
+        <v>6.1260000000000003</v>
       </c>
       <c r="M46">
-        <v>6.1955900000000002</v>
+        <v>68.293000000000006</v>
       </c>
       <c r="N46">
-        <v>4.5269700000000004</v>
+        <v>8.1150000000000002</v>
       </c>
       <c r="O46">
-        <v>1.1589700000000001</v>
+        <v>2.1779999999999999</v>
       </c>
       <c r="P46">
-        <v>0.81845699999999999</v>
+        <v>4.133</v>
       </c>
       <c r="Q46">
-        <v>0.30617499999999997</v>
+        <v>2.5059999999999998</v>
       </c>
       <c r="R46">
-        <v>0.38430700000000001</v>
+        <v>1.27</v>
       </c>
       <c r="S46">
-        <v>0.1211</v>
+        <v>1.073</v>
       </c>
       <c r="T46">
-        <v>1.384398</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="U46">
-        <v>0.1769355</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="V46">
-        <v>0.10943310000000001</v>
+        <v>0.158</v>
       </c>
       <c r="W46">
-        <v>0.1143941</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
@@ -40054,58 +40078,58 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>2012</v>
+        <v>2005</v>
       </c>
       <c r="G47">
         <v>7</v>
       </c>
       <c r="H47">
-        <v>851</v>
+        <v>613</v>
       </c>
       <c r="I47">
-        <v>0.18087181999999999</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="J47">
-        <v>40.891272999999998</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="K47">
-        <v>11.555820000000001</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="L47">
-        <v>33.011890000000001</v>
+        <v>6.5609999999999999</v>
       </c>
       <c r="M47">
-        <v>2.4923000000000002</v>
+        <v>5.3810000000000002</v>
       </c>
       <c r="N47">
-        <v>5.0941900000000002</v>
+        <v>68.722999999999999</v>
       </c>
       <c r="O47">
-        <v>2.5222600000000002</v>
+        <v>7.9539999999999997</v>
       </c>
       <c r="P47">
-        <v>1.134747</v>
+        <v>2.359</v>
       </c>
       <c r="Q47">
-        <v>0.66180000000000005</v>
+        <v>2.9079999999999999</v>
       </c>
       <c r="R47">
-        <v>0.232792</v>
+        <v>2.2080000000000002</v>
       </c>
       <c r="S47">
-        <v>0.32998499999999997</v>
+        <v>1.177</v>
       </c>
       <c r="T47">
-        <v>0.34776400000000002</v>
+        <v>1.091</v>
       </c>
       <c r="U47">
-        <v>0.87483820000000001</v>
+        <v>0.25</v>
       </c>
       <c r="V47">
-        <v>0.28430569999999999</v>
+        <v>0.09</v>
       </c>
       <c r="W47">
-        <v>0.38516430000000001</v>
+        <v>0.248</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
@@ -40125,58 +40149,58 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="G48">
         <v>7</v>
       </c>
       <c r="H48">
-        <v>1094</v>
+        <v>720</v>
       </c>
       <c r="I48">
-        <v>3.0260220000000001E-2</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="J48">
-        <v>0.544574</v>
+        <v>2.8079999999999998</v>
       </c>
       <c r="K48">
-        <v>70.313540000000003</v>
+        <v>10.444000000000001</v>
       </c>
       <c r="L48">
-        <v>5.9026399999999999</v>
+        <v>1.673</v>
       </c>
       <c r="M48">
-        <v>10.46529</v>
+        <v>8.5670000000000002</v>
       </c>
       <c r="N48">
-        <v>1.12317</v>
+        <v>4.8789999999999996</v>
       </c>
       <c r="O48">
-        <v>3.4123800000000002</v>
+        <v>59.036999999999999</v>
       </c>
       <c r="P48">
-        <v>2.0593080000000001</v>
+        <v>5.2759999999999998</v>
       </c>
       <c r="Q48">
-        <v>0.90681</v>
+        <v>1.716</v>
       </c>
       <c r="R48">
-        <v>1.3667830000000001</v>
+        <v>2.3759999999999999</v>
       </c>
       <c r="S48">
-        <v>0.26430399999999998</v>
+        <v>1.1339999999999999</v>
       </c>
       <c r="T48">
-        <v>0.33317099999999999</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="U48">
-        <v>0.52975309999999998</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="V48">
-        <v>2.2846907000000001</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="W48">
-        <v>0.46332459999999998</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
@@ -40196,58 +40220,58 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="G49">
         <v>7</v>
       </c>
       <c r="H49">
-        <v>1153</v>
+        <v>629</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="J49">
-        <v>3.2970039999999998</v>
+        <v>11.522</v>
       </c>
       <c r="K49">
-        <v>3.6792500000000001</v>
+        <v>3.8069999999999999</v>
       </c>
       <c r="L49">
-        <v>64.405079999999998</v>
+        <v>15.696999999999999</v>
       </c>
       <c r="M49">
-        <v>6.9786599999999996</v>
+        <v>1.589</v>
       </c>
       <c r="N49">
-        <v>12.085760000000001</v>
+        <v>6.8869999999999996</v>
       </c>
       <c r="O49">
-        <v>1.5920300000000001</v>
+        <v>3.8109999999999999</v>
       </c>
       <c r="P49">
-        <v>3.1229979999999999</v>
+        <v>43.947000000000003</v>
       </c>
       <c r="Q49">
-        <v>1.8362339999999999</v>
+        <v>5.08</v>
       </c>
       <c r="R49">
-        <v>0.81752599999999997</v>
+        <v>1.7130000000000001</v>
       </c>
       <c r="S49">
-        <v>0.46601100000000001</v>
+        <v>2.2029999999999998</v>
       </c>
       <c r="T49">
-        <v>0.117885</v>
+        <v>1.661</v>
       </c>
       <c r="U49">
-        <v>0.19159119999999999</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="V49">
-        <v>0.27802100000000002</v>
+        <v>0.187</v>
       </c>
       <c r="W49">
-        <v>1.1319493</v>
+        <v>0.63900000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
@@ -40267,58 +40291,58 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <v>2015</v>
+        <v>2008</v>
       </c>
       <c r="G50">
         <v>7</v>
       </c>
       <c r="H50">
-        <v>798</v>
+        <v>763</v>
       </c>
       <c r="I50">
-        <v>3.5910063499999998</v>
+        <v>0.76905100000000004</v>
       </c>
       <c r="J50">
-        <v>1.135642</v>
+        <v>8.8523700000000005</v>
       </c>
       <c r="K50">
-        <v>6.8823999999999996</v>
+        <v>30.567299999999999</v>
       </c>
       <c r="L50">
-        <v>3.9457900000000001</v>
+        <v>2.2403300000000002</v>
       </c>
       <c r="M50">
-        <v>70.009029999999996</v>
+        <v>14.2111</v>
       </c>
       <c r="N50">
-        <v>4.9389700000000003</v>
+        <v>1.09013</v>
       </c>
       <c r="O50">
-        <v>5.0940500000000002</v>
+        <v>3.7504200000000001</v>
       </c>
       <c r="P50">
-        <v>0.961148</v>
+        <v>3.4664600000000001</v>
       </c>
       <c r="Q50">
-        <v>1.5535019999999999</v>
+        <v>28.854199999999999</v>
       </c>
       <c r="R50">
-        <v>1.0902019999999999</v>
+        <v>2.6880799999999998</v>
       </c>
       <c r="S50">
-        <v>0.20227899999999999</v>
+        <v>1.4707600000000001</v>
       </c>
       <c r="T50">
-        <v>0.206483</v>
+        <v>0.67583099999999996</v>
       </c>
       <c r="U50">
-        <v>6.0756999999999999E-2</v>
+        <v>0.49945800000000001</v>
       </c>
       <c r="V50">
-        <v>5.41822E-2</v>
+        <v>0.21666299999999999</v>
       </c>
       <c r="W50">
-        <v>0.27455560000000001</v>
+        <v>0.64788999999999997</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
@@ -40338,58 +40362,58 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>2016</v>
+        <v>2009</v>
       </c>
       <c r="G51">
         <v>7</v>
       </c>
       <c r="H51">
-        <v>1440</v>
+        <v>664</v>
       </c>
       <c r="I51">
-        <v>0.29168954000000002</v>
+        <v>0.78587700000000005</v>
       </c>
       <c r="J51">
-        <v>50.181780000000003</v>
+        <v>0.62445600000000001</v>
       </c>
       <c r="K51">
-        <v>1.69143</v>
+        <v>37.451700000000002</v>
       </c>
       <c r="L51">
-        <v>4.4739000000000004</v>
+        <v>30.09</v>
       </c>
       <c r="M51">
-        <v>2.4769100000000002</v>
+        <v>2.75976</v>
       </c>
       <c r="N51">
-        <v>32.875149999999998</v>
+        <v>9.0741700000000005</v>
       </c>
       <c r="O51">
-        <v>2.7772299999999999</v>
+        <v>0.70457000000000003</v>
       </c>
       <c r="P51">
-        <v>3.2349899999999998</v>
+        <v>1.99681</v>
       </c>
       <c r="Q51">
-        <v>0.76114400000000004</v>
+        <v>1.3022499999999999</v>
       </c>
       <c r="R51">
-        <v>0.443687</v>
+        <v>12.4129</v>
       </c>
       <c r="S51">
-        <v>0.36904599999999999</v>
+        <v>1.4837400000000001</v>
       </c>
       <c r="T51">
-        <v>0.23539099999999999</v>
+        <v>0.356711</v>
       </c>
       <c r="U51">
-        <v>6.35183E-2</v>
+        <v>0.59601899999999997</v>
       </c>
       <c r="V51">
-        <v>5.4651900000000003E-2</v>
+        <v>0.16830700000000001</v>
       </c>
       <c r="W51">
-        <v>6.9480299999999995E-2</v>
+        <v>0.19273699999999999</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
@@ -40409,58 +40433,58 @@
         <v>0</v>
       </c>
       <c r="F52">
-        <v>2017</v>
+        <v>2010</v>
       </c>
       <c r="G52">
         <v>7</v>
       </c>
       <c r="H52">
-        <v>1300</v>
+        <v>860</v>
       </c>
       <c r="I52">
-        <v>3.7585688799999999</v>
+        <v>2.6928899999999999E-2</v>
       </c>
       <c r="J52">
-        <v>0.72456100000000001</v>
+        <v>25.0106</v>
       </c>
       <c r="K52">
-        <v>38.373939999999997</v>
+        <v>3.31684</v>
       </c>
       <c r="L52">
-        <v>2.3737699999999999</v>
+        <v>35.1357</v>
       </c>
       <c r="M52">
-        <v>4.1235499999999998</v>
+        <v>23.8354</v>
       </c>
       <c r="N52">
-        <v>3.1163400000000001</v>
+        <v>2.3516599999999999</v>
       </c>
       <c r="O52">
-        <v>36.846989999999998</v>
+        <v>2.57355</v>
       </c>
       <c r="P52">
-        <v>4.4140920000000001</v>
+        <v>0.34839500000000001</v>
       </c>
       <c r="Q52">
-        <v>3.1005250000000002</v>
+        <v>0.460561</v>
       </c>
       <c r="R52">
-        <v>1.3295980000000001</v>
+        <v>0.95934299999999995</v>
       </c>
       <c r="S52">
-        <v>0.61585199999999996</v>
+        <v>4.3331900000000001</v>
       </c>
       <c r="T52">
-        <v>0.71799000000000002</v>
+        <v>1.0765400000000001</v>
       </c>
       <c r="U52">
-        <v>0.20772889999999999</v>
+        <v>0.27774700000000002</v>
       </c>
       <c r="V52">
-        <v>9.2680999999999999E-2</v>
+        <v>0.148066</v>
       </c>
       <c r="W52">
-        <v>0.20380499999999999</v>
+        <v>0.14541599999999999</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
@@ -40480,58 +40504,58 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>2018</v>
+        <v>2011</v>
       </c>
       <c r="G53">
         <v>7</v>
       </c>
       <c r="H53">
-        <v>1174</v>
+        <v>1075</v>
       </c>
       <c r="I53">
-        <v>7.3480661400000002</v>
+        <v>2.6735600000000002</v>
       </c>
       <c r="J53">
-        <v>25.520558000000001</v>
+        <v>8.6921900000000001</v>
       </c>
       <c r="K53">
-        <v>1.49211</v>
+        <v>71.576099999999997</v>
       </c>
       <c r="L53">
-        <v>26.967140000000001</v>
+        <v>2.60005</v>
       </c>
       <c r="M53">
-        <v>1.51678</v>
+        <v>6.05471</v>
       </c>
       <c r="N53">
-        <v>2.8050000000000002</v>
+        <v>4.2575399999999997</v>
       </c>
       <c r="O53">
-        <v>3.0360100000000001</v>
+        <v>0.99419900000000005</v>
       </c>
       <c r="P53">
-        <v>22.783263000000002</v>
+        <v>0.81207700000000005</v>
       </c>
       <c r="Q53">
-        <v>4.3114220000000003</v>
+        <v>0.28128599999999998</v>
       </c>
       <c r="R53">
-        <v>1.9116109999999999</v>
+        <v>0.33081899999999997</v>
       </c>
       <c r="S53">
-        <v>0.94222799999999995</v>
+        <v>6.9584900000000005E-2</v>
       </c>
       <c r="T53">
-        <v>0.54535999999999996</v>
+        <v>1.3264</v>
       </c>
       <c r="U53">
-        <v>0.41080309999999998</v>
+        <v>0.13855300000000001</v>
       </c>
       <c r="V53">
-        <v>0.31440760000000001</v>
+        <v>7.6237299999999994E-2</v>
       </c>
       <c r="W53">
-        <v>9.5247399999999996E-2</v>
+        <v>0.11669499999999999</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
@@ -40551,58 +40575,839 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="G54">
         <v>7</v>
       </c>
       <c r="H54">
-        <v>1001</v>
+        <v>796</v>
       </c>
       <c r="I54">
-        <v>5.1881100000000001E-3</v>
+        <v>0.17596700000000001</v>
       </c>
       <c r="J54">
-        <v>13.706896</v>
+        <v>40.406300000000002</v>
       </c>
       <c r="K54">
-        <v>20.71518</v>
+        <v>11.578900000000001</v>
       </c>
       <c r="L54">
-        <v>1.5696099999999999</v>
+        <v>33.188499999999998</v>
       </c>
       <c r="M54">
-        <v>32.34901</v>
+        <v>2.4483199999999998</v>
       </c>
       <c r="N54">
-        <v>1.76491</v>
+        <v>5.3725199999999997</v>
       </c>
       <c r="O54">
-        <v>3.8224900000000002</v>
+        <v>2.57707</v>
       </c>
       <c r="P54">
-        <v>2.2397040000000001</v>
+        <v>1.1066800000000001</v>
       </c>
       <c r="Q54">
-        <v>18.663888</v>
+        <v>0.66058600000000001</v>
       </c>
       <c r="R54">
-        <v>1.977719</v>
+        <v>0.232546</v>
       </c>
       <c r="S54">
-        <v>1.656258</v>
+        <v>0.34797499999999998</v>
       </c>
       <c r="T54">
-        <v>0.68714900000000001</v>
+        <v>0.32686199999999999</v>
       </c>
       <c r="U54">
-        <v>0.3833954</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="V54">
-        <v>0.22775139999999999</v>
+        <v>0.26022600000000001</v>
       </c>
       <c r="W54">
-        <v>0.23085420000000001</v>
+        <v>0.39660299999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>381</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>2013</v>
+      </c>
+      <c r="G55">
+        <v>7</v>
+      </c>
+      <c r="H55">
+        <v>1044</v>
+      </c>
+      <c r="I55">
+        <v>3.0162999999999999E-2</v>
+      </c>
+      <c r="J55">
+        <v>0.53978999999999999</v>
+      </c>
+      <c r="K55">
+        <v>69.852000000000004</v>
+      </c>
+      <c r="L55">
+        <v>5.9241000000000001</v>
+      </c>
+      <c r="M55">
+        <v>10.5138</v>
+      </c>
+      <c r="N55">
+        <v>1.1887099999999999</v>
+      </c>
+      <c r="O55">
+        <v>3.5394800000000002</v>
+      </c>
+      <c r="P55">
+        <v>2.0773600000000001</v>
+      </c>
+      <c r="Q55">
+        <v>0.98362099999999997</v>
+      </c>
+      <c r="R55">
+        <v>1.4374800000000001</v>
+      </c>
+      <c r="S55">
+        <v>0.28304400000000002</v>
+      </c>
+      <c r="T55">
+        <v>0.31610300000000002</v>
+      </c>
+      <c r="U55">
+        <v>0.55864599999999998</v>
+      </c>
+      <c r="V55">
+        <v>2.2767599999999999</v>
+      </c>
+      <c r="W55">
+        <v>0.47894799999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>381</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>2014</v>
+      </c>
+      <c r="G56">
+        <v>7</v>
+      </c>
+      <c r="H56">
+        <v>1104</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>3.2926899999999999</v>
+      </c>
+      <c r="K56">
+        <v>3.82402</v>
+      </c>
+      <c r="L56">
+        <v>64.812700000000007</v>
+      </c>
+      <c r="M56">
+        <v>7.0507299999999997</v>
+      </c>
+      <c r="N56">
+        <v>12.2044</v>
+      </c>
+      <c r="O56">
+        <v>1.6866000000000001</v>
+      </c>
+      <c r="P56">
+        <v>2.8971499999999999</v>
+      </c>
+      <c r="Q56">
+        <v>1.8165899999999999</v>
+      </c>
+      <c r="R56">
+        <v>0.67685499999999998</v>
+      </c>
+      <c r="S56">
+        <v>0.39116000000000001</v>
+      </c>
+      <c r="T56">
+        <v>6.6864499999999993E-2</v>
+      </c>
+      <c r="U56">
+        <v>0.193573</v>
+      </c>
+      <c r="V56">
+        <v>0.21700800000000001</v>
+      </c>
+      <c r="W56">
+        <v>0.86961599999999994</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>381</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>2015</v>
+      </c>
+      <c r="G57">
+        <v>7</v>
+      </c>
+      <c r="H57">
+        <v>745</v>
+      </c>
+      <c r="I57">
+        <v>3.61511</v>
+      </c>
+      <c r="J57">
+        <v>1.10307</v>
+      </c>
+      <c r="K57">
+        <v>7.0629799999999996</v>
+      </c>
+      <c r="L57">
+        <v>3.85141</v>
+      </c>
+      <c r="M57">
+        <v>69.583799999999997</v>
+      </c>
+      <c r="N57">
+        <v>4.9533199999999997</v>
+      </c>
+      <c r="O57">
+        <v>5.5609200000000003</v>
+      </c>
+      <c r="P57">
+        <v>0.92841399999999996</v>
+      </c>
+      <c r="Q57">
+        <v>1.4547399999999999</v>
+      </c>
+      <c r="R57">
+        <v>1.20048</v>
+      </c>
+      <c r="S57">
+        <v>0.23869199999999999</v>
+      </c>
+      <c r="T57">
+        <v>0.166625</v>
+      </c>
+      <c r="U57">
+        <v>4.42583E-2</v>
+      </c>
+      <c r="V57">
+        <v>2.78938E-2</v>
+      </c>
+      <c r="W57">
+        <v>0.20832500000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>381</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>2016</v>
+      </c>
+      <c r="G58">
+        <v>7</v>
+      </c>
+      <c r="H58">
+        <v>1308</v>
+      </c>
+      <c r="I58">
+        <v>0.31984000000000001</v>
+      </c>
+      <c r="J58">
+        <v>50.493400000000001</v>
+      </c>
+      <c r="K58">
+        <v>1.6456500000000001</v>
+      </c>
+      <c r="L58">
+        <v>4.6774800000000001</v>
+      </c>
+      <c r="M58">
+        <v>2.74376</v>
+      </c>
+      <c r="N58">
+        <v>32.542099999999998</v>
+      </c>
+      <c r="O58">
+        <v>2.3075700000000001</v>
+      </c>
+      <c r="P58">
+        <v>3.0013800000000002</v>
+      </c>
+      <c r="Q58">
+        <v>0.81447000000000003</v>
+      </c>
+      <c r="R58">
+        <v>0.43951499999999999</v>
+      </c>
+      <c r="S58">
+        <v>0.271901</v>
+      </c>
+      <c r="T58">
+        <v>0.32560899999999998</v>
+      </c>
+      <c r="U58">
+        <v>0.14294699999999999</v>
+      </c>
+      <c r="V58">
+        <v>6.4579200000000003E-2</v>
+      </c>
+      <c r="W58">
+        <v>0.20979999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>381</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>2017</v>
+      </c>
+      <c r="G59">
+        <v>7</v>
+      </c>
+      <c r="H59">
+        <v>1293</v>
+      </c>
+      <c r="I59">
+        <v>3.7664399999999998</v>
+      </c>
+      <c r="J59">
+        <v>0.72325200000000001</v>
+      </c>
+      <c r="K59">
+        <v>38.471200000000003</v>
+      </c>
+      <c r="L59">
+        <v>2.37717</v>
+      </c>
+      <c r="M59">
+        <v>4.1212799999999996</v>
+      </c>
+      <c r="N59">
+        <v>3.1032999999999999</v>
+      </c>
+      <c r="O59">
+        <v>36.814</v>
+      </c>
+      <c r="P59">
+        <v>4.38009</v>
+      </c>
+      <c r="Q59">
+        <v>3.08094</v>
+      </c>
+      <c r="R59">
+        <v>1.32884</v>
+      </c>
+      <c r="S59">
+        <v>0.61193500000000001</v>
+      </c>
+      <c r="T59">
+        <v>0.71745199999999998</v>
+      </c>
+      <c r="U59">
+        <v>0.20866100000000001</v>
+      </c>
+      <c r="V59">
+        <v>9.2763499999999999E-2</v>
+      </c>
+      <c r="W59">
+        <v>0.20271800000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>381</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>2018</v>
+      </c>
+      <c r="G60">
+        <v>7</v>
+      </c>
+      <c r="H60">
+        <v>1209</v>
+      </c>
+      <c r="I60">
+        <v>7.1488500000000004</v>
+      </c>
+      <c r="J60">
+        <v>25.583200000000001</v>
+      </c>
+      <c r="K60">
+        <v>1.3712</v>
+      </c>
+      <c r="L60">
+        <v>27.784099999999999</v>
+      </c>
+      <c r="M60">
+        <v>1.5137700000000001</v>
+      </c>
+      <c r="N60">
+        <v>2.7593000000000001</v>
+      </c>
+      <c r="O60">
+        <v>3.04033</v>
+      </c>
+      <c r="P60">
+        <v>22.522500000000001</v>
+      </c>
+      <c r="Q60">
+        <v>4.0024499999999996</v>
+      </c>
+      <c r="R60">
+        <v>1.85216</v>
+      </c>
+      <c r="S60">
+        <v>0.96630499999999997</v>
+      </c>
+      <c r="T60">
+        <v>0.58314100000000002</v>
+      </c>
+      <c r="U60">
+        <v>0.41465999999999997</v>
+      </c>
+      <c r="V60">
+        <v>0.36117199999999999</v>
+      </c>
+      <c r="W60">
+        <v>9.6937200000000001E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>381</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>2019</v>
+      </c>
+      <c r="G61">
+        <v>7</v>
+      </c>
+      <c r="H61">
+        <v>1138</v>
+      </c>
+      <c r="I61">
+        <v>5.0497500000000004E-3</v>
+      </c>
+      <c r="J61">
+        <v>13.1303</v>
+      </c>
+      <c r="K61">
+        <v>21.212700000000002</v>
+      </c>
+      <c r="L61">
+        <v>1.6132500000000001</v>
+      </c>
+      <c r="M61">
+        <v>32.562100000000001</v>
+      </c>
+      <c r="N61">
+        <v>1.8378099999999999</v>
+      </c>
+      <c r="O61">
+        <v>3.7816000000000001</v>
+      </c>
+      <c r="P61">
+        <v>2.1152500000000001</v>
+      </c>
+      <c r="Q61">
+        <v>18.628799999999998</v>
+      </c>
+      <c r="R61">
+        <v>1.9095599999999999</v>
+      </c>
+      <c r="S61">
+        <v>1.64716</v>
+      </c>
+      <c r="T61">
+        <v>0.68703099999999995</v>
+      </c>
+      <c r="U61">
+        <v>0.39589000000000002</v>
+      </c>
+      <c r="V61">
+        <v>0.24992200000000001</v>
+      </c>
+      <c r="W61">
+        <v>0.22356300000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>381</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>2020</v>
+      </c>
+      <c r="G62">
+        <v>7</v>
+      </c>
+      <c r="H62">
+        <v>756</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>6.1957499999999999E-2</v>
+      </c>
+      <c r="K62">
+        <v>8.8378099999999993</v>
+      </c>
+      <c r="L62">
+        <v>36.463299999999997</v>
+      </c>
+      <c r="M62">
+        <v>1.5484500000000001</v>
+      </c>
+      <c r="N62">
+        <v>30.684000000000001</v>
+      </c>
+      <c r="O62">
+        <v>1.57091</v>
+      </c>
+      <c r="P62">
+        <v>2.14</v>
+      </c>
+      <c r="Q62">
+        <v>1.77935</v>
+      </c>
+      <c r="R62">
+        <v>14.2097</v>
+      </c>
+      <c r="S62">
+        <v>1.0838000000000001</v>
+      </c>
+      <c r="T62">
+        <v>1.0265599999999999</v>
+      </c>
+      <c r="U62">
+        <v>0.27924300000000002</v>
+      </c>
+      <c r="V62">
+        <v>8.6039400000000002E-2</v>
+      </c>
+      <c r="W62">
+        <v>0.22874800000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>381</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>2021</v>
+      </c>
+      <c r="G63">
+        <v>7</v>
+      </c>
+      <c r="H63">
+        <v>721</v>
+      </c>
+      <c r="I63">
+        <v>1.39306</v>
+      </c>
+      <c r="J63">
+        <v>0.36449500000000001</v>
+      </c>
+      <c r="K63">
+        <v>1.96034</v>
+      </c>
+      <c r="L63">
+        <v>13.446899999999999</v>
+      </c>
+      <c r="M63">
+        <v>33.994599999999998</v>
+      </c>
+      <c r="N63">
+        <v>2.87202</v>
+      </c>
+      <c r="O63">
+        <v>24.694500000000001</v>
+      </c>
+      <c r="P63">
+        <v>1.9777199999999999</v>
+      </c>
+      <c r="Q63">
+        <v>2.4432800000000001</v>
+      </c>
+      <c r="R63">
+        <v>3.0555699999999999</v>
+      </c>
+      <c r="S63">
+        <v>10.542999999999999</v>
+      </c>
+      <c r="T63">
+        <v>1.8132900000000001</v>
+      </c>
+      <c r="U63">
+        <v>0.56567800000000001</v>
+      </c>
+      <c r="V63">
+        <v>0.57433400000000001</v>
+      </c>
+      <c r="W63">
+        <v>0.301313</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>381</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>2022</v>
+      </c>
+      <c r="G64">
+        <v>7</v>
+      </c>
+      <c r="H64">
+        <v>899</v>
+      </c>
+      <c r="I64">
+        <v>0.79811900000000002</v>
+      </c>
+      <c r="J64">
+        <v>32.369100000000003</v>
+      </c>
+      <c r="K64">
+        <v>1.4585699999999999</v>
+      </c>
+      <c r="L64">
+        <v>1.9623900000000001</v>
+      </c>
+      <c r="M64">
+        <v>9.0089400000000008</v>
+      </c>
+      <c r="N64">
+        <v>23.934000000000001</v>
+      </c>
+      <c r="O64">
+        <v>1.63381</v>
+      </c>
+      <c r="P64">
+        <v>15.4781</v>
+      </c>
+      <c r="Q64">
+        <v>2.2827999999999999</v>
+      </c>
+      <c r="R64">
+        <v>1.17862</v>
+      </c>
+      <c r="S64">
+        <v>1.1199600000000001</v>
+      </c>
+      <c r="T64">
+        <v>5.8855899999999997</v>
+      </c>
+      <c r="U64">
+        <v>1.8578399999999999</v>
+      </c>
+      <c r="V64">
+        <v>0.66521300000000005</v>
+      </c>
+      <c r="W64">
+        <v>0.36692200000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>381</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>2023</v>
+      </c>
+      <c r="G65">
+        <v>7</v>
+      </c>
+      <c r="H65">
+        <v>610</v>
+      </c>
+      <c r="I65">
+        <v>0.69062400000000002</v>
+      </c>
+      <c r="J65">
+        <v>35.254600000000003</v>
+      </c>
+      <c r="K65">
+        <v>24.896999999999998</v>
+      </c>
+      <c r="L65">
+        <v>1.27983</v>
+      </c>
+      <c r="M65">
+        <v>1.9525999999999999</v>
+      </c>
+      <c r="N65">
+        <v>5.8779000000000003</v>
+      </c>
+      <c r="O65">
+        <v>12.927899999999999</v>
+      </c>
+      <c r="P65">
+        <v>1.6308</v>
+      </c>
+      <c r="Q65">
+        <v>7.9703999999999997</v>
+      </c>
+      <c r="R65">
+        <v>1.3553200000000001</v>
+      </c>
+      <c r="S65">
+        <v>0.67327199999999998</v>
+      </c>
+      <c r="T65">
+        <v>1.0873600000000001</v>
+      </c>
+      <c r="U65">
+        <v>3.39561</v>
+      </c>
+      <c r="V65">
+        <v>0.57847999999999999</v>
+      </c>
+      <c r="W65">
+        <v>0.42821300000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set up testing script to run new model & compare to assessment output
</commit_message>
<xml_diff>
--- a/data/hake_input_yr24.xlsx
+++ b/data/hake_input_yr24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD90087A-2089-B24B-A1DE-89C296712346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F986DC0-9BFE-494F-87B4-0661AE12A48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="8840" windowWidth="43300" windowHeight="33040" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5500" yWindow="8840" windowWidth="43300" windowHeight="33040" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1607,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23740,10 +23740,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24073,6 +24073,38 @@
         <v>2019</v>
       </c>
       <c r="B41" s="3">
+        <v>7.3799565200000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2020</v>
+      </c>
+      <c r="B42" s="3">
+        <v>7.3799565200000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2021</v>
+      </c>
+      <c r="B43" s="3">
+        <v>7.3799565200000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2022</v>
+      </c>
+      <c r="B44" s="3">
+        <v>7.3799565200000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2023</v>
+      </c>
+      <c r="B45" s="3">
         <v>7.3799565200000004</v>
       </c>
     </row>
@@ -31423,7 +31455,7 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39849,7 +39881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added another data file with an attempt at the age-1 index
</commit_message>
<xml_diff>
--- a/data/hake_input_yr24.xlsx
+++ b/data/hake_input_yr24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F986DC0-9BFE-494F-87B4-0661AE12A48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2996D723-6B8D-3C49-A0C4-184015DC8D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="8840" windowWidth="43300" windowHeight="33040" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5500" yWindow="8840" windowWidth="34420" windowHeight="33040" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1607,7 +1607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -2556,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2668,7 +2668,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.32924199999999998</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2739,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.34691699999999998</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.36863200000000002</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -2881,7 +2881,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.395312</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0.42809000000000003</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3023,7 +3023,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0.468362</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -3094,7 +3094,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0.517841</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -3165,7 +3165,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0.57862999999999998</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3236,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0.65331600000000001</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -3307,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0.74507599999999996</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -3378,7 +3378,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>0.85781300000000005</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -3449,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>0.99632200000000004</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -3520,7 +3520,7 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>1</v>
+        <v>1.1665000000000001</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -3591,7 +3591,7 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>1.37557</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -3662,7 +3662,7 @@
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>1.6324399999999999</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -3733,7 +3733,7 @@
         <v>0</v>
       </c>
       <c r="R17">
-        <v>1</v>
+        <v>1.8580000000000001</v>
       </c>
       <c r="S17">
         <v>0</v>
@@ -3804,7 +3804,7 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>1</v>
+        <v>2.1720000000000002</v>
       </c>
       <c r="T18">
         <v>0</v>
@@ -3875,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>1</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -3946,7 +3946,7 @@
         <v>0</v>
       </c>
       <c r="U20">
-        <v>1</v>
+        <v>2.9340000000000002</v>
       </c>
       <c r="V20">
         <v>0</v>
@@ -4017,7 +4017,7 @@
         <v>0</v>
       </c>
       <c r="V21">
-        <v>1</v>
+        <v>3.3879999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -4029,8 +4029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Y246"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F198" sqref="F198:Y246"/>
+    <sheetView topLeftCell="A230" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A247" sqref="A247:XFD295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15451,64 +15451,64 @@
         <v>1975</v>
       </c>
       <c r="F149">
-        <v>6.3106846507991398E-3</v>
+        <v>1.5858565105263201E-3</v>
       </c>
       <c r="G149">
-        <v>0.105643567764722</v>
+        <v>3.9686836105263197E-2</v>
       </c>
       <c r="H149">
-        <v>0.330366822375114</v>
+        <v>0.21494590842105299</v>
       </c>
       <c r="I149">
-        <v>0.54172873700875301</v>
+        <v>0.47807245605263199</v>
       </c>
       <c r="J149">
-        <v>0.67393065746534497</v>
+        <v>0.65179900673684199</v>
       </c>
       <c r="K149">
-        <v>0.75707817837345504</v>
+        <v>0.74843338357894695</v>
       </c>
       <c r="L149">
-        <v>0.87412604184361897</v>
+        <v>0.87145749031579001</v>
       </c>
       <c r="M149">
-        <v>0.99298663083236705</v>
+        <v>0.94536761094736799</v>
       </c>
       <c r="N149">
-        <v>1.06355801060855</v>
+        <v>1.0632652920000001</v>
       </c>
       <c r="O149">
-        <v>1.1633970484548599</v>
+        <v>1.16296758947368</v>
       </c>
       <c r="P149">
-        <v>1.35859401827304</v>
+        <v>1.3580419646842099</v>
       </c>
       <c r="Q149">
-        <v>1.5614727323661</v>
+        <v>1.5608252804210501</v>
       </c>
       <c r="R149">
-        <v>1.5753873024981699</v>
+        <v>1.57061156178947</v>
       </c>
       <c r="S149">
-        <v>1.8604085191897599</v>
+        <v>1.8421277490000001</v>
       </c>
       <c r="T149">
-        <v>1.08193903054143</v>
+        <v>1.0520702532631601</v>
       </c>
       <c r="U149">
-        <v>1.08193903054143</v>
+        <v>1.0520702532631601</v>
       </c>
       <c r="V149">
-        <v>1.08193903054143</v>
+        <v>1.0520702532631601</v>
       </c>
       <c r="W149">
-        <v>1.08193903054143</v>
+        <v>1.0520702532631601</v>
       </c>
       <c r="X149">
-        <v>1.08193903054143</v>
+        <v>1.0520702532631601</v>
       </c>
       <c r="Y149">
-        <v>1.08193903054143</v>
+        <v>1.0520702532631601</v>
       </c>
     </row>
     <row r="150" spans="1:25" x14ac:dyDescent="0.2">
@@ -15528,64 +15528,64 @@
         <v>1976</v>
       </c>
       <c r="F150">
-        <v>7.6066183109621899E-3</v>
+        <v>1.9115208315789499E-3</v>
       </c>
       <c r="G150">
-        <v>0.10407909535865401</v>
+        <v>3.9099114947368403E-2</v>
       </c>
       <c r="H150">
-        <v>0.39846155127696198</v>
+        <v>0.25925024642105299</v>
       </c>
       <c r="I150">
-        <v>0.55149361640716299</v>
+        <v>0.48668990526315797</v>
       </c>
       <c r="J150">
-        <v>0.72907847294656403</v>
+        <v>0.705135786947368</v>
       </c>
       <c r="K150">
-        <v>0.82665345964074399</v>
+        <v>0.81721421052631604</v>
       </c>
       <c r="L150">
-        <v>0.91517731566929394</v>
+        <v>0.91238344189473697</v>
       </c>
       <c r="M150">
-        <v>1.0918299567583001</v>
+        <v>1.0394708707368401</v>
       </c>
       <c r="N150">
-        <v>1.2145011903297001</v>
+        <v>1.21416692826316</v>
       </c>
       <c r="O150">
-        <v>1.25684905253607</v>
+        <v>1.25638509647368</v>
       </c>
       <c r="P150">
-        <v>1.40377839447019</v>
+        <v>1.4032079805789499</v>
       </c>
       <c r="Q150">
-        <v>1.64500189942301</v>
+        <v>1.64431981278947</v>
       </c>
       <c r="R150">
-        <v>1.80741587562061</v>
+        <v>1.80193674705263</v>
       </c>
       <c r="S150">
-        <v>1.8361115843350699</v>
+        <v>1.8180695609999999</v>
       </c>
       <c r="T150">
-        <v>2.3022448641598401</v>
+        <v>2.2386874573684201</v>
       </c>
       <c r="U150">
-        <v>2.3022448641598401</v>
+        <v>2.2386874573684201</v>
       </c>
       <c r="V150">
-        <v>2.3022448641598401</v>
+        <v>2.2386874573684201</v>
       </c>
       <c r="W150">
-        <v>2.3022448641598401</v>
+        <v>2.2386874573684201</v>
       </c>
       <c r="X150">
-        <v>2.3022448641598401</v>
+        <v>2.2386874573684201</v>
       </c>
       <c r="Y150">
-        <v>2.3022448641598401</v>
+        <v>2.2386874573684201</v>
       </c>
     </row>
     <row r="151" spans="1:25" x14ac:dyDescent="0.2">
@@ -15605,64 +15605,64 @@
         <v>1977</v>
       </c>
       <c r="F151">
-        <v>5.7512919289892696E-3</v>
+        <v>1.4452827631578999E-3</v>
       </c>
       <c r="G151">
-        <v>0.108814761884461</v>
+        <v>4.0878150105263203E-2</v>
       </c>
       <c r="H151">
-        <v>0.34049917255735102</v>
+        <v>0.22153829926315799</v>
       </c>
       <c r="I151">
-        <v>0.57695185833401297</v>
+        <v>0.50915665552631595</v>
       </c>
       <c r="J151">
-        <v>0.64378667547667801</v>
+        <v>0.62264494273684201</v>
       </c>
       <c r="K151">
-        <v>0.775696275516226</v>
+        <v>0.76683888757894703</v>
       </c>
       <c r="L151">
-        <v>0.86675650965516704</v>
+        <v>0.86411045600000003</v>
       </c>
       <c r="M151">
-        <v>0.99150595547713805</v>
+        <v>0.94395794189473703</v>
       </c>
       <c r="N151">
-        <v>1.15829361092189</v>
+        <v>1.1579748186315799</v>
       </c>
       <c r="O151">
-        <v>1.2448844340480101</v>
+        <v>1.2444248946315799</v>
       </c>
       <c r="P151">
-        <v>1.3154152013342999</v>
+        <v>1.3148806931052599</v>
       </c>
       <c r="Q151">
-        <v>1.4742949729764201</v>
+        <v>1.4736836685789501</v>
       </c>
       <c r="R151">
-        <v>1.65157853959254</v>
+        <v>1.64657182736842</v>
       </c>
       <c r="S151">
-        <v>1.8271699539714501</v>
+        <v>1.8092157929999999</v>
       </c>
       <c r="T151">
-        <v>1.9708401565946001</v>
+        <v>1.9164317435263201</v>
       </c>
       <c r="U151">
-        <v>1.9708401565946001</v>
+        <v>1.9164317435263201</v>
       </c>
       <c r="V151">
-        <v>1.9708401565946001</v>
+        <v>1.9164317435263201</v>
       </c>
       <c r="W151">
-        <v>1.9708401565946001</v>
+        <v>1.9164317435263201</v>
       </c>
       <c r="X151">
-        <v>1.9708401565946001</v>
+        <v>1.9164317435263201</v>
       </c>
       <c r="Y151">
-        <v>1.9708401565946001</v>
+        <v>1.9164317435263201</v>
       </c>
     </row>
     <row r="152" spans="1:25" x14ac:dyDescent="0.2">
@@ -15682,64 +15682,64 @@
         <v>1978</v>
       </c>
       <c r="F152">
-        <v>7.5486079357544103E-3</v>
+        <v>1.89694299473684E-3</v>
       </c>
       <c r="G152">
-        <v>7.5831854331045598E-2</v>
+        <v>2.8487549578947401E-2</v>
       </c>
       <c r="H152">
-        <v>0.328118384384535</v>
+        <v>0.21348301168421099</v>
       </c>
       <c r="I152">
-        <v>0.454422041678124</v>
+        <v>0.40102480578947403</v>
       </c>
       <c r="J152">
-        <v>0.62077089049693002</v>
+        <v>0.60038498821052599</v>
       </c>
       <c r="K152">
-        <v>0.631320111993524</v>
+        <v>0.62411130189473696</v>
       </c>
       <c r="L152">
-        <v>0.74964476366656996</v>
+        <v>0.747356231368421</v>
       </c>
       <c r="M152">
-        <v>0.86552051294436005</v>
+        <v>0.82401417515789499</v>
       </c>
       <c r="N152">
-        <v>0.96950313928097198</v>
+        <v>0.96923630699999996</v>
       </c>
       <c r="O152">
-        <v>1.09430901298547</v>
+        <v>1.09390505731579</v>
       </c>
       <c r="P152">
-        <v>1.2008782500212301</v>
+        <v>1.20039028294737</v>
       </c>
       <c r="Q152">
-        <v>1.27332402801167</v>
+        <v>1.2727960545789501</v>
       </c>
       <c r="R152">
-        <v>1.36429227449207</v>
+        <v>1.36015646221053</v>
       </c>
       <c r="S152">
-        <v>1.5388996576673399</v>
+        <v>1.5237781020000001</v>
       </c>
       <c r="T152">
-        <v>1.8076797996396401</v>
+        <v>1.7577757072631599</v>
       </c>
       <c r="U152">
-        <v>1.8076797996396401</v>
+        <v>1.7577757072631599</v>
       </c>
       <c r="V152">
-        <v>1.8076797996396401</v>
+        <v>1.7577757072631599</v>
       </c>
       <c r="W152">
-        <v>1.8076797996396401</v>
+        <v>1.7577757072631599</v>
       </c>
       <c r="X152">
-        <v>1.8076797996396401</v>
+        <v>1.7577757072631599</v>
       </c>
       <c r="Y152">
-        <v>1.8076797996396401</v>
+        <v>1.7577757072631599</v>
       </c>
     </row>
     <row r="153" spans="1:25" x14ac:dyDescent="0.2">
@@ -15759,64 +15759,64 @@
         <v>1979</v>
       </c>
       <c r="F153">
-        <v>5.9000566482352501E-3</v>
+        <v>1.4826669E-3</v>
       </c>
       <c r="G153">
-        <v>0.120362587838898</v>
+        <v>4.5216290947368398E-2</v>
       </c>
       <c r="H153">
-        <v>0.27652399302430197</v>
+        <v>0.179914255473684</v>
       </c>
       <c r="I153">
-        <v>0.52955633583607098</v>
+        <v>0.467330382894737</v>
       </c>
       <c r="J153">
-        <v>0.59127489946608103</v>
+        <v>0.57185763536842105</v>
       </c>
       <c r="K153">
-        <v>0.73616849892369696</v>
+        <v>0.727762464</v>
       </c>
       <c r="L153">
-        <v>0.73782220855859104</v>
+        <v>0.73556976842105304</v>
       </c>
       <c r="M153">
-        <v>0.90526156361370902</v>
+        <v>0.86184942989473701</v>
       </c>
       <c r="N153">
-        <v>1.0234568849018799</v>
+        <v>1.02317520315789</v>
       </c>
       <c r="O153">
-        <v>1.10766581254424</v>
+        <v>1.1072569263157901</v>
       </c>
       <c r="P153">
-        <v>1.2765804629448501</v>
+        <v>1.2760617348947401</v>
       </c>
       <c r="Q153">
-        <v>1.40576692980276</v>
+        <v>1.40518404</v>
       </c>
       <c r="R153">
-        <v>1.4249519813629701</v>
+        <v>1.4206322809473699</v>
       </c>
       <c r="S153">
-        <v>1.53729343962691</v>
+        <v>1.5221876670000001</v>
       </c>
       <c r="T153">
-        <v>1.8411581802763</v>
+        <v>1.79032985994737</v>
       </c>
       <c r="U153">
-        <v>1.8411581802763</v>
+        <v>1.79032985994737</v>
       </c>
       <c r="V153">
-        <v>1.8411581802763</v>
+        <v>1.79032985994737</v>
       </c>
       <c r="W153">
-        <v>1.8411581802763</v>
+        <v>1.79032985994737</v>
       </c>
       <c r="X153">
-        <v>1.8411581802763</v>
+        <v>1.79032985994737</v>
       </c>
       <c r="Y153">
-        <v>1.8411581802763</v>
+        <v>1.79032985994737</v>
       </c>
     </row>
     <row r="154" spans="1:25" x14ac:dyDescent="0.2">
@@ -15836,64 +15836,64 @@
         <v>1980</v>
       </c>
       <c r="F154">
-        <v>5.5658243280992097E-3</v>
+        <v>1.3986752999999999E-3</v>
       </c>
       <c r="G154">
-        <v>7.1648402039463294E-2</v>
+        <v>2.6915963263157899E-2</v>
       </c>
       <c r="H154">
-        <v>0.33427072276959202</v>
+        <v>0.217485895368421</v>
       </c>
       <c r="I154">
-        <v>0.33989148698604499</v>
+        <v>0.299952258157895</v>
       </c>
       <c r="J154">
-        <v>0.52476881149043397</v>
+        <v>0.50753558442105295</v>
       </c>
       <c r="K154">
-        <v>0.53402438886562997</v>
+        <v>0.52792656252631598</v>
       </c>
       <c r="L154">
-        <v>0.65524711029416205</v>
+        <v>0.65324675726315795</v>
       </c>
       <c r="M154">
-        <v>0.67857220573029098</v>
+        <v>0.64603103915789495</v>
       </c>
       <c r="N154">
-        <v>0.81525229051973802</v>
+        <v>0.81502791205263103</v>
       </c>
       <c r="O154">
-        <v>0.890543056471085</v>
+        <v>0.890214319421052</v>
       </c>
       <c r="P154">
-        <v>0.98410807049148197</v>
+        <v>0.98370818621052603</v>
       </c>
       <c r="Q154">
-        <v>1.1381207346467099</v>
+        <v>1.13764882215789</v>
       </c>
       <c r="R154">
-        <v>1.19812024915446</v>
+        <v>1.1944881825263201</v>
       </c>
       <c r="S154">
-        <v>1.22285613674522</v>
+        <v>1.210840092</v>
       </c>
       <c r="T154">
-        <v>1.4007588668984301</v>
+        <v>1.3620885227894699</v>
       </c>
       <c r="U154">
-        <v>1.4007588668984301</v>
+        <v>1.3620885227894699</v>
       </c>
       <c r="V154">
-        <v>1.4007588668984301</v>
+        <v>1.3620885227894699</v>
       </c>
       <c r="W154">
-        <v>1.4007588668984301</v>
+        <v>1.3620885227894699</v>
       </c>
       <c r="X154">
-        <v>1.4007588668984301</v>
+        <v>1.3620885227894699</v>
       </c>
       <c r="Y154">
-        <v>1.4007588668984301</v>
+        <v>1.3620885227894699</v>
       </c>
     </row>
     <row r="155" spans="1:25" x14ac:dyDescent="0.2">
@@ -15913,64 +15913,64 @@
         <v>1981</v>
       </c>
       <c r="F155">
-        <v>6.1941234203171901E-3</v>
+        <v>1.55656501578947E-3</v>
       </c>
       <c r="G155">
-        <v>7.9918401173388803E-2</v>
+        <v>3.0022731684210501E-2</v>
       </c>
       <c r="H155">
-        <v>0.23527744324008401</v>
+        <v>0.15307809484210499</v>
       </c>
       <c r="I155">
-        <v>0.48581685237058297</v>
+        <v>0.42873054342105199</v>
       </c>
       <c r="J155">
-        <v>0.39825650762663101</v>
+        <v>0.385177901052631</v>
       </c>
       <c r="K155">
-        <v>0.56041072379102297</v>
+        <v>0.55401160168421004</v>
       </c>
       <c r="L155">
-        <v>0.56202519001550799</v>
+        <v>0.56030942694736896</v>
       </c>
       <c r="M155">
-        <v>0.71255147622362303</v>
+        <v>0.67838082189473703</v>
       </c>
       <c r="N155">
-        <v>0.72257147399907595</v>
+        <v>0.72237260368420997</v>
       </c>
       <c r="O155">
-        <v>0.83877249771893303</v>
+        <v>0.83846287136842101</v>
       </c>
       <c r="P155">
-        <v>0.935525702179549</v>
+        <v>0.93514555894736795</v>
       </c>
       <c r="Q155">
-        <v>1.0374082875248301</v>
+        <v>1.0369781346315801</v>
       </c>
       <c r="R155">
-        <v>1.1469440395449899</v>
+        <v>1.14346711210526</v>
       </c>
       <c r="S155">
-        <v>1.21574458512496</v>
+        <v>1.20379842</v>
       </c>
       <c r="T155">
-        <v>1.3174943374800101</v>
+        <v>1.28112265310526</v>
       </c>
       <c r="U155">
-        <v>1.3174943374800101</v>
+        <v>1.28112265310526</v>
       </c>
       <c r="V155">
-        <v>1.3174943374800101</v>
+        <v>1.28112265310526</v>
       </c>
       <c r="W155">
-        <v>1.3174943374800101</v>
+        <v>1.28112265310526</v>
       </c>
       <c r="X155">
-        <v>1.3174943374800101</v>
+        <v>1.28112265310526</v>
       </c>
       <c r="Y155">
-        <v>1.3174943374800101</v>
+        <v>1.28112265310526</v>
       </c>
     </row>
     <row r="156" spans="1:25" x14ac:dyDescent="0.2">
@@ -15990,64 +15990,64 @@
         <v>1982</v>
       </c>
       <c r="F156">
-        <v>4.2141051077331298E-3</v>
+        <v>1.0589922315789499E-3</v>
       </c>
       <c r="G156">
-        <v>8.1504126706391802E-2</v>
+        <v>3.0618436947368401E-2</v>
       </c>
       <c r="H156">
-        <v>0.24049320166249599</v>
+        <v>0.156471613368421</v>
       </c>
       <c r="I156">
-        <v>0.31335528714912098</v>
+        <v>0.27653421631578901</v>
       </c>
       <c r="J156">
-        <v>0.52164813763562201</v>
+        <v>0.50451739242105198</v>
       </c>
       <c r="K156">
-        <v>0.389747989353249</v>
+        <v>0.38529760168421001</v>
       </c>
       <c r="L156">
-        <v>0.54048503258332203</v>
+        <v>0.53883502778947401</v>
       </c>
       <c r="M156">
-        <v>0.56007919638931003</v>
+        <v>0.53322040336842103</v>
       </c>
       <c r="N156">
-        <v>0.69531812064667298</v>
+        <v>0.69512675115789402</v>
       </c>
       <c r="O156">
-        <v>0.68126416690030001</v>
+        <v>0.68101268352631605</v>
       </c>
       <c r="P156">
-        <v>0.80747207336965399</v>
+        <v>0.80714396368421004</v>
       </c>
       <c r="Q156">
-        <v>0.90374342226707605</v>
+        <v>0.903368692421052</v>
       </c>
       <c r="R156">
-        <v>0.95804549648366999</v>
+        <v>0.95514120947368397</v>
       </c>
       <c r="S156">
-        <v>1.06651428138938</v>
+        <v>1.0560344850000001</v>
       </c>
       <c r="T156">
-        <v>1.2003233542594101</v>
+        <v>1.1671863752631599</v>
       </c>
       <c r="U156">
-        <v>1.2003233542594101</v>
+        <v>1.1671863752631599</v>
       </c>
       <c r="V156">
-        <v>1.2003233542594101</v>
+        <v>1.1671863752631599</v>
       </c>
       <c r="W156">
-        <v>1.2003233542594101</v>
+        <v>1.1671863752631599</v>
       </c>
       <c r="X156">
-        <v>1.2003233542594101</v>
+        <v>1.1671863752631599</v>
       </c>
       <c r="Y156">
-        <v>1.2003233542594101</v>
+        <v>1.1671863752631599</v>
       </c>
     </row>
     <row r="157" spans="1:25" x14ac:dyDescent="0.2">
@@ -16067,64 +16067,64 @@
         <v>1983</v>
       </c>
       <c r="F157">
-        <v>4.1638418438606399E-3</v>
+        <v>1.04636122105263E-3</v>
       </c>
       <c r="G157">
-        <v>6.1170463633878798E-2</v>
+        <v>2.2979744210526301E-2</v>
       </c>
       <c r="H157">
-        <v>0.27056547870823699</v>
+        <v>0.176037479157895</v>
       </c>
       <c r="I157">
-        <v>0.35334284545672701</v>
+        <v>0.31182300368421001</v>
       </c>
       <c r="J157">
-        <v>0.371174991978036</v>
+        <v>0.35898573305263098</v>
       </c>
       <c r="K157">
-        <v>0.56316454933464</v>
+        <v>0.55673398231578897</v>
       </c>
       <c r="L157">
-        <v>0.414665310479987</v>
+        <v>0.41339941094736898</v>
       </c>
       <c r="M157">
-        <v>0.59417451009092004</v>
+        <v>0.56568066442105303</v>
       </c>
       <c r="N157">
-        <v>0.60291123530841495</v>
+        <v>0.60274529857894699</v>
       </c>
       <c r="O157">
-        <v>0.72319407315730599</v>
+        <v>0.72292711168420998</v>
       </c>
       <c r="P157">
-        <v>0.72349495374209105</v>
+        <v>0.72320096747368401</v>
       </c>
       <c r="Q157">
-        <v>0.86050535337518197</v>
+        <v>0.86014855184210504</v>
       </c>
       <c r="R157">
-        <v>0.92070013278588603</v>
+        <v>0.91790905715789495</v>
       </c>
       <c r="S157">
-        <v>0.98275938393561801</v>
+        <v>0.97310258099999902</v>
       </c>
       <c r="T157">
-        <v>1.1616070255828199</v>
+        <v>1.12953887705263</v>
       </c>
       <c r="U157">
-        <v>1.1616070255828199</v>
+        <v>1.12953887705263</v>
       </c>
       <c r="V157">
-        <v>1.1616070255828199</v>
+        <v>1.12953887705263</v>
       </c>
       <c r="W157">
-        <v>1.1616070255828199</v>
+        <v>1.12953887705263</v>
       </c>
       <c r="X157">
-        <v>1.1616070255828199</v>
+        <v>1.12953887705263</v>
       </c>
       <c r="Y157">
-        <v>1.1616070255828199</v>
+        <v>1.12953887705263</v>
       </c>
     </row>
     <row r="158" spans="1:25" x14ac:dyDescent="0.2">
@@ -16144,64 +16144,64 @@
         <v>1984</v>
       </c>
       <c r="F158">
-        <v>4.4088624689459302E-3</v>
+        <v>1.1079341842105299E-3</v>
       </c>
       <c r="G158">
-        <v>6.3022018433317201E-2</v>
+        <v>2.3675312842105299E-2</v>
       </c>
       <c r="H158">
-        <v>0.21173672215828601</v>
+        <v>0.13776184231579</v>
       </c>
       <c r="I158">
-        <v>0.41450278320986</v>
+        <v>0.36579629263157898</v>
       </c>
       <c r="J158">
-        <v>0.43641504180199397</v>
+        <v>0.422083322105263</v>
       </c>
       <c r="K158">
-        <v>0.417828518495859</v>
+        <v>0.41305748968421002</v>
       </c>
       <c r="L158">
-        <v>0.62475665846625505</v>
+        <v>0.62284938736842099</v>
       </c>
       <c r="M158">
-        <v>0.47532397572323198</v>
+        <v>0.452529648842105</v>
       </c>
       <c r="N158">
-        <v>0.66692895263613505</v>
+        <v>0.66674539657894705</v>
       </c>
       <c r="O158">
-        <v>0.65386247598952996</v>
+        <v>0.65362110773684201</v>
       </c>
       <c r="P158">
-        <v>0.80082297150875903</v>
+        <v>0.80049756363157898</v>
       </c>
       <c r="Q158">
-        <v>0.80393927365851603</v>
+        <v>0.80360592678947296</v>
       </c>
       <c r="R158">
-        <v>0.91408877126764398</v>
+        <v>0.911317737789474</v>
       </c>
       <c r="S158">
-        <v>0.98478402852439395</v>
+        <v>0.97510733099999902</v>
       </c>
       <c r="T158">
-        <v>1.11609581017416</v>
+        <v>1.08528407657895</v>
       </c>
       <c r="U158">
-        <v>1.11609581017416</v>
+        <v>1.08528407657895</v>
       </c>
       <c r="V158">
-        <v>1.11609581017416</v>
+        <v>1.08528407657895</v>
       </c>
       <c r="W158">
-        <v>1.11609581017416</v>
+        <v>1.08528407657895</v>
       </c>
       <c r="X158">
-        <v>1.11609581017416</v>
+        <v>1.08528407657895</v>
       </c>
       <c r="Y158">
-        <v>1.11609581017416</v>
+        <v>1.08528407657895</v>
       </c>
     </row>
     <row r="159" spans="1:25" x14ac:dyDescent="0.2">
@@ -16221,64 +16221,64 @@
         <v>1985</v>
       </c>
       <c r="F159">
-        <v>6.7625481031342296E-3</v>
+        <v>1.6994084684210499E-3</v>
       </c>
       <c r="G159">
-        <v>7.11080440401268E-2</v>
+        <v>2.6712968421052599E-2</v>
       </c>
       <c r="H159">
-        <v>0.23245604239189999</v>
+        <v>0.15124241242105299</v>
       </c>
       <c r="I159">
-        <v>0.34565702077792299</v>
+        <v>0.30504030815789501</v>
       </c>
       <c r="J159">
-        <v>0.54553792475521301</v>
+        <v>0.52762264715789498</v>
       </c>
       <c r="K159">
-        <v>0.52349564802821102</v>
+        <v>0.51751804547368396</v>
       </c>
       <c r="L159">
-        <v>0.49393255445286399</v>
+        <v>0.49242466610526298</v>
       </c>
       <c r="M159">
-        <v>0.76312712442445896</v>
+        <v>0.72653109726315801</v>
       </c>
       <c r="N159">
-        <v>0.56852467397626805</v>
+        <v>0.56836820131578902</v>
       </c>
       <c r="O159">
-        <v>0.77073769662177105</v>
+        <v>0.770453184789473</v>
       </c>
       <c r="P159">
-        <v>0.77154648577408702</v>
+        <v>0.77123297415789405</v>
       </c>
       <c r="Q159">
-        <v>0.94824015052550503</v>
+        <v>0.94784697047368405</v>
       </c>
       <c r="R159">
-        <v>0.91002228699694898</v>
+        <v>0.90726358094736903</v>
       </c>
       <c r="S159">
-        <v>1.0418499110352499</v>
+        <v>1.0316124719999999</v>
       </c>
       <c r="T159">
-        <v>1.19176129112689</v>
+        <v>1.1588606825263199</v>
       </c>
       <c r="U159">
-        <v>1.19176129112689</v>
+        <v>1.1588606825263199</v>
       </c>
       <c r="V159">
-        <v>1.19176129112689</v>
+        <v>1.1588606825263199</v>
       </c>
       <c r="W159">
-        <v>1.19176129112689</v>
+        <v>1.1588606825263199</v>
       </c>
       <c r="X159">
-        <v>1.19176129112689</v>
+        <v>1.1588606825263199</v>
       </c>
       <c r="Y159">
-        <v>1.19176129112689</v>
+        <v>1.1588606825263199</v>
       </c>
     </row>
     <row r="160" spans="1:25" x14ac:dyDescent="0.2">
@@ -16298,64 +16298,64 @@
         <v>1986</v>
       </c>
       <c r="F160">
-        <v>5.4042899033459896E-3</v>
+        <v>1.3580821736842101E-3</v>
       </c>
       <c r="G160">
-        <v>9.5560996250710795E-2</v>
+        <v>3.5899143473684197E-2</v>
       </c>
       <c r="H160">
-        <v>0.22979757982610299</v>
+        <v>0.14951274221052599</v>
       </c>
       <c r="I160">
-        <v>0.33248209591884298</v>
+        <v>0.29341351368420998</v>
       </c>
       <c r="J160">
-        <v>0.39858509843565199</v>
+        <v>0.38549570105263098</v>
       </c>
       <c r="K160">
-        <v>0.57334566093329997</v>
+        <v>0.56679883957894694</v>
       </c>
       <c r="L160">
-        <v>0.54220173674459504</v>
+        <v>0.54054649115789499</v>
       </c>
       <c r="M160">
-        <v>0.52860579951761599</v>
+        <v>0.50325632421052602</v>
       </c>
       <c r="N160">
-        <v>0.79971419403463995</v>
+        <v>0.799494092052631</v>
       </c>
       <c r="O160">
-        <v>0.57564487620187599</v>
+        <v>0.57543238136842101</v>
       </c>
       <c r="P160">
-        <v>0.79682065193571505</v>
+        <v>0.79649687036842098</v>
       </c>
       <c r="Q160">
-        <v>0.80042776600890297</v>
+        <v>0.80009587515789404</v>
       </c>
       <c r="R160">
-        <v>0.94042753087105702</v>
+        <v>0.937576652210527</v>
       </c>
       <c r="S160">
-        <v>0.90875557475119195</v>
+        <v>0.89982594899999901</v>
       </c>
       <c r="T160">
-        <v>1.10466779619883</v>
+        <v>1.0741715524736899</v>
       </c>
       <c r="U160">
-        <v>1.10466779619883</v>
+        <v>1.0741715524736899</v>
       </c>
       <c r="V160">
-        <v>1.10466779619883</v>
+        <v>1.0741715524736899</v>
       </c>
       <c r="W160">
-        <v>1.10466779619883</v>
+        <v>1.0741715524736899</v>
       </c>
       <c r="X160">
-        <v>1.10466779619883</v>
+        <v>1.0741715524736899</v>
       </c>
       <c r="Y160">
-        <v>1.10466779619883</v>
+        <v>1.0741715524736899</v>
       </c>
     </row>
     <row r="161" spans="1:25" x14ac:dyDescent="0.2">
@@ -16375,64 +16375,64 @@
         <v>1987</v>
       </c>
       <c r="F161">
-        <v>5.5181611742136198E-3</v>
+        <v>1.3866976894736801E-3</v>
       </c>
       <c r="G161">
-        <v>7.1648218506415506E-2</v>
+        <v>2.6915894315789501E-2</v>
       </c>
       <c r="H161">
-        <v>0.289736964049433</v>
+        <v>0.18851098452631601</v>
       </c>
       <c r="I161">
-        <v>0.30836787687510397</v>
+        <v>0.27213285578947299</v>
       </c>
       <c r="J161">
-        <v>0.35969990915691202</v>
+        <v>0.34788748800000002</v>
       </c>
       <c r="K161">
-        <v>0.39301498661428702</v>
+        <v>0.38852729431578897</v>
       </c>
       <c r="L161">
-        <v>0.55713537491018705</v>
+        <v>0.55543453957894795</v>
       </c>
       <c r="M161">
-        <v>0.54440426772324402</v>
+        <v>0.51829717136842102</v>
       </c>
       <c r="N161">
-        <v>0.51971613576499298</v>
+        <v>0.51957309647368399</v>
       </c>
       <c r="O161">
-        <v>0.75969003393661205</v>
+        <v>0.75940960026315796</v>
       </c>
       <c r="P161">
-        <v>0.55834797751116705</v>
+        <v>0.55812109736842097</v>
       </c>
       <c r="Q161">
-        <v>0.775562844234855</v>
+        <v>0.77524126342105204</v>
       </c>
       <c r="R161">
-        <v>0.74477574428559001</v>
+        <v>0.74251797831579003</v>
       </c>
       <c r="S161">
-        <v>0.88108293247670799</v>
+        <v>0.872425223999999</v>
       </c>
       <c r="T161">
-        <v>0.90400325142011295</v>
+        <v>0.87904669563158</v>
       </c>
       <c r="U161">
-        <v>0.90400325142011295</v>
+        <v>0.87904669563158</v>
       </c>
       <c r="V161">
-        <v>0.90400325142011295</v>
+        <v>0.87904669563158</v>
       </c>
       <c r="W161">
-        <v>0.90400325142011295</v>
+        <v>0.87904669563158</v>
       </c>
       <c r="X161">
-        <v>0.90400325142011295</v>
+        <v>0.87904669563158</v>
       </c>
       <c r="Y161">
-        <v>0.90400325142011295</v>
+        <v>0.87904669563158</v>
       </c>
     </row>
     <row r="162" spans="1:25" x14ac:dyDescent="0.2">
@@ -16452,64 +16452,64 @@
         <v>1988</v>
       </c>
       <c r="F162">
-        <v>6.4099691802330001E-3</v>
+        <v>1.61080642105263E-3</v>
       </c>
       <c r="G162">
-        <v>8.3928524854627595E-2</v>
+        <v>3.1529204105263199E-2</v>
       </c>
       <c r="H162">
-        <v>0.24921654541148699</v>
+        <v>0.16214726515789499</v>
       </c>
       <c r="I162">
-        <v>0.44604227921658102</v>
+        <v>0.393629714210526</v>
       </c>
       <c r="J162">
-        <v>0.38272745422877202</v>
+        <v>0.37015881642105197</v>
       </c>
       <c r="K162">
-        <v>0.40688965887475598</v>
+        <v>0.40224353684210501</v>
       </c>
       <c r="L162">
-        <v>0.43812863204327002</v>
+        <v>0.43679110315789499</v>
       </c>
       <c r="M162">
-        <v>0.64175582372364903</v>
+        <v>0.610980199578947</v>
       </c>
       <c r="N162">
-        <v>0.61405063684336902</v>
+        <v>0.613881634263158</v>
       </c>
       <c r="O162">
-        <v>0.56639093144322605</v>
+        <v>0.56618185263157905</v>
       </c>
       <c r="P162">
-        <v>0.84534732693291303</v>
+        <v>0.84500382694736798</v>
       </c>
       <c r="Q162">
-        <v>0.62346163891997197</v>
+        <v>0.62320312563157898</v>
       </c>
       <c r="R162">
-        <v>0.82788270429776101</v>
+        <v>0.82537300199999997</v>
       </c>
       <c r="S162">
-        <v>0.80050737691323903</v>
+        <v>0.79264142099999901</v>
       </c>
       <c r="T162">
-        <v>1.005513874674</v>
+        <v>0.97775494452631695</v>
       </c>
       <c r="U162">
-        <v>1.005513874674</v>
+        <v>0.97775494452631695</v>
       </c>
       <c r="V162">
-        <v>1.005513874674</v>
+        <v>0.97775494452631695</v>
       </c>
       <c r="W162">
-        <v>1.005513874674</v>
+        <v>0.97775494452631695</v>
       </c>
       <c r="X162">
-        <v>1.005513874674</v>
+        <v>0.97775494452631695</v>
       </c>
       <c r="Y162">
-        <v>1.005513874674</v>
+        <v>0.97775494452631695</v>
       </c>
     </row>
     <row r="163" spans="1:25" x14ac:dyDescent="0.2">
@@ -16529,64 +16529,64 @@
         <v>1989</v>
       </c>
       <c r="F163">
-        <v>6.2531677573911103E-3</v>
+        <v>1.57140268421053E-3</v>
       </c>
       <c r="G163">
-        <v>8.9468506609118703E-2</v>
+        <v>3.36103942105263E-2</v>
       </c>
       <c r="H163">
-        <v>0.26790457364400999</v>
+        <v>0.174306219789474</v>
       </c>
       <c r="I163">
-        <v>0.352085481561973</v>
+        <v>0.31071338736842102</v>
       </c>
       <c r="J163">
-        <v>0.50803736279231904</v>
+        <v>0.49135359073684198</v>
       </c>
       <c r="K163">
-        <v>0.397306035030211</v>
+        <v>0.39276934484210502</v>
       </c>
       <c r="L163">
-        <v>0.41626355236539703</v>
+        <v>0.414992773684211</v>
       </c>
       <c r="M163">
-        <v>0.46313733988135097</v>
+        <v>0.440927427368421</v>
       </c>
       <c r="N163">
-        <v>0.66428061795661997</v>
+        <v>0.66409779078947295</v>
       </c>
       <c r="O163">
-        <v>0.61412022570978297</v>
+        <v>0.61389352799999997</v>
       </c>
       <c r="P163">
-        <v>0.57838107279590101</v>
+        <v>0.57814605236842098</v>
       </c>
       <c r="Q163">
-        <v>0.86624171243603998</v>
+        <v>0.86588253236842105</v>
       </c>
       <c r="R163">
-        <v>0.61074604251805098</v>
+        <v>0.60889458368421101</v>
       </c>
       <c r="S163">
-        <v>0.81659695250850195</v>
+        <v>0.80857289699999901</v>
       </c>
       <c r="T163">
-        <v>0.83837009797289497</v>
+        <v>0.81522545763158005</v>
       </c>
       <c r="U163">
-        <v>0.83837009797289497</v>
+        <v>0.81522545763158005</v>
       </c>
       <c r="V163">
-        <v>0.83837009797289497</v>
+        <v>0.81522545763158005</v>
       </c>
       <c r="W163">
-        <v>0.83837009797289497</v>
+        <v>0.81522545763158005</v>
       </c>
       <c r="X163">
-        <v>0.83837009797289497</v>
+        <v>0.81522545763158005</v>
       </c>
       <c r="Y163">
-        <v>0.83837009797289497</v>
+        <v>0.81522545763158005</v>
       </c>
     </row>
     <row r="164" spans="1:25" x14ac:dyDescent="0.2">
@@ -16606,64 +16606,64 @@
         <v>1990</v>
       </c>
       <c r="F164">
-        <v>6.1711675316661104E-3</v>
+        <v>1.55079626842105E-3</v>
       </c>
       <c r="G164">
-        <v>9.1535492500066207E-2</v>
+        <v>3.43868932631579E-2</v>
       </c>
       <c r="H164">
-        <v>0.29951326099273701</v>
+        <v>0.194871717157895</v>
       </c>
       <c r="I164">
-        <v>0.39694163886318001</v>
+        <v>0.350298685</v>
       </c>
       <c r="J164">
-        <v>0.42057449419961401</v>
+        <v>0.40676297263157901</v>
       </c>
       <c r="K164">
-        <v>0.55310333394418598</v>
+        <v>0.54678765221052605</v>
       </c>
       <c r="L164">
-        <v>0.42627711061151402</v>
+        <v>0.42497576231578998</v>
       </c>
       <c r="M164">
-        <v>0.46147875159697999</v>
+        <v>0.43934837726315801</v>
       </c>
       <c r="N164">
-        <v>0.50276699376586398</v>
+        <v>0.50262861931578895</v>
       </c>
       <c r="O164">
-        <v>0.69674833191740304</v>
+        <v>0.69649113268421003</v>
       </c>
       <c r="P164">
-        <v>0.65769785183737395</v>
+        <v>0.65743060168420997</v>
       </c>
       <c r="Q164">
-        <v>0.62157454976962201</v>
+        <v>0.62131681894736801</v>
       </c>
       <c r="R164">
-        <v>0.88994923274940396</v>
+        <v>0.88725137757894801</v>
       </c>
       <c r="S164">
-        <v>0.63179299346222695</v>
+        <v>0.62558486099999999</v>
       </c>
       <c r="T164">
-        <v>0.89691925035020303</v>
+        <v>0.87215826052631595</v>
       </c>
       <c r="U164">
-        <v>0.89691925035020303</v>
+        <v>0.87215826052631595</v>
       </c>
       <c r="V164">
-        <v>0.89691925035020303</v>
+        <v>0.87215826052631595</v>
       </c>
       <c r="W164">
-        <v>0.89691925035020303</v>
+        <v>0.87215826052631595</v>
       </c>
       <c r="X164">
-        <v>0.89691925035020303</v>
+        <v>0.87215826052631595</v>
       </c>
       <c r="Y164">
-        <v>0.89691925035020303</v>
+        <v>0.87215826052631595</v>
       </c>
     </row>
     <row r="165" spans="1:25" x14ac:dyDescent="0.2">
@@ -16683,64 +16683,64 @@
         <v>1991</v>
       </c>
       <c r="F165">
-        <v>6.5083151266359697E-3</v>
+        <v>1.6355204684210499E-3</v>
       </c>
       <c r="G165">
-        <v>8.9436278205924799E-2</v>
+        <v>3.3598287052631598E-2</v>
       </c>
       <c r="H165">
-        <v>0.303383754311909</v>
+        <v>0.19738996852631599</v>
       </c>
       <c r="I165">
-        <v>0.43935888309905102</v>
+        <v>0.38773165605263099</v>
       </c>
       <c r="J165">
-        <v>0.469438171047806</v>
+        <v>0.45402198315789399</v>
       </c>
       <c r="K165">
-        <v>0.45332596860153201</v>
+        <v>0.44814960757894701</v>
       </c>
       <c r="L165">
-        <v>0.58753013798575304</v>
+        <v>0.58573651284210604</v>
       </c>
       <c r="M165">
-        <v>0.467877719932143</v>
+        <v>0.44544048084210502</v>
       </c>
       <c r="N165">
-        <v>0.49598169838275002</v>
+        <v>0.49584519142105199</v>
       </c>
       <c r="O165">
-        <v>0.52209329752637201</v>
+        <v>0.52190057084210495</v>
       </c>
       <c r="P165">
-        <v>0.73876432085108401</v>
+        <v>0.73846413</v>
       </c>
       <c r="Q165">
-        <v>0.69978151149114698</v>
+        <v>0.69949135278947305</v>
       </c>
       <c r="R165">
-        <v>0.63223171761084795</v>
+        <v>0.63031512557894798</v>
       </c>
       <c r="S165">
-        <v>0.911457200500984</v>
+        <v>0.90250102799999898</v>
       </c>
       <c r="T165">
-        <v>0.68703263799274705</v>
+        <v>0.66806592705263201</v>
       </c>
       <c r="U165">
-        <v>0.68703263799274705</v>
+        <v>0.66806592705263201</v>
       </c>
       <c r="V165">
-        <v>0.68703263799274705</v>
+        <v>0.66806592705263201</v>
       </c>
       <c r="W165">
-        <v>0.68703263799274705</v>
+        <v>0.66806592705263201</v>
       </c>
       <c r="X165">
-        <v>0.68703263799274705</v>
+        <v>0.66806592705263201</v>
       </c>
       <c r="Y165">
-        <v>0.68703263799274705</v>
+        <v>0.66806592705263201</v>
       </c>
     </row>
     <row r="166" spans="1:25" x14ac:dyDescent="0.2">
@@ -16760,64 +16760,64 @@
         <v>1992</v>
       </c>
       <c r="F166">
-        <v>7.1052186855856004E-3</v>
+        <v>1.7855205789473699E-3</v>
       </c>
       <c r="G166">
-        <v>9.4738327717246301E-2</v>
+        <v>3.5590093789473698E-2</v>
       </c>
       <c r="H166">
-        <v>0.297733231168888</v>
+        <v>0.193713579894737</v>
       </c>
       <c r="I166">
-        <v>0.44699904771812699</v>
+        <v>0.39447405684210501</v>
       </c>
       <c r="J166">
-        <v>0.521893716029732</v>
+        <v>0.50475490610526297</v>
       </c>
       <c r="K166">
-        <v>0.50822597391713997</v>
+        <v>0.50242273010526295</v>
       </c>
       <c r="L166">
-        <v>0.483665790583379</v>
+        <v>0.48218924484210601</v>
       </c>
       <c r="M166">
-        <v>0.647711109197879</v>
+        <v>0.616649897263158</v>
       </c>
       <c r="N166">
-        <v>0.50507641358831801</v>
+        <v>0.504937403526316</v>
       </c>
       <c r="O166">
-        <v>0.51731834841732405</v>
+        <v>0.51712738436842098</v>
       </c>
       <c r="P166">
-        <v>0.55601815717611303</v>
+        <v>0.55579222373684201</v>
       </c>
       <c r="Q166">
-        <v>0.78950128685440701</v>
+        <v>0.78917392657894703</v>
       </c>
       <c r="R166">
-        <v>0.71491823094590301</v>
+        <v>0.71275097715789504</v>
       </c>
       <c r="S166">
-        <v>0.65036653301618297</v>
+        <v>0.64397589300000002</v>
       </c>
       <c r="T166">
-        <v>0.99551933597197095</v>
+        <v>0.96803632215789504</v>
       </c>
       <c r="U166">
-        <v>0.99551933597197095</v>
+        <v>0.96803632215789504</v>
       </c>
       <c r="V166">
-        <v>0.99551933597197095</v>
+        <v>0.96803632215789504</v>
       </c>
       <c r="W166">
-        <v>0.99551933597197095</v>
+        <v>0.96803632215789504</v>
       </c>
       <c r="X166">
-        <v>0.99551933597197095</v>
+        <v>0.96803632215789504</v>
       </c>
       <c r="Y166">
-        <v>0.99551933597197095</v>
+        <v>0.96803632215789504</v>
       </c>
     </row>
     <row r="167" spans="1:25" x14ac:dyDescent="0.2">
@@ -16837,64 +16837,64 @@
         <v>1993</v>
       </c>
       <c r="F167">
-        <v>5.5221822906155E-3</v>
+        <v>1.3877081842105299E-3</v>
       </c>
       <c r="G167">
-        <v>8.7417891866035005E-2</v>
+        <v>3.2840045263157903E-2</v>
       </c>
       <c r="H167">
-        <v>0.26656624208470198</v>
+        <v>0.173435463789474</v>
       </c>
       <c r="I167">
-        <v>0.37077233663119302</v>
+        <v>0.32720442815789402</v>
       </c>
       <c r="J167">
-        <v>0.44878142101606699</v>
+        <v>0.43404359368421003</v>
       </c>
       <c r="K167">
-        <v>0.47755805868869</v>
+        <v>0.47210500042105202</v>
       </c>
       <c r="L167">
-        <v>0.45830787167727499</v>
+        <v>0.45690873915789498</v>
       </c>
       <c r="M167">
-        <v>0.45067363963521001</v>
+        <v>0.42906142821052601</v>
       </c>
       <c r="N167">
-        <v>0.59097863304310005</v>
+        <v>0.590815980473684</v>
       </c>
       <c r="O167">
-        <v>0.44526127984716601</v>
+        <v>0.445096915105263</v>
       </c>
       <c r="P167">
-        <v>0.46565510409767502</v>
+        <v>0.46546588894736801</v>
       </c>
       <c r="Q167">
-        <v>0.50222868461068504</v>
+        <v>0.50202043957894704</v>
       </c>
       <c r="R167">
-        <v>0.68173004001730197</v>
+        <v>0.679663395263158</v>
       </c>
       <c r="S167">
-        <v>0.62158998452418501</v>
+        <v>0.615482109</v>
       </c>
       <c r="T167">
-        <v>0.60039530790686702</v>
+        <v>0.58382036863157905</v>
       </c>
       <c r="U167">
-        <v>0.60039530790686702</v>
+        <v>0.58382036863157905</v>
       </c>
       <c r="V167">
-        <v>0.60039530790686702</v>
+        <v>0.58382036863157905</v>
       </c>
       <c r="W167">
-        <v>0.60039530790686702</v>
+        <v>0.58382036863157905</v>
       </c>
       <c r="X167">
-        <v>0.60039530790686702</v>
+        <v>0.58382036863157905</v>
       </c>
       <c r="Y167">
-        <v>0.60039530790686702</v>
+        <v>0.58382036863157905</v>
       </c>
     </row>
     <row r="168" spans="1:25" x14ac:dyDescent="0.2">
@@ -16914,64 +16914,64 @@
         <v>1994</v>
       </c>
       <c r="F168">
-        <v>6.4527085745367798E-3</v>
+        <v>1.6215467052631599E-3</v>
       </c>
       <c r="G168">
-        <v>8.7086871661020707E-2</v>
+        <v>3.27156917894737E-2</v>
       </c>
       <c r="H168">
-        <v>0.31528163690795602</v>
+        <v>0.20513106421052599</v>
       </c>
       <c r="I168">
-        <v>0.425504384351022</v>
+        <v>0.37550514157894699</v>
       </c>
       <c r="J168">
-        <v>0.47714962909577502</v>
+        <v>0.46148019957894698</v>
       </c>
       <c r="K168">
-        <v>0.52637833957117297</v>
+        <v>0.52036782063157805</v>
       </c>
       <c r="L168">
-        <v>0.55200833560151397</v>
+        <v>0.55032315221052697</v>
       </c>
       <c r="M168">
-        <v>0.54738530879720704</v>
+        <v>0.52113525557894702</v>
       </c>
       <c r="N168">
-        <v>0.52707398730928401</v>
+        <v>0.52692892294736804</v>
       </c>
       <c r="O168">
-        <v>0.66780338369360803</v>
+        <v>0.66755686926315805</v>
       </c>
       <c r="P168">
-        <v>0.51373663252899004</v>
+        <v>0.51352787984210502</v>
       </c>
       <c r="Q168">
-        <v>0.53913306118340498</v>
+        <v>0.53890951405263099</v>
       </c>
       <c r="R168">
-        <v>0.55587890100869597</v>
+        <v>0.55419377031578998</v>
       </c>
       <c r="S168">
-        <v>0.75976462899811104</v>
+        <v>0.75229902000000004</v>
       </c>
       <c r="T168">
-        <v>0.73553296775189903</v>
+        <v>0.71522732226315799</v>
       </c>
       <c r="U168">
-        <v>0.73553296775189903</v>
+        <v>0.71522732226315799</v>
       </c>
       <c r="V168">
-        <v>0.73553296775189903</v>
+        <v>0.71522732226315799</v>
       </c>
       <c r="W168">
-        <v>0.73553296775189903</v>
+        <v>0.71522732226315799</v>
       </c>
       <c r="X168">
-        <v>0.73553296775189903</v>
+        <v>0.71522732226315799</v>
       </c>
       <c r="Y168">
-        <v>0.73553296775189903</v>
+        <v>0.71522732226315799</v>
       </c>
     </row>
     <row r="169" spans="1:25" x14ac:dyDescent="0.2">
@@ -16991,64 +16991,64 @@
         <v>1995</v>
       </c>
       <c r="F169">
-        <v>7.4252782637249199E-3</v>
+        <v>1.8659506105263199E-3</v>
       </c>
       <c r="G169">
-        <v>9.9896010133167401E-2</v>
+        <v>3.7527666526315798E-2</v>
       </c>
       <c r="H169">
-        <v>0.308329577262627</v>
+        <v>0.20060785947368401</v>
       </c>
       <c r="I169">
-        <v>0.49403965837681102</v>
+        <v>0.43598712184210497</v>
       </c>
       <c r="J169">
-        <v>0.53754590450970796</v>
+        <v>0.51989308210526297</v>
       </c>
       <c r="K169">
-        <v>0.54939153470706503</v>
+        <v>0.54311823663157899</v>
       </c>
       <c r="L169">
-        <v>0.59728499699537096</v>
+        <v>0.59546159200000004</v>
       </c>
       <c r="M169">
-        <v>0.64721065412135403</v>
+        <v>0.61617344168420995</v>
       </c>
       <c r="N169">
-        <v>0.62844422085541696</v>
+        <v>0.62827125678947404</v>
       </c>
       <c r="O169">
-        <v>0.58467245655775901</v>
+        <v>0.584456629263158</v>
       </c>
       <c r="P169">
-        <v>0.75637700667482399</v>
+        <v>0.75606965905263102</v>
       </c>
       <c r="Q169">
-        <v>0.58389705957900795</v>
+        <v>0.58365495142105295</v>
       </c>
       <c r="R169">
-        <v>0.58578570809673403</v>
+        <v>0.58400991578947403</v>
       </c>
       <c r="S169">
-        <v>0.60815034375267096</v>
+        <v>0.60217452900000001</v>
       </c>
       <c r="T169">
-        <v>0.88255410662178402</v>
+        <v>0.85818969115789501</v>
       </c>
       <c r="U169">
-        <v>0.88255410662178402</v>
+        <v>0.85818969115789501</v>
       </c>
       <c r="V169">
-        <v>0.88255410662178402</v>
+        <v>0.85818969115789501</v>
       </c>
       <c r="W169">
-        <v>0.88255410662178402</v>
+        <v>0.85818969115789501</v>
       </c>
       <c r="X169">
-        <v>0.88255410662178402</v>
+        <v>0.85818969115789501</v>
       </c>
       <c r="Y169">
-        <v>0.88255410662178402</v>
+        <v>0.85818969115789501</v>
       </c>
     </row>
     <row r="170" spans="1:25" x14ac:dyDescent="0.2">
@@ -17068,64 +17068,64 @@
         <v>1996</v>
       </c>
       <c r="F170">
-        <v>6.4100362218780698E-3</v>
+        <v>1.6108232684210501E-3</v>
       </c>
       <c r="G170">
-        <v>0.10279150090849901</v>
+        <v>3.8615407789473699E-2</v>
       </c>
       <c r="H170">
-        <v>0.31626352127697099</v>
+        <v>0.20576990568421</v>
       </c>
       <c r="I170">
-        <v>0.43203272651572699</v>
+        <v>0.38126636552631499</v>
       </c>
       <c r="J170">
-        <v>0.55809948196862902</v>
+        <v>0.53977168715789503</v>
       </c>
       <c r="K170">
-        <v>0.55345365412028602</v>
+        <v>0.54713397221052595</v>
       </c>
       <c r="L170">
-        <v>0.55744741213598703</v>
+        <v>0.55574562421052698</v>
       </c>
       <c r="M170">
-        <v>0.62621003185783597</v>
+        <v>0.59617991157894701</v>
       </c>
       <c r="N170">
-        <v>0.66444287719349704</v>
+        <v>0.664260005368421</v>
       </c>
       <c r="O170">
-        <v>0.62337037106591198</v>
+        <v>0.62314025873684198</v>
       </c>
       <c r="P170">
-        <v>0.59216221854671502</v>
+        <v>0.59192159826315804</v>
       </c>
       <c r="Q170">
-        <v>0.76872770794339296</v>
+        <v>0.76840896126315805</v>
       </c>
       <c r="R170">
-        <v>0.56730605176750204</v>
+        <v>0.56558628</v>
       </c>
       <c r="S170">
-        <v>0.57307030179183704</v>
+        <v>0.56743919099999995</v>
       </c>
       <c r="T170">
-        <v>0.63170113225373203</v>
+        <v>0.61426194215789498</v>
       </c>
       <c r="U170">
-        <v>0.63170113225373203</v>
+        <v>0.61426194215789498</v>
       </c>
       <c r="V170">
-        <v>0.63170113225373203</v>
+        <v>0.61426194215789498</v>
       </c>
       <c r="W170">
-        <v>0.63170113225373203</v>
+        <v>0.61426194215789498</v>
       </c>
       <c r="X170">
-        <v>0.63170113225373203</v>
+        <v>0.61426194215789498</v>
       </c>
       <c r="Y170">
-        <v>0.63170113225373203</v>
+        <v>0.61426194215789498</v>
       </c>
     </row>
     <row r="171" spans="1:25" x14ac:dyDescent="0.2">
@@ -17145,64 +17145,64 @@
         <v>1997</v>
       </c>
       <c r="F171">
-        <v>6.2958677560890196E-3</v>
+        <v>1.58213306842105E-3</v>
       </c>
       <c r="G171">
-        <v>9.3929864641681696E-2</v>
+        <v>3.5286380631578997E-2</v>
       </c>
       <c r="H171">
-        <v>0.34447429935766999</v>
+        <v>0.22412462810526301</v>
       </c>
       <c r="I171">
-        <v>0.46908253560547197</v>
+        <v>0.41396260631578902</v>
       </c>
       <c r="J171">
-        <v>0.51661294054978402</v>
+        <v>0.49964754947368401</v>
       </c>
       <c r="K171">
-        <v>0.60824163671101905</v>
+        <v>0.60129635115789404</v>
       </c>
       <c r="L171">
-        <v>0.59443171421938101</v>
+        <v>0.59261701978947401</v>
       </c>
       <c r="M171">
-        <v>0.61864433452162104</v>
+        <v>0.58897702989473599</v>
       </c>
       <c r="N171">
-        <v>0.68050414224703104</v>
+        <v>0.68031684994736796</v>
       </c>
       <c r="O171">
-        <v>0.69764709058191798</v>
+        <v>0.69738955957894699</v>
       </c>
       <c r="P171">
-        <v>0.66830227891238103</v>
+        <v>0.66803071973684203</v>
       </c>
       <c r="Q171">
-        <v>0.63705012064161504</v>
+        <v>0.63678597299999995</v>
       </c>
       <c r="R171">
-        <v>0.79059193367624403</v>
+        <v>0.78819527726315797</v>
       </c>
       <c r="S171">
-        <v>0.58746957410720702</v>
+        <v>0.58169697300000001</v>
       </c>
       <c r="T171">
-        <v>0.63009690757204795</v>
+        <v>0.61270200484210502</v>
       </c>
       <c r="U171">
-        <v>0.63009690757204795</v>
+        <v>0.61270200484210502</v>
       </c>
       <c r="V171">
-        <v>0.63009690757204795</v>
+        <v>0.61270200484210502</v>
       </c>
       <c r="W171">
-        <v>0.63009690757204795</v>
+        <v>0.61270200484210502</v>
       </c>
       <c r="X171">
-        <v>0.63009690757204795</v>
+        <v>0.61270200484210502</v>
       </c>
       <c r="Y171">
-        <v>0.63009690757204795</v>
+        <v>0.61270200484210502</v>
       </c>
     </row>
     <row r="172" spans="1:25" x14ac:dyDescent="0.2">
@@ -17222,64 +17222,64 @@
         <v>1998</v>
       </c>
       <c r="F172">
-        <v>6.5478323750707904E-3</v>
+        <v>1.6454510368421099E-3</v>
       </c>
       <c r="G172">
-        <v>8.4850264527295202E-2</v>
+        <v>3.1875471578947399E-2</v>
       </c>
       <c r="H172">
-        <v>0.28950610855262499</v>
+        <v>0.18836078347368401</v>
       </c>
       <c r="I172">
-        <v>0.46990660455843503</v>
+        <v>0.41468984236842099</v>
       </c>
       <c r="J172">
-        <v>0.51588430896033799</v>
+        <v>0.49894284589473697</v>
       </c>
       <c r="K172">
-        <v>0.51782634137180805</v>
+        <v>0.51191347452631497</v>
       </c>
       <c r="L172">
-        <v>0.60082957607090004</v>
+        <v>0.59899535010526395</v>
       </c>
       <c r="M172">
-        <v>0.60672736670379901</v>
+        <v>0.57763154442105202</v>
       </c>
       <c r="N172">
-        <v>0.61830996680509198</v>
+        <v>0.61813979194736801</v>
       </c>
       <c r="O172">
-        <v>0.65714825927932297</v>
+        <v>0.65690567810526301</v>
       </c>
       <c r="P172">
-        <v>0.687886928027307</v>
+        <v>0.68760741078947396</v>
       </c>
       <c r="Q172">
-        <v>0.66124181763691503</v>
+        <v>0.66096763910526302</v>
       </c>
       <c r="R172">
-        <v>0.60257067935333197</v>
+        <v>0.60074400389473703</v>
       </c>
       <c r="S172">
-        <v>0.75296502261818898</v>
+        <v>0.74556622800000005</v>
       </c>
       <c r="T172">
-        <v>0.59407218139620899</v>
+        <v>0.57767180284210495</v>
       </c>
       <c r="U172">
-        <v>0.59407218139620899</v>
+        <v>0.57767180284210495</v>
       </c>
       <c r="V172">
-        <v>0.59407218139620899</v>
+        <v>0.57767180284210495</v>
       </c>
       <c r="W172">
-        <v>0.59407218139620899</v>
+        <v>0.57767180284210495</v>
       </c>
       <c r="X172">
-        <v>0.59407218139620899</v>
+        <v>0.57767180284210495</v>
       </c>
       <c r="Y172">
-        <v>0.59407218139620899</v>
+        <v>0.57767180284210495</v>
       </c>
     </row>
     <row r="173" spans="1:25" x14ac:dyDescent="0.2">
@@ -17299,64 +17299,64 @@
         <v>1999</v>
       </c>
       <c r="F173">
-        <v>5.9225356427101E-3</v>
+        <v>1.48831580526316E-3</v>
       </c>
       <c r="G173">
-        <v>9.3202119400540101E-2</v>
+        <v>3.5012990526315797E-2</v>
       </c>
       <c r="H173">
-        <v>0.27620898951705403</v>
+        <v>0.179709305368421</v>
       </c>
       <c r="I173">
-        <v>0.41710264798573599</v>
+        <v>0.36809065815789399</v>
       </c>
       <c r="J173">
-        <v>0.54581453398061097</v>
+        <v>0.527890172631579</v>
       </c>
       <c r="K173">
-        <v>0.54613719481796497</v>
+        <v>0.53990105684210499</v>
       </c>
       <c r="L173">
-        <v>0.54024391290884</v>
+        <v>0.53859464421052705</v>
       </c>
       <c r="M173">
-        <v>0.64769921501890804</v>
+        <v>0.616638573473684</v>
       </c>
       <c r="N173">
-        <v>0.64045600322893004</v>
+        <v>0.640279733210526</v>
       </c>
       <c r="O173">
-        <v>0.63062233064939399</v>
+        <v>0.63038954131578995</v>
       </c>
       <c r="P173">
-        <v>0.68434505318379801</v>
+        <v>0.68406697515789505</v>
       </c>
       <c r="Q173">
-        <v>0.71884448153318603</v>
+        <v>0.71854641852631596</v>
       </c>
       <c r="R173">
-        <v>0.660579722393006</v>
+        <v>0.65857719421052596</v>
       </c>
       <c r="S173">
-        <v>0.60612309962022604</v>
+        <v>0.60016720499999998</v>
       </c>
       <c r="T173">
-        <v>0.804190924975132</v>
+        <v>0.78198985915789498</v>
       </c>
       <c r="U173">
-        <v>0.804190924975132</v>
+        <v>0.78198985915789498</v>
       </c>
       <c r="V173">
-        <v>0.804190924975132</v>
+        <v>0.78198985915789498</v>
       </c>
       <c r="W173">
-        <v>0.804190924975132</v>
+        <v>0.78198985915789498</v>
       </c>
       <c r="X173">
-        <v>0.804190924975132</v>
+        <v>0.78198985915789498</v>
       </c>
       <c r="Y173">
-        <v>0.804190924975132</v>
+        <v>0.78198985915789498</v>
       </c>
     </row>
     <row r="174" spans="1:25" x14ac:dyDescent="0.2">
@@ -17376,64 +17376,64 @@
         <v>2000</v>
       </c>
       <c r="F174">
-        <v>7.4791880401681096E-3</v>
+        <v>1.8794979789473699E-3</v>
       </c>
       <c r="G174">
-        <v>0.111258687948983</v>
+        <v>4.1796253263157897E-2</v>
       </c>
       <c r="H174">
-        <v>0.40041326510338499</v>
+        <v>0.260520086105263</v>
       </c>
       <c r="I174">
-        <v>0.52519570500694301</v>
+        <v>0.46348215157894701</v>
       </c>
       <c r="J174">
-        <v>0.63940292819928102</v>
+        <v>0.61840515621052605</v>
       </c>
       <c r="K174">
-        <v>0.76259260663621498</v>
+        <v>0.75388484463157801</v>
       </c>
       <c r="L174">
-        <v>0.75197875017593596</v>
+        <v>0.74968309263157995</v>
       </c>
       <c r="M174">
-        <v>0.76861713760365802</v>
+        <v>0.73175783494736801</v>
       </c>
       <c r="N174">
-        <v>0.90233371373234805</v>
+        <v>0.90208536821052598</v>
       </c>
       <c r="O174">
-        <v>0.86208583154971496</v>
+        <v>0.86176759926315805</v>
       </c>
       <c r="P174">
-        <v>0.866720861315186</v>
+        <v>0.86636867636842096</v>
       </c>
       <c r="Q174">
-        <v>0.94382424392686903</v>
+        <v>0.94343289489473703</v>
       </c>
       <c r="R174">
-        <v>0.94775900106196997</v>
+        <v>0.94488589726315797</v>
       </c>
       <c r="S174">
-        <v>0.87695275749805601</v>
+        <v>0.86833563300000005</v>
       </c>
       <c r="T174">
-        <v>0.85436475888904195</v>
+        <v>0.830778558578947</v>
       </c>
       <c r="U174">
-        <v>0.85436475888904195</v>
+        <v>0.830778558578947</v>
       </c>
       <c r="V174">
-        <v>0.85436475888904195</v>
+        <v>0.830778558578947</v>
       </c>
       <c r="W174">
-        <v>0.85436475888904195</v>
+        <v>0.830778558578947</v>
       </c>
       <c r="X174">
-        <v>0.85436475888904195</v>
+        <v>0.830778558578947</v>
       </c>
       <c r="Y174">
-        <v>0.85436475888904195</v>
+        <v>0.830778558578947</v>
       </c>
     </row>
     <row r="175" spans="1:25" x14ac:dyDescent="0.2">
@@ -17453,64 +17453,64 @@
         <v>2001</v>
       </c>
       <c r="F175">
-        <v>8.1184418754197494E-3</v>
+        <v>2.0401405894736801E-3</v>
       </c>
       <c r="G175">
-        <v>0.11224374652314199</v>
+        <v>4.2166307578947397E-2</v>
       </c>
       <c r="H175">
-        <v>0.38185461049739999</v>
+        <v>0.24844530557894701</v>
       </c>
       <c r="I175">
-        <v>0.608237465383623</v>
+        <v>0.53676602157894704</v>
       </c>
       <c r="J175">
-        <v>0.64318256250959704</v>
+        <v>0.62206066863157905</v>
       </c>
       <c r="K175">
-        <v>0.71368013623370596</v>
+        <v>0.705530887578947</v>
       </c>
       <c r="L175">
-        <v>0.83883746830772898</v>
+        <v>0.83627664652631595</v>
       </c>
       <c r="M175">
-        <v>0.854687114825878</v>
+        <v>0.81370029642105202</v>
       </c>
       <c r="N175">
-        <v>0.85543159658576395</v>
+        <v>0.85519615973684204</v>
       </c>
       <c r="O175">
-        <v>0.97030851284849995</v>
+        <v>0.96995033100000005</v>
       </c>
       <c r="P175">
-        <v>0.94654617931310103</v>
+        <v>0.94616155800000001</v>
       </c>
       <c r="Q175">
-        <v>0.95494130178748304</v>
+        <v>0.95454534315789497</v>
       </c>
       <c r="R175">
-        <v>0.99411242231853103</v>
+        <v>0.99109879947368396</v>
       </c>
       <c r="S175">
-        <v>1.0051487536491099</v>
+        <v>0.99527194799999996</v>
       </c>
       <c r="T175">
-        <v>0.987506810016196</v>
+        <v>0.96024499568420996</v>
       </c>
       <c r="U175">
-        <v>0.987506810016196</v>
+        <v>0.96024499568420996</v>
       </c>
       <c r="V175">
-        <v>0.987506810016196</v>
+        <v>0.96024499568420996</v>
       </c>
       <c r="W175">
-        <v>0.987506810016196</v>
+        <v>0.96024499568420996</v>
       </c>
       <c r="X175">
-        <v>0.987506810016196</v>
+        <v>0.96024499568420996</v>
       </c>
       <c r="Y175">
-        <v>0.987506810016196</v>
+        <v>0.96024499568420996</v>
       </c>
     </row>
     <row r="176" spans="1:25" x14ac:dyDescent="0.2">
@@ -17530,64 +17530,64 @@
         <v>2002</v>
       </c>
       <c r="F176">
-        <v>8.6415740522127506E-3</v>
+        <v>2.17160216842105E-3</v>
       </c>
       <c r="G176">
-        <v>0.120052049922018</v>
+        <v>4.5099632000000098E-2</v>
       </c>
       <c r="H176">
-        <v>0.379590650823247</v>
+        <v>0.24697231</v>
       </c>
       <c r="I176">
-        <v>0.57154713413910996</v>
+        <v>0.50438701789473595</v>
       </c>
       <c r="J176">
-        <v>0.73396523592859697</v>
+        <v>0.70986207031578996</v>
       </c>
       <c r="K176">
-        <v>0.70737945594555596</v>
+        <v>0.69930215242105198</v>
       </c>
       <c r="L176">
-        <v>0.77353159286025996</v>
+        <v>0.77117013831578995</v>
       </c>
       <c r="M176">
-        <v>0.93943923700835996</v>
+        <v>0.894388101052631</v>
       </c>
       <c r="N176">
-        <v>0.93728493320982897</v>
+        <v>0.937026968210526</v>
       </c>
       <c r="O176">
-        <v>0.90639436375274496</v>
+        <v>0.90605977531578996</v>
       </c>
       <c r="P176">
-        <v>1.04976088971548</v>
+        <v>1.0493343279473699</v>
       </c>
       <c r="Q176">
-        <v>1.0276102822828499</v>
+        <v>1.0271841920526299</v>
       </c>
       <c r="R176">
-        <v>0.99108360644619498</v>
+        <v>0.988079165368421</v>
       </c>
       <c r="S176">
-        <v>1.0388603358328301</v>
+        <v>1.0286522730000001</v>
       </c>
       <c r="T176">
-        <v>1.1152788522319399</v>
+        <v>1.0844896721578901</v>
       </c>
       <c r="U176">
-        <v>1.1152788522319399</v>
+        <v>1.0844896721578901</v>
       </c>
       <c r="V176">
-        <v>1.1152788522319399</v>
+        <v>1.0844896721578901</v>
       </c>
       <c r="W176">
-        <v>1.1152788522319399</v>
+        <v>1.0844896721578901</v>
       </c>
       <c r="X176">
-        <v>1.1152788522319399</v>
+        <v>1.0844896721578901</v>
       </c>
       <c r="Y176">
-        <v>1.1152788522319399</v>
+        <v>1.0844896721578901</v>
       </c>
     </row>
     <row r="177" spans="1:25" x14ac:dyDescent="0.2">
@@ -17607,64 +17607,64 @@
         <v>2003</v>
       </c>
       <c r="F177">
-        <v>7.7552959451846802E-3</v>
+        <v>1.94888308421053E-3</v>
       </c>
       <c r="G177">
-        <v>0.11178216090792099</v>
+        <v>4.1992904947368501E-2</v>
       </c>
       <c r="H177">
-        <v>0.35514502346812699</v>
+        <v>0.231067300105263</v>
       </c>
       <c r="I177">
-        <v>0.49699529111806501</v>
+        <v>0.43859545052631499</v>
       </c>
       <c r="J177">
-        <v>0.60330527604837403</v>
+        <v>0.58349293852631601</v>
       </c>
       <c r="K177">
-        <v>0.706116609017715</v>
+        <v>0.69805372547368305</v>
       </c>
       <c r="L177">
-        <v>0.67067117828647504</v>
+        <v>0.66862373831579003</v>
       </c>
       <c r="M177">
-        <v>0.75779483405547698</v>
+        <v>0.72145451873684197</v>
       </c>
       <c r="N177">
-        <v>0.90118910128441498</v>
+        <v>0.90094107078947405</v>
       </c>
       <c r="O177">
-        <v>0.86873288625831502</v>
+        <v>0.86841220026315802</v>
       </c>
       <c r="P177">
-        <v>0.85778903346616697</v>
+        <v>0.85744047789473699</v>
       </c>
       <c r="Q177">
-        <v>0.99691881152511097</v>
+        <v>0.99650544726315804</v>
       </c>
       <c r="R177">
-        <v>0.93292088289695496</v>
+        <v>0.93009276042105204</v>
       </c>
       <c r="S177">
-        <v>0.90597176342846197</v>
+        <v>0.89706949199999997</v>
       </c>
       <c r="T177">
-        <v>1.0083075469323399</v>
+        <v>0.98047149268420997</v>
       </c>
       <c r="U177">
-        <v>1.0083075469323399</v>
+        <v>0.98047149268420997</v>
       </c>
       <c r="V177">
-        <v>1.0083075469323399</v>
+        <v>0.98047149268420997</v>
       </c>
       <c r="W177">
-        <v>1.0083075469323399</v>
+        <v>0.98047149268420997</v>
       </c>
       <c r="X177">
-        <v>1.0083075469323399</v>
+        <v>0.98047149268420997</v>
       </c>
       <c r="Y177">
-        <v>1.0083075469323399</v>
+        <v>0.98047149268420997</v>
       </c>
     </row>
     <row r="178" spans="1:25" x14ac:dyDescent="0.2">
@@ -17684,64 +17684,64 @@
         <v>2004</v>
       </c>
       <c r="F178">
-        <v>7.4181372917991404E-3</v>
+        <v>1.86415610526316E-3</v>
       </c>
       <c r="G178">
-        <v>0.10338464301238399</v>
+        <v>3.8838231894736903E-2</v>
       </c>
       <c r="H178">
-        <v>0.340789829870567</v>
+        <v>0.221727409052631</v>
       </c>
       <c r="I178">
-        <v>0.47920403909538101</v>
+        <v>0.42289477421052601</v>
       </c>
       <c r="J178">
-        <v>0.54064888881420003</v>
+        <v>0.52289416547368395</v>
       </c>
       <c r="K178">
-        <v>0.59815819617141297</v>
+        <v>0.59132804968421004</v>
       </c>
       <c r="L178">
-        <v>0.68994047581835605</v>
+        <v>0.68783421010526402</v>
       </c>
       <c r="M178">
-        <v>0.67711311980916</v>
+        <v>0.64464192421052602</v>
       </c>
       <c r="N178">
-        <v>0.74916389339276801</v>
+        <v>0.74895770415789498</v>
       </c>
       <c r="O178">
-        <v>0.86081243179988098</v>
+        <v>0.86049466957894805</v>
       </c>
       <c r="P178">
-        <v>0.84728119479696495</v>
+        <v>0.84693690899999996</v>
       </c>
       <c r="Q178">
-        <v>0.83951379881918398</v>
+        <v>0.83916570126315804</v>
       </c>
       <c r="R178">
-        <v>0.93272610759921004</v>
+        <v>0.92989857557894695</v>
       </c>
       <c r="S178">
-        <v>0.87887522002412799</v>
+        <v>0.87023920499999996</v>
       </c>
       <c r="T178">
-        <v>0.90620939775746001</v>
+        <v>0.88119193752631597</v>
       </c>
       <c r="U178">
-        <v>0.90620939775746001</v>
+        <v>0.88119193752631597</v>
       </c>
       <c r="V178">
-        <v>0.90620939775746001</v>
+        <v>0.88119193752631597</v>
       </c>
       <c r="W178">
-        <v>0.90620939775746001</v>
+        <v>0.88119193752631597</v>
       </c>
       <c r="X178">
-        <v>0.90620939775746001</v>
+        <v>0.88119193752631597</v>
       </c>
       <c r="Y178">
-        <v>0.90620939775746001</v>
+        <v>0.88119193752631597</v>
       </c>
     </row>
     <row r="179" spans="1:25" x14ac:dyDescent="0.2">
@@ -17761,64 +17761,64 @@
         <v>2005</v>
       </c>
       <c r="F179">
-        <v>6.8494478981567398E-3</v>
+        <v>1.7212461315789501E-3</v>
       </c>
       <c r="G179">
-        <v>0.10542174972314899</v>
+        <v>3.9603506315789502E-2</v>
       </c>
       <c r="H179">
-        <v>0.33600655125087697</v>
+        <v>0.218615274</v>
       </c>
       <c r="I179">
-        <v>0.490206306112414</v>
+        <v>0.43260421078947298</v>
       </c>
       <c r="J179">
-        <v>0.55572651279383101</v>
+        <v>0.53747664547368401</v>
       </c>
       <c r="K179">
-        <v>0.57144157360346104</v>
+        <v>0.56491649431578905</v>
       </c>
       <c r="L179">
-        <v>0.62305843282187401</v>
+        <v>0.62115634610526405</v>
       </c>
       <c r="M179">
-        <v>0.74257578228256604</v>
+        <v>0.70696530189473605</v>
       </c>
       <c r="N179">
-        <v>0.71361512403308802</v>
+        <v>0.71341871873684204</v>
       </c>
       <c r="O179">
-        <v>0.76286393482062098</v>
+        <v>0.76258232952631599</v>
       </c>
       <c r="P179">
-        <v>0.89500896569231903</v>
+        <v>0.89464528610526295</v>
       </c>
       <c r="Q179">
-        <v>0.884000528194816</v>
+        <v>0.88363398457894804</v>
       </c>
       <c r="R179">
-        <v>0.83733610537612602</v>
+        <v>0.834797745368421</v>
       </c>
       <c r="S179">
-        <v>0.93672936416154595</v>
+        <v>0.92752486199999995</v>
       </c>
       <c r="T179">
-        <v>0.937170624205791</v>
+        <v>0.91129842636842096</v>
       </c>
       <c r="U179">
-        <v>0.937170624205791</v>
+        <v>0.91129842636842096</v>
       </c>
       <c r="V179">
-        <v>0.937170624205791</v>
+        <v>0.91129842636842096</v>
       </c>
       <c r="W179">
-        <v>0.937170624205791</v>
+        <v>0.91129842636842096</v>
       </c>
       <c r="X179">
-        <v>0.937170624205791</v>
+        <v>0.91129842636842096</v>
       </c>
       <c r="Y179">
-        <v>0.937170624205791</v>
+        <v>0.91129842636842096</v>
       </c>
     </row>
     <row r="180" spans="1:25" x14ac:dyDescent="0.2">
@@ -17838,64 +17838,64 @@
         <v>2006</v>
       </c>
       <c r="F180">
-        <v>6.1294724664931804E-3</v>
+        <v>1.54031842105263E-3</v>
       </c>
       <c r="G180">
-        <v>0.100731085500663</v>
+        <v>3.7841377052631603E-2</v>
       </c>
       <c r="H180">
-        <v>0.35456386642223903</v>
+        <v>0.230689183052631</v>
       </c>
       <c r="I180">
-        <v>0.50016428951342295</v>
+        <v>0.44139207315789403</v>
       </c>
       <c r="J180">
-        <v>0.58829099844726396</v>
+        <v>0.56897172463157897</v>
       </c>
       <c r="K180">
-        <v>0.60784138469758597</v>
+        <v>0.60090066947368403</v>
       </c>
       <c r="L180">
-        <v>0.61596677757393803</v>
+        <v>0.61408634042105303</v>
       </c>
       <c r="M180">
-        <v>0.69395397786760804</v>
+        <v>0.66067517305263102</v>
       </c>
       <c r="N180">
-        <v>0.80987174223295699</v>
+        <v>0.80964884463157905</v>
       </c>
       <c r="O180">
-        <v>0.75198104622369499</v>
+        <v>0.75170345826315799</v>
       </c>
       <c r="P180">
-        <v>0.82080237323871397</v>
+        <v>0.82046884689473698</v>
       </c>
       <c r="Q180">
-        <v>0.96632902940542198</v>
+        <v>0.96592834894736901</v>
       </c>
       <c r="R180">
-        <v>0.91242498227663504</v>
+        <v>0.90965899252631499</v>
       </c>
       <c r="S180">
-        <v>0.87022673820047103</v>
+        <v>0.86167570500000001</v>
       </c>
       <c r="T180">
-        <v>1.0336612348473</v>
+        <v>1.0051252486842099</v>
       </c>
       <c r="U180">
-        <v>1.0336612348473</v>
+        <v>1.0051252486842099</v>
       </c>
       <c r="V180">
-        <v>1.0336612348473</v>
+        <v>1.0051252486842099</v>
       </c>
       <c r="W180">
-        <v>1.0336612348473</v>
+        <v>1.0051252486842099</v>
       </c>
       <c r="X180">
-        <v>1.0336612348473</v>
+        <v>1.0051252486842099</v>
       </c>
       <c r="Y180">
-        <v>1.0336612348473</v>
+        <v>1.0051252486842099</v>
       </c>
     </row>
     <row r="181" spans="1:25" x14ac:dyDescent="0.2">
@@ -17915,64 +17915,64 @@
         <v>2007</v>
       </c>
       <c r="F181">
-        <v>5.06463481262055E-3</v>
+        <v>1.27272784736842E-3</v>
       </c>
       <c r="G181">
-        <v>8.3520237236488895E-2</v>
+        <v>3.1375823789473699E-2</v>
       </c>
       <c r="H181">
-        <v>0.31389800094227699</v>
+        <v>0.20423083189473701</v>
       </c>
       <c r="I181">
-        <v>0.48901267605102999</v>
+        <v>0.431550839210526</v>
       </c>
       <c r="J181">
-        <v>0.55614315605723896</v>
+        <v>0.53787960631579002</v>
       </c>
       <c r="K181">
-        <v>0.59618643675065697</v>
+        <v>0.58937880505263096</v>
       </c>
       <c r="L181">
-        <v>0.60706662488351504</v>
+        <v>0.60521335831579004</v>
       </c>
       <c r="M181">
-        <v>0.63565251069433004</v>
+        <v>0.60516957305263097</v>
       </c>
       <c r="N181">
-        <v>0.70124013290567899</v>
+        <v>0.70104713352631598</v>
       </c>
       <c r="O181">
-        <v>0.79071465511868</v>
+        <v>0.79042276894736896</v>
       </c>
       <c r="P181">
-        <v>0.74965091405567896</v>
+        <v>0.74934629952631604</v>
       </c>
       <c r="Q181">
-        <v>0.8211015560696</v>
+        <v>0.820761093</v>
       </c>
       <c r="R181">
-        <v>0.92412409854358701</v>
+        <v>0.92132264326315705</v>
       </c>
       <c r="S181">
-        <v>0.87859846860577095</v>
+        <v>0.86996517299999998</v>
       </c>
       <c r="T181">
-        <v>0.88972788109258705</v>
+        <v>0.865165421315789</v>
       </c>
       <c r="U181">
-        <v>0.88972788109258705</v>
+        <v>0.865165421315789</v>
       </c>
       <c r="V181">
-        <v>0.88972788109258705</v>
+        <v>0.865165421315789</v>
       </c>
       <c r="W181">
-        <v>0.88972788109258705</v>
+        <v>0.865165421315789</v>
       </c>
       <c r="X181">
-        <v>0.88972788109258705</v>
+        <v>0.865165421315789</v>
       </c>
       <c r="Y181">
-        <v>0.88972788109258705</v>
+        <v>0.865165421315789</v>
       </c>
     </row>
     <row r="182" spans="1:25" x14ac:dyDescent="0.2">
@@ -17992,64 +17992,64 @@
         <v>2008</v>
       </c>
       <c r="F182">
-        <v>5.5347280632051998E-3</v>
+        <v>1.3908608999999999E-3</v>
       </c>
       <c r="G182">
-        <v>8.3277533134076501E-2</v>
+        <v>3.12846477894737E-2</v>
       </c>
       <c r="H182">
-        <v>0.31407102437947498</v>
+        <v>0.20434340578947399</v>
       </c>
       <c r="I182">
-        <v>0.52242661263470103</v>
+        <v>0.46103844368420999</v>
       </c>
       <c r="J182">
-        <v>0.65615325233935795</v>
+        <v>0.63460540547368505</v>
       </c>
       <c r="K182">
-        <v>0.68012335027284498</v>
+        <v>0.67235727410526203</v>
       </c>
       <c r="L182">
-        <v>0.71852084830280405</v>
+        <v>0.71632733178947405</v>
       </c>
       <c r="M182">
-        <v>0.75597952247172795</v>
+        <v>0.71972626105263104</v>
       </c>
       <c r="N182">
-        <v>0.77511667347805902</v>
+        <v>0.77490334136842098</v>
       </c>
       <c r="O182">
-        <v>0.82619297592830798</v>
+        <v>0.82588799321052697</v>
       </c>
       <c r="P182">
-        <v>0.951224817702776</v>
+        <v>0.950838295263158</v>
       </c>
       <c r="Q182">
-        <v>0.90495828652695798</v>
+        <v>0.90458305294736896</v>
       </c>
       <c r="R182">
-        <v>0.94757442447078</v>
+        <v>0.94470188021052603</v>
       </c>
       <c r="S182">
-        <v>1.0738281974860799</v>
+        <v>1.063276533</v>
       </c>
       <c r="T182">
-        <v>1.0839928220202399</v>
+        <v>1.0540673463157899</v>
       </c>
       <c r="U182">
-        <v>1.0839928220202399</v>
+        <v>1.0540673463157899</v>
       </c>
       <c r="V182">
-        <v>1.0839928220202399</v>
+        <v>1.0540673463157899</v>
       </c>
       <c r="W182">
-        <v>1.0839928220202399</v>
+        <v>1.0540673463157899</v>
       </c>
       <c r="X182">
-        <v>1.0839928220202399</v>
+        <v>1.0540673463157899</v>
       </c>
       <c r="Y182">
-        <v>1.0839928220202399</v>
+        <v>1.0540673463157899</v>
       </c>
     </row>
     <row r="183" spans="1:25" x14ac:dyDescent="0.2">
@@ -18069,64 +18069,64 @@
         <v>2009</v>
       </c>
       <c r="F183">
-        <v>5.3163112216436399E-3</v>
+        <v>7.6919680000000004E-4</v>
       </c>
       <c r="G183">
-        <v>7.8766033872854205E-2</v>
+        <v>2.1458270000000002E-2</v>
       </c>
       <c r="H183">
-        <v>0.27103601421230999</v>
+        <v>0.15135859199999999</v>
       </c>
       <c r="I183">
-        <v>0.45240519878989799</v>
+        <v>0.38522757600000002</v>
       </c>
       <c r="J183">
-        <v>0.60669910027796303</v>
+        <v>0.58322105499999999</v>
       </c>
       <c r="K183">
-        <v>0.69449504862668698</v>
+        <v>0.68289732000000003</v>
       </c>
       <c r="L183">
-        <v>0.70942712066244595</v>
+        <v>0.70314938100000002</v>
       </c>
       <c r="M183">
-        <v>0.77441879826210602</v>
+        <v>0.77479779999999998</v>
       </c>
       <c r="N183">
-        <v>0.79784806284823695</v>
+        <v>0.79804850000000005</v>
       </c>
       <c r="O183">
-        <v>0.79039590524411396</v>
+        <v>0.79052020000000001</v>
       </c>
       <c r="P183">
-        <v>0.86021644208700299</v>
+        <v>0.86031970000000002</v>
       </c>
       <c r="Q183">
-        <v>0.99383775577992595</v>
+        <v>0.99394879999999997</v>
       </c>
       <c r="R183">
-        <v>0.90387396675378995</v>
+        <v>0.89494871399999998</v>
       </c>
       <c r="S183">
-        <v>0.95297321267535096</v>
+        <v>0.94360909500000001</v>
       </c>
       <c r="T183">
-        <v>1.1466572550744101</v>
+        <v>1.1011171200000001</v>
       </c>
       <c r="U183">
-        <v>1.1466572550744101</v>
+        <v>1.1011171200000001</v>
       </c>
       <c r="V183">
-        <v>1.1466572550744101</v>
+        <v>1.1011171200000001</v>
       </c>
       <c r="W183">
-        <v>1.1466572550744101</v>
+        <v>1.1011171200000001</v>
       </c>
       <c r="X183">
-        <v>1.1466572550744101</v>
+        <v>1.1011171200000001</v>
       </c>
       <c r="Y183">
-        <v>1.1466572550744101</v>
+        <v>1.1011171200000001</v>
       </c>
     </row>
     <row r="184" spans="1:25" x14ac:dyDescent="0.2">
@@ -18146,64 +18146,64 @@
         <v>2010</v>
       </c>
       <c r="F184">
-        <v>6.0046837747448302E-3</v>
+        <v>2.6063843999999999E-3</v>
       </c>
       <c r="G184">
-        <v>8.1855776025979099E-2</v>
+        <v>4.9060022000000002E-2</v>
       </c>
       <c r="H184">
-        <v>0.27735389095872998</v>
+        <v>0.23233016400000001</v>
       </c>
       <c r="I184">
-        <v>0.42239902466390999</v>
+        <v>0.40408158700000002</v>
       </c>
       <c r="J184">
-        <v>0.56842316283008398</v>
+        <v>0.56368188799999996</v>
       </c>
       <c r="K184">
-        <v>0.69475786350702196</v>
+        <v>0.690126723</v>
       </c>
       <c r="L184">
-        <v>0.78376439621221305</v>
+        <v>0.78467560000000003</v>
       </c>
       <c r="M184">
-        <v>0.82725733899989295</v>
+        <v>0.82766220000000001</v>
       </c>
       <c r="N184">
-        <v>0.88426475305653995</v>
+        <v>0.88448689999999996</v>
       </c>
       <c r="O184">
-        <v>0.88022567894396597</v>
+        <v>0.88036409999999998</v>
       </c>
       <c r="P184">
-        <v>0.89036302337790196</v>
+        <v>0.89046990000000004</v>
       </c>
       <c r="Q184">
-        <v>0.97238065324088196</v>
+        <v>0.9724893</v>
       </c>
       <c r="R184">
-        <v>1.0739672947746599</v>
+        <v>1.0741035000000001</v>
       </c>
       <c r="S184">
-        <v>0.98349345507491603</v>
+        <v>0.97382943899999996</v>
       </c>
       <c r="T184">
-        <v>1.1009706916199</v>
+        <v>1.0792709620000001</v>
       </c>
       <c r="U184">
-        <v>1.1009706916199</v>
+        <v>1.0792709620000001</v>
       </c>
       <c r="V184">
-        <v>1.1009706916199</v>
+        <v>1.0792709620000001</v>
       </c>
       <c r="W184">
-        <v>1.1009706916199</v>
+        <v>1.0792709620000001</v>
       </c>
       <c r="X184">
-        <v>1.1009706916199</v>
+        <v>1.0792709620000001</v>
       </c>
       <c r="Y184">
-        <v>1.1009706916199</v>
+        <v>1.0792709620000001</v>
       </c>
     </row>
     <row r="185" spans="1:25" x14ac:dyDescent="0.2">
@@ -18223,64 +18223,64 @@
         <v>2011</v>
       </c>
       <c r="F185">
-        <v>5.6862836501085801E-3</v>
+        <v>8.2272669999999999E-4</v>
       </c>
       <c r="G185">
-        <v>8.5250146331844606E-2</v>
+        <v>1.8579792000000001E-2</v>
       </c>
       <c r="H185">
-        <v>0.26577290283645799</v>
+        <v>0.131553591</v>
       </c>
       <c r="I185">
-        <v>0.398562285608143</v>
+        <v>0.32681017200000001</v>
       </c>
       <c r="J185">
-        <v>0.48936530124706401</v>
+        <v>0.46547596800000002</v>
       </c>
       <c r="K185">
-        <v>0.60020281022907596</v>
+        <v>0.59017971599999997</v>
       </c>
       <c r="L185">
-        <v>0.72296268422832</v>
+        <v>0.71656516800000003</v>
       </c>
       <c r="M185">
-        <v>0.84272207053675396</v>
+        <v>0.84313450000000001</v>
       </c>
       <c r="N185">
-        <v>0.87098978802256299</v>
+        <v>0.8712086</v>
       </c>
       <c r="O185">
-        <v>0.89954354108794499</v>
+        <v>0.89968499999999996</v>
       </c>
       <c r="P185">
-        <v>0.91428705160621204</v>
+        <v>0.91439680000000001</v>
       </c>
       <c r="Q185">
-        <v>0.928029508715983</v>
+        <v>0.92813319999999999</v>
       </c>
       <c r="R185">
-        <v>0.96889772015724196</v>
+        <v>0.95933039399999998</v>
       </c>
       <c r="S185">
-        <v>1.0775085514274501</v>
+        <v>1.066920723</v>
       </c>
       <c r="T185">
-        <v>1.0476895783668001</v>
+        <v>1.0060800000000001</v>
       </c>
       <c r="U185">
-        <v>1.0476895783668001</v>
+        <v>1.0060800000000001</v>
       </c>
       <c r="V185">
-        <v>1.0476895783668001</v>
+        <v>1.0060800000000001</v>
       </c>
       <c r="W185">
-        <v>1.0476895783668001</v>
+        <v>1.0060800000000001</v>
       </c>
       <c r="X185">
-        <v>1.0476895783668001</v>
+        <v>1.0060800000000001</v>
       </c>
       <c r="Y185">
-        <v>1.0476895783668001</v>
+        <v>1.0060800000000001</v>
       </c>
     </row>
     <row r="186" spans="1:25" x14ac:dyDescent="0.2">
@@ -18300,64 +18300,64 @@
         <v>2012</v>
       </c>
       <c r="F186">
-        <v>6.4090693016569901E-3</v>
+        <v>9.2730380000000004E-4</v>
       </c>
       <c r="G186">
-        <v>8.3586529373354701E-2</v>
+        <v>1.3662911999999999E-2</v>
       </c>
       <c r="H186">
-        <v>0.28658889873375198</v>
+        <v>0.112758284</v>
       </c>
       <c r="I186">
-        <v>0.39543533251778501</v>
+        <v>0.29930414399999999</v>
       </c>
       <c r="J186">
-        <v>0.478089744694636</v>
+        <v>0.44507530000000001</v>
       </c>
       <c r="K186">
-        <v>0.53501046790469997</v>
+        <v>0.52070793100000001</v>
       </c>
       <c r="L186">
-        <v>0.64667088101067605</v>
+        <v>0.64094847300000002</v>
       </c>
       <c r="M186">
-        <v>0.80485500273733801</v>
+        <v>7.2472401000000006E-2</v>
       </c>
       <c r="N186">
-        <v>0.91867050956643204</v>
+        <v>0.91890130000000003</v>
       </c>
       <c r="O186">
-        <v>0.91739393400074398</v>
+        <v>0.91753819999999997</v>
       </c>
       <c r="P186">
-        <v>0.96741677406680304</v>
+        <v>0.96753290000000003</v>
       </c>
       <c r="Q186">
-        <v>0.98668855457979698</v>
+        <v>0.98679879999999998</v>
       </c>
       <c r="R186">
-        <v>0.95742837474974596</v>
+        <v>0.94797430199999999</v>
       </c>
       <c r="S186">
-        <v>1.00649231779647</v>
+        <v>0.98653561999999995</v>
       </c>
       <c r="T186">
-        <v>1.18846046913276</v>
+        <v>1.12937197</v>
       </c>
       <c r="U186">
-        <v>1.18846046913276</v>
+        <v>1.12937197</v>
       </c>
       <c r="V186">
-        <v>1.18846046913276</v>
+        <v>1.12937197</v>
       </c>
       <c r="W186">
-        <v>1.18846046913276</v>
+        <v>1.12937197</v>
       </c>
       <c r="X186">
-        <v>1.18846046913276</v>
+        <v>1.12937197</v>
       </c>
       <c r="Y186">
-        <v>1.18846046913276</v>
+        <v>1.12937197</v>
       </c>
     </row>
     <row r="187" spans="1:25" x14ac:dyDescent="0.2">
@@ -18377,64 +18377,64 @@
         <v>2013</v>
       </c>
       <c r="F187">
-        <v>7.2376611832869198E-3</v>
+        <v>1.0471896E-3</v>
       </c>
       <c r="G187">
-        <v>9.9561099027539596E-2</v>
+        <v>2.1698783999999999E-2</v>
       </c>
       <c r="H187">
-        <v>0.29695289231551503</v>
+        <v>0.146987217</v>
       </c>
       <c r="I187">
-        <v>0.45062074658066098</v>
+        <v>0.36949668600000002</v>
       </c>
       <c r="J187">
-        <v>0.50127451923330901</v>
+        <v>0.47680381399999999</v>
       </c>
       <c r="K187">
-        <v>0.552364123490095</v>
+        <v>0.543139912</v>
       </c>
       <c r="L187">
-        <v>0.609164485912155</v>
+        <v>0.60377397300000002</v>
       </c>
       <c r="M187">
-        <v>0.76080266201989599</v>
+        <v>0.76117500000000005</v>
       </c>
       <c r="N187">
-        <v>0.92721396326113303</v>
+        <v>0.92744689999999996</v>
       </c>
       <c r="O187">
-        <v>1.02256159572068</v>
+        <v>1.0227223999999999</v>
       </c>
       <c r="P187">
-        <v>1.04263964452931</v>
+        <v>1.0427648</v>
       </c>
       <c r="Q187">
-        <v>1.10331142398652</v>
+        <v>1.1034347</v>
       </c>
       <c r="R187">
-        <v>1.0757505686120801</v>
+        <v>1.075887</v>
       </c>
       <c r="S187">
-        <v>1.0510557950111199</v>
+        <v>1.040727897</v>
       </c>
       <c r="T187">
-        <v>1.1731712991855601</v>
+        <v>1.1383133329999999</v>
       </c>
       <c r="U187">
-        <v>1.1731712991855601</v>
+        <v>1.1383133329999999</v>
       </c>
       <c r="V187">
-        <v>1.1731712991855601</v>
+        <v>1.1383133329999999</v>
       </c>
       <c r="W187">
-        <v>1.1731712991855601</v>
+        <v>1.1383133329999999</v>
       </c>
       <c r="X187">
-        <v>1.1731712991855601</v>
+        <v>1.1383133329999999</v>
       </c>
       <c r="Y187">
-        <v>1.1731712991855601</v>
+        <v>1.1383133329999999</v>
       </c>
     </row>
     <row r="188" spans="1:25" x14ac:dyDescent="0.2">
@@ -18454,64 +18454,64 @@
         <v>2014</v>
       </c>
       <c r="F188">
-        <v>7.5506053620867297E-3</v>
+        <v>2.1849365999999999E-3</v>
       </c>
       <c r="G188">
-        <v>0.114007205459635</v>
+        <v>5.5906272E-2</v>
       </c>
       <c r="H188">
-        <v>0.358657730162383</v>
+        <v>0.27767541600000001</v>
       </c>
       <c r="I188">
-        <v>0.47345496195003001</v>
+        <v>0.44794629000000002</v>
       </c>
       <c r="J188">
-        <v>0.57922940276535795</v>
+        <v>0.56853678799999996</v>
       </c>
       <c r="K188">
-        <v>0.58726079691823496</v>
+        <v>0.58334621399999997</v>
       </c>
       <c r="L188">
-        <v>0.63773017546696398</v>
+        <v>0.63847160000000003</v>
       </c>
       <c r="M188">
-        <v>0.72671234587247602</v>
+        <v>0.72706800000000005</v>
       </c>
       <c r="N188">
-        <v>0.88873772934556206</v>
+        <v>0.888961</v>
       </c>
       <c r="O188">
-        <v>1.04652342757105</v>
+        <v>1.0466880000000001</v>
       </c>
       <c r="P188">
-        <v>1.1784390435591801</v>
+        <v>1.1785805</v>
       </c>
       <c r="Q188">
-        <v>1.2057519780222701</v>
+        <v>1.2058867</v>
       </c>
       <c r="R188">
-        <v>1.2197445066716299</v>
+        <v>1.2198992</v>
       </c>
       <c r="S188">
-        <v>1.19748569033746</v>
+        <v>1.1976959</v>
       </c>
       <c r="T188">
-        <v>1.2422701257828901</v>
+        <v>1.2302118179999999</v>
       </c>
       <c r="U188">
-        <v>1.2422701257828901</v>
+        <v>1.2302118179999999</v>
       </c>
       <c r="V188">
-        <v>1.2422701257828901</v>
+        <v>1.2302118179999999</v>
       </c>
       <c r="W188">
-        <v>1.2422701257828901</v>
+        <v>1.2302118179999999</v>
       </c>
       <c r="X188">
-        <v>1.2422701257828901</v>
+        <v>1.2302118179999999</v>
       </c>
       <c r="Y188">
-        <v>1.2422701257828901</v>
+        <v>1.2302118179999999</v>
       </c>
     </row>
     <row r="189" spans="1:25" x14ac:dyDescent="0.2">
@@ -18531,64 +18531,64 @@
         <v>2015</v>
       </c>
       <c r="F189">
-        <v>6.1203741549919104E-3</v>
+        <v>2.6566008000000001E-3</v>
       </c>
       <c r="G189">
-        <v>8.8762454974227203E-2</v>
+        <v>4.8363200000000002E-2</v>
       </c>
       <c r="H189">
-        <v>0.30650408545186397</v>
+        <v>0.24896806399999999</v>
       </c>
       <c r="I189">
-        <v>0.42676108236990501</v>
+        <v>0.408254483</v>
       </c>
       <c r="J189">
-        <v>0.454183750389277</v>
+        <v>0.45039535800000002</v>
       </c>
       <c r="K189">
-        <v>0.50642992273833698</v>
+        <v>0.50305414500000001</v>
       </c>
       <c r="L189">
-        <v>0.50600641739058405</v>
+        <v>0.50659469999999995</v>
       </c>
       <c r="M189">
-        <v>0.56777782866696302</v>
+        <v>0.56805570000000005</v>
       </c>
       <c r="N189">
-        <v>0.63354523936628404</v>
+        <v>0.63370439999999995</v>
       </c>
       <c r="O189">
-        <v>0.74861087620424904</v>
+        <v>0.74872859999999997</v>
       </c>
       <c r="P189">
-        <v>0.90007795722512296</v>
+        <v>0.90018600000000004</v>
       </c>
       <c r="Q189">
-        <v>1.0170548616689601</v>
+        <v>1.0171684999999999</v>
       </c>
       <c r="R189">
-        <v>0.99481473324838998</v>
+        <v>0.99494090000000002</v>
       </c>
       <c r="S189">
-        <v>1.01330712150861</v>
+        <v>1.0033501499999999</v>
       </c>
       <c r="T189">
-        <v>1.05626793667119</v>
+        <v>1.0354492820000001</v>
       </c>
       <c r="U189">
-        <v>1.05626793667119</v>
+        <v>1.0354492820000001</v>
       </c>
       <c r="V189">
-        <v>1.05626793667119</v>
+        <v>1.0354492820000001</v>
       </c>
       <c r="W189">
-        <v>1.05626793667119</v>
+        <v>1.0354492820000001</v>
       </c>
       <c r="X189">
-        <v>1.05626793667119</v>
+        <v>1.0354492820000001</v>
       </c>
       <c r="Y189">
-        <v>1.05626793667119</v>
+        <v>1.0354492820000001</v>
       </c>
     </row>
     <row r="190" spans="1:25" x14ac:dyDescent="0.2">
@@ -18608,64 +18608,64 @@
         <v>2016</v>
       </c>
       <c r="F190">
-        <v>6.9830895428084402E-3</v>
+        <v>0</v>
       </c>
       <c r="G190">
-        <v>8.8868500369246803E-2</v>
+        <v>9.6841960000000008E-3</v>
       </c>
       <c r="H190">
-        <v>0.29475117695620101</v>
+        <v>8.6042057000000005E-2</v>
       </c>
       <c r="I190">
-        <v>0.45046711950470197</v>
+        <v>0.293602364</v>
       </c>
       <c r="J190">
-        <v>0.50566162653702396</v>
+        <v>0.44515933800000002</v>
       </c>
       <c r="K190">
-        <v>0.49048153443117998</v>
+        <v>0.472448064</v>
       </c>
       <c r="L190">
-        <v>0.53897259094661898</v>
+        <v>0.52880721600000002</v>
       </c>
       <c r="M190">
-        <v>0.556441776548114</v>
+        <v>0.55114695899999999</v>
       </c>
       <c r="N190">
-        <v>0.61138640615728401</v>
+        <v>0.60542459999999998</v>
       </c>
       <c r="O190">
-        <v>0.65914714494190796</v>
+        <v>0.65265829200000003</v>
       </c>
       <c r="P190">
-        <v>0.79526073918316498</v>
+        <v>0.78740263799999999</v>
       </c>
       <c r="Q190">
-        <v>0.95948819375076499</v>
+        <v>0.94999944599999997</v>
       </c>
       <c r="R190">
-        <v>1.03645605211437</v>
+        <v>1.0158557500000001</v>
       </c>
       <c r="S190">
-        <v>1.02079080780342</v>
+        <v>0.98013119999999998</v>
       </c>
       <c r="T190">
-        <v>1.10399499554402</v>
+        <v>0.98284666899999995</v>
       </c>
       <c r="U190">
-        <v>1.10399499554402</v>
+        <v>0.98284666899999995</v>
       </c>
       <c r="V190">
-        <v>1.10399499554402</v>
+        <v>0.98284666899999995</v>
       </c>
       <c r="W190">
-        <v>1.10399499554402</v>
+        <v>0.98284666899999995</v>
       </c>
       <c r="X190">
-        <v>1.10399499554402</v>
+        <v>0.98284666899999995</v>
       </c>
       <c r="Y190">
-        <v>1.10399499554402</v>
+        <v>0.98284666899999995</v>
       </c>
     </row>
     <row r="191" spans="1:25" x14ac:dyDescent="0.2">
@@ -18685,64 +18685,64 @@
         <v>2017</v>
       </c>
       <c r="F191">
-        <v>7.8105189084899497E-3</v>
+        <v>2.2601484000000002E-3</v>
       </c>
       <c r="G191">
-        <v>0.11098805011669501</v>
+        <v>5.1402100999999999E-2</v>
       </c>
       <c r="H191">
-        <v>0.32302246596575601</v>
+        <v>0.24598655999999999</v>
       </c>
       <c r="I191">
-        <v>0.47417772264547098</v>
+        <v>0.44364533099999998</v>
       </c>
       <c r="J191">
-        <v>0.58424779971960605</v>
+        <v>0.57346254500000005</v>
       </c>
       <c r="K191">
-        <v>0.59773651632359504</v>
+        <v>0.593752104</v>
       </c>
       <c r="L191">
-        <v>0.57138480853137197</v>
+        <v>0.57204909999999998</v>
       </c>
       <c r="M191">
-        <v>0.64876769210459695</v>
+        <v>0.64908520000000003</v>
       </c>
       <c r="N191">
-        <v>0.655867131611235</v>
+        <v>0.6560319</v>
       </c>
       <c r="O191">
-        <v>0.69627260672819902</v>
+        <v>0.6963821</v>
       </c>
       <c r="P191">
-        <v>0.76646889527347895</v>
+        <v>0.76656089999999999</v>
       </c>
       <c r="Q191">
-        <v>0.92795691682687398</v>
+        <v>0.92806060000000001</v>
       </c>
       <c r="R191">
-        <v>1.07029846007231</v>
+        <v>1.0704342</v>
       </c>
       <c r="S191">
-        <v>1.16413714442544</v>
+        <v>1.1526980849999999</v>
       </c>
       <c r="T191">
-        <v>1.21736700436886</v>
+        <v>1.1933731460000001</v>
       </c>
       <c r="U191">
-        <v>1.21736700436886</v>
+        <v>1.1933731460000001</v>
       </c>
       <c r="V191">
-        <v>1.21736700436886</v>
+        <v>1.1933731460000001</v>
       </c>
       <c r="W191">
-        <v>1.21736700436886</v>
+        <v>1.1933731460000001</v>
       </c>
       <c r="X191">
-        <v>1.21736700436886</v>
+        <v>1.1933731460000001</v>
       </c>
       <c r="Y191">
-        <v>1.21736700436886</v>
+        <v>1.1933731460000001</v>
       </c>
     </row>
     <row r="192" spans="1:25" x14ac:dyDescent="0.2">
@@ -18762,64 +18762,64 @@
         <v>2018</v>
       </c>
       <c r="F192">
-        <v>8.97015206618108E-3</v>
+        <v>2.5957141999999999E-3</v>
       </c>
       <c r="G192">
-        <v>0.120078845746997</v>
+        <v>6.2154965999999999E-2</v>
       </c>
       <c r="H192">
-        <v>0.39022867697084601</v>
+        <v>0.31697612800000002</v>
       </c>
       <c r="I192">
-        <v>0.50266237040615502</v>
+        <v>0.480864293</v>
       </c>
       <c r="J192">
-        <v>0.59488514892025901</v>
+        <v>0.58992315200000001</v>
       </c>
       <c r="K192">
-        <v>0.66804373254771898</v>
+        <v>0.663590664</v>
       </c>
       <c r="L192">
-        <v>0.67355632401862098</v>
+        <v>0.67433940000000003</v>
       </c>
       <c r="M192">
-        <v>0.66528720742866798</v>
+        <v>0.6656128</v>
       </c>
       <c r="N192">
-        <v>0.73967907618948603</v>
+        <v>0.73986490000000005</v>
       </c>
       <c r="O192">
-        <v>0.72249928241754502</v>
+        <v>0.7226129</v>
       </c>
       <c r="P192">
-        <v>0.78315819193820302</v>
+        <v>0.78325219999999995</v>
       </c>
       <c r="Q192">
-        <v>0.86510903899275304</v>
+        <v>0.86520569999999997</v>
       </c>
       <c r="R192">
-        <v>1.00126971459945</v>
+        <v>1.0013966999999999</v>
       </c>
       <c r="S192">
-        <v>1.16282987390701</v>
+        <v>1.1630339999999999</v>
       </c>
       <c r="T192">
-        <v>1.3429101070007099</v>
+        <v>1.32987492</v>
       </c>
       <c r="U192">
-        <v>1.3429101070007099</v>
+        <v>1.32987492</v>
       </c>
       <c r="V192">
-        <v>1.3429101070007099</v>
+        <v>1.32987492</v>
       </c>
       <c r="W192">
-        <v>1.3429101070007099</v>
+        <v>1.32987492</v>
       </c>
       <c r="X192">
-        <v>1.3429101070007099</v>
+        <v>1.32987492</v>
       </c>
       <c r="Y192">
-        <v>1.3429101070007099</v>
+        <v>1.32987492</v>
       </c>
     </row>
     <row r="193" spans="1:25" x14ac:dyDescent="0.2">
@@ -18839,64 +18839,64 @@
         <v>2019</v>
       </c>
       <c r="F193">
-        <v>6.1768626157416504E-3</v>
+        <v>8.9370669999999999E-4</v>
       </c>
       <c r="G193">
-        <v>0.11594278168835701</v>
+        <v>2.2110444999999999E-2</v>
       </c>
       <c r="H193">
-        <v>0.35494962359369597</v>
+        <v>0.16217974800000001</v>
       </c>
       <c r="I193">
-        <v>0.51052864744600801</v>
+        <v>0.40788569200000002</v>
       </c>
       <c r="J193">
-        <v>0.53018280213145297</v>
+        <v>0.49893597899999997</v>
       </c>
       <c r="K193">
-        <v>0.57187122659895595</v>
+        <v>0.56232125600000005</v>
       </c>
       <c r="L193">
-        <v>0.63288710601518805</v>
+        <v>0.62728667100000002</v>
       </c>
       <c r="M193">
-        <v>0.65934341632907401</v>
+        <v>0.65966610000000003</v>
       </c>
       <c r="N193">
-        <v>0.63770609406718104</v>
+        <v>0.6378663</v>
       </c>
       <c r="O193">
-        <v>0.68504977159001601</v>
+        <v>0.68515749999999997</v>
       </c>
       <c r="P193">
-        <v>0.683226687429214</v>
+        <v>0.68330869999999999</v>
       </c>
       <c r="Q193">
-        <v>0.74316126455228104</v>
+        <v>0.74324429999999997</v>
       </c>
       <c r="R193">
-        <v>0.78478626997588397</v>
+        <v>0.77703694199999995</v>
       </c>
       <c r="S193">
-        <v>0.91457565307994204</v>
+        <v>0.90558883800000001</v>
       </c>
       <c r="T193">
-        <v>1.1277587545415799</v>
+        <v>1.082969184</v>
       </c>
       <c r="U193">
-        <v>1.1277587545415799</v>
+        <v>1.082969184</v>
       </c>
       <c r="V193">
-        <v>1.1277587545415799</v>
+        <v>1.082969184</v>
       </c>
       <c r="W193">
-        <v>1.1277587545415799</v>
+        <v>1.082969184</v>
       </c>
       <c r="X193">
-        <v>1.1277587545415799</v>
+        <v>1.082969184</v>
       </c>
       <c r="Y193">
-        <v>1.1277587545415799</v>
+        <v>1.082969184</v>
       </c>
     </row>
     <row r="194" spans="1:25" x14ac:dyDescent="0.2">
@@ -18916,64 +18916,64 @@
         <v>2020</v>
       </c>
       <c r="F194">
-        <v>7.4287222690584704E-3</v>
+        <v>3.2245005000000001E-3</v>
       </c>
       <c r="G194">
-        <v>9.0967237477463894E-2</v>
+        <v>4.9564499999999997E-2</v>
       </c>
       <c r="H194">
-        <v>0.39049648510519802</v>
+        <v>0.32214981500000001</v>
       </c>
       <c r="I194">
-        <v>0.52910382561914404</v>
+        <v>0.50615910799999997</v>
       </c>
       <c r="J194">
-        <v>0.61353952091519304</v>
+        <v>0.608421926</v>
       </c>
       <c r="K194">
-        <v>0.58071623797548499</v>
+        <v>0.57684528000000002</v>
       </c>
       <c r="L194">
-        <v>0.61729503334496305</v>
+        <v>0.61801269999999997</v>
       </c>
       <c r="M194">
-        <v>0.70589033619568498</v>
+        <v>0.70623579999999997</v>
       </c>
       <c r="N194">
-        <v>0.72010579343279202</v>
+        <v>0.72028669999999995</v>
       </c>
       <c r="O194">
-        <v>0.67293417684392898</v>
+        <v>0.67303999999999997</v>
       </c>
       <c r="P194">
-        <v>0.73811289904588795</v>
+        <v>0.73820149999999995</v>
       </c>
       <c r="Q194">
-        <v>0.73870596235542296</v>
+        <v>0.73878849999999996</v>
       </c>
       <c r="R194">
-        <v>0.76813368192986897</v>
+        <v>0.76823109999999994</v>
       </c>
       <c r="S194">
-        <v>0.81675752432132098</v>
+        <v>0.81690090000000004</v>
       </c>
       <c r="T194">
-        <v>1.01063165831763</v>
+        <v>1.000821789</v>
       </c>
       <c r="U194">
-        <v>1.01063165831763</v>
+        <v>1.000821789</v>
       </c>
       <c r="V194">
-        <v>1.01063165831763</v>
+        <v>1.000821789</v>
       </c>
       <c r="W194">
-        <v>1.01063165831763</v>
+        <v>1.000821789</v>
       </c>
       <c r="X194">
-        <v>1.01063165831763</v>
+        <v>1.000821789</v>
       </c>
       <c r="Y194">
-        <v>1.01063165831763</v>
+        <v>1.000821789</v>
       </c>
     </row>
     <row r="195" spans="1:25" x14ac:dyDescent="0.2">
@@ -18993,64 +18993,64 @@
         <v>2021</v>
       </c>
       <c r="F195">
-        <v>8.5033666641869E-3</v>
+        <v>2.4606393999999998E-3</v>
       </c>
       <c r="G195">
-        <v>0.112447284673153</v>
+        <v>5.2077919E-2</v>
       </c>
       <c r="H195">
-        <v>0.31490257690961398</v>
+        <v>0.23980314</v>
       </c>
       <c r="I195">
-        <v>0.59828614074132502</v>
+        <v>0.56605185000000002</v>
       </c>
       <c r="J195">
-        <v>0.65355328373950194</v>
+        <v>0.64810193000000005</v>
       </c>
       <c r="K195">
-        <v>0.69071448099084398</v>
+        <v>0.68611029300000004</v>
       </c>
       <c r="L195">
-        <v>0.64428235790550703</v>
+        <v>0.64503140000000003</v>
       </c>
       <c r="M195">
-        <v>0.70765487262887095</v>
+        <v>0.7080012</v>
       </c>
       <c r="N195">
-        <v>0.79239103377512798</v>
+        <v>0.79259009999999996</v>
       </c>
       <c r="O195">
-        <v>0.78102697856709802</v>
+        <v>0.78114980000000001</v>
       </c>
       <c r="P195">
-        <v>0.74523114459212103</v>
+        <v>0.7453206</v>
       </c>
       <c r="Q195">
-        <v>0.82025195099830595</v>
+        <v>0.82034359999999995</v>
       </c>
       <c r="R195">
-        <v>0.78477127187800799</v>
+        <v>0.78487079999999998</v>
       </c>
       <c r="S195">
-        <v>0.82166786234818201</v>
+        <v>0.82181210000000005</v>
       </c>
       <c r="T195">
-        <v>0.92764994510314203</v>
+        <v>0.91864555199999998</v>
       </c>
       <c r="U195">
-        <v>0.92764994510314203</v>
+        <v>0.91864555199999998</v>
       </c>
       <c r="V195">
-        <v>0.92764994510314203</v>
+        <v>0.91864555199999998</v>
       </c>
       <c r="W195">
-        <v>0.92764994510314203</v>
+        <v>0.91864555199999998</v>
       </c>
       <c r="X195">
-        <v>0.92764994510314203</v>
+        <v>0.91864555199999998</v>
       </c>
       <c r="Y195">
-        <v>0.92764994510314203</v>
+        <v>0.91864555199999998</v>
       </c>
     </row>
     <row r="196" spans="1:25" x14ac:dyDescent="0.2">
@@ -19070,64 +19070,64 @@
         <v>2022</v>
       </c>
       <c r="F196">
-        <v>7.0606055809749203E-3</v>
+        <v>2.0431441999999998E-3</v>
       </c>
       <c r="G196">
-        <v>0.12922081039102701</v>
+        <v>5.2805535000000001E-2</v>
       </c>
       <c r="H196">
-        <v>0.39079305168881001</v>
+        <v>0.27775524000000001</v>
       </c>
       <c r="I196">
-        <v>0.48436733572447399</v>
+        <v>0.44808693599999999</v>
       </c>
       <c r="J196">
-        <v>0.74191792410132296</v>
+        <v>0.728222068</v>
       </c>
       <c r="K196">
-        <v>0.73865871227221203</v>
+        <v>0.73373493599999995</v>
       </c>
       <c r="L196">
-        <v>0.76933876743535801</v>
+        <v>0.77023319999999995</v>
       </c>
       <c r="M196">
-        <v>0.74150090832751403</v>
+        <v>0.74186379999999996</v>
       </c>
       <c r="N196">
-        <v>0.79749975035207099</v>
+        <v>0.79770010000000002</v>
       </c>
       <c r="O196">
-        <v>0.86281171739957396</v>
+        <v>0.86294740000000003</v>
       </c>
       <c r="P196">
-        <v>0.86834266663832904</v>
+        <v>0.86844690000000002</v>
       </c>
       <c r="Q196">
-        <v>0.83142340278133797</v>
+        <v>0.83151629999999999</v>
       </c>
       <c r="R196">
-        <v>0.87483364977368905</v>
+        <v>0.87494459999999996</v>
       </c>
       <c r="S196">
-        <v>0.84277055792770095</v>
+        <v>0.83448931500000001</v>
       </c>
       <c r="T196">
-        <v>0.93690170388462601</v>
+        <v>0.91843571400000001</v>
       </c>
       <c r="U196">
-        <v>0.93690170388462601</v>
+        <v>0.91843571400000001</v>
       </c>
       <c r="V196">
-        <v>0.93690170388462601</v>
+        <v>0.91843571400000001</v>
       </c>
       <c r="W196">
-        <v>0.93690170388462601</v>
+        <v>0.91843571400000001</v>
       </c>
       <c r="X196">
-        <v>0.93690170388462601</v>
+        <v>0.91843571400000001</v>
       </c>
       <c r="Y196">
-        <v>0.93690170388462601</v>
+        <v>0.91843571400000001</v>
       </c>
     </row>
     <row r="197" spans="1:25" x14ac:dyDescent="0.2">
@@ -19147,64 +19147,64 @@
         <v>2023</v>
       </c>
       <c r="F197">
-        <v>6.0506135219724703E-3</v>
+        <v>8.7544019999999997E-4</v>
       </c>
       <c r="G197">
-        <v>9.7543263286793302E-2</v>
+        <v>2.9231136000000001E-2</v>
       </c>
       <c r="H197">
-        <v>0.40826692183061403</v>
+        <v>0.23835783199999999</v>
       </c>
       <c r="I197">
-        <v>0.54646111682416498</v>
+        <v>0.47680644799999999</v>
       </c>
       <c r="J197">
-        <v>0.54605388644360298</v>
+        <v>0.53044819200000004</v>
       </c>
       <c r="K197">
-        <v>0.76231155318056698</v>
+        <v>0.75723011100000004</v>
       </c>
       <c r="L197">
-        <v>0.74795712571294903</v>
+        <v>0.74133843300000002</v>
       </c>
       <c r="M197">
-        <v>0.80494625807683595</v>
+        <v>0.80534019999999995</v>
       </c>
       <c r="N197">
-        <v>0.75968684979242995</v>
+        <v>0.75987769999999999</v>
       </c>
       <c r="O197">
-        <v>0.78944315507010498</v>
+        <v>0.78956729999999997</v>
       </c>
       <c r="P197">
-        <v>0.87207741832945396</v>
+        <v>0.87218209999999996</v>
       </c>
       <c r="Q197">
-        <v>0.88071669510649897</v>
+        <v>0.88081509999999996</v>
       </c>
       <c r="R197">
-        <v>0.80614706090703603</v>
+        <v>0.80624929999999995</v>
       </c>
       <c r="S197">
-        <v>0.85409377022241595</v>
+        <v>0.84570126300000004</v>
       </c>
       <c r="T197">
-        <v>0.87361665471381</v>
+        <v>0.85639799000000005</v>
       </c>
       <c r="U197">
-        <v>0.87361665471381</v>
+        <v>0.85639799000000005</v>
       </c>
       <c r="V197">
-        <v>0.87361665471381</v>
+        <v>0.85639799000000005</v>
       </c>
       <c r="W197">
-        <v>0.87361665471381</v>
+        <v>0.85639799000000005</v>
       </c>
       <c r="X197">
-        <v>0.87361665471381</v>
+        <v>0.85639799000000005</v>
       </c>
       <c r="Y197">
-        <v>0.87361665471381</v>
+        <v>0.85639799000000005</v>
       </c>
     </row>
     <row r="198" spans="1:25" x14ac:dyDescent="0.2">
@@ -22991,7 +22991,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23742,7 +23742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
@@ -28330,7 +28330,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScale="186" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28421,7 +28421,7 @@
         <v>45</v>
       </c>
       <c r="B11">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -31455,7 +31455,7 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31709,10 +31709,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="A31" sqref="A31:XFD59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32591,6 +32591,27 @@
       <c r="I30">
         <v>0.35149599999999998</v>
       </c>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H43" s="2"/>
+    </row>
+    <row r="45" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H45" s="2"/>
+    </row>
+    <row r="47" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H47" s="2"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H51" s="2"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H53" s="2"/>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H57" s="2"/>
+    </row>
+    <row r="59" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H59" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34527,7 +34548,7 @@
   <dimension ref="A1:DU65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y29" sqref="Y29"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35841,7 +35862,7 @@
         <v>382</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -35912,7 +35933,7 @@
         <v>382</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -39881,8 +39902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Y35" sqref="Y35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39891,8 +39912,13 @@
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="31" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="24" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Looked through selectivity & got age-1 model to converge. & plot saving.
</commit_message>
<xml_diff>
--- a/data/hake_input_yr24.xlsx
+++ b/data/hake_input_yr24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2996D723-6B8D-3C49-A0C4-184015DC8D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBAA02C-C1A3-B94B-A0A1-CE8B7C4CBC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="8840" windowWidth="34420" windowHeight="33040" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40700" yWindow="8120" windowWidth="36740" windowHeight="35080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1607,7 +1607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -2556,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4029,8 +4029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Y246"/>
   <sheetViews>
-    <sheetView topLeftCell="A230" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A247" sqref="A247:XFD295"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P182" sqref="P182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15451,64 +15451,64 @@
         <v>1975</v>
       </c>
       <c r="F149">
-        <v>1.5858565105263201E-3</v>
+        <v>6.3441649999999997E-3</v>
       </c>
       <c r="G149">
-        <v>3.9686836105263197E-2</v>
+        <v>0.11256462</v>
       </c>
       <c r="H149">
-        <v>0.21494590842105299</v>
+        <v>0.3362137</v>
       </c>
       <c r="I149">
-        <v>0.47807245605263199</v>
+        <v>0.54395230000000006</v>
       </c>
       <c r="J149">
-        <v>0.65179900673684199</v>
+        <v>0.67452129999999999</v>
       </c>
       <c r="K149">
-        <v>0.74843338357894695</v>
+        <v>0.75712710000000005</v>
       </c>
       <c r="L149">
-        <v>0.87145749031579001</v>
+        <v>0.87402469999999999</v>
       </c>
       <c r="M149">
-        <v>0.94536761094736799</v>
+        <v>0.99283719999999998</v>
       </c>
       <c r="N149">
-        <v>1.0632652920000001</v>
+        <v>1.0633846</v>
       </c>
       <c r="O149">
-        <v>1.16296758947368</v>
+        <v>1.1631762000000001</v>
       </c>
       <c r="P149">
-        <v>1.3580419646842099</v>
+        <v>1.3582460999999999</v>
       </c>
       <c r="Q149">
-        <v>1.5608252804210501</v>
+        <v>1.5608234999999999</v>
       </c>
       <c r="R149">
-        <v>1.57061156178947</v>
+        <v>1.5740794</v>
       </c>
       <c r="S149">
-        <v>1.8421277490000001</v>
+        <v>1.8565604</v>
       </c>
       <c r="T149">
-        <v>1.0520702532631601</v>
+        <v>1.0749333999999999</v>
       </c>
       <c r="U149">
-        <v>1.0520702532631601</v>
+        <v>1.0749333999999999</v>
       </c>
       <c r="V149">
-        <v>1.0520702532631601</v>
+        <v>1.0749333999999999</v>
       </c>
       <c r="W149">
-        <v>1.0520702532631601</v>
+        <v>1.0749333999999999</v>
       </c>
       <c r="X149">
-        <v>1.0520702532631601</v>
+        <v>1.0749333999999999</v>
       </c>
       <c r="Y149">
-        <v>1.0520702532631601</v>
+        <v>1.0749333999999999</v>
       </c>
     </row>
     <row r="150" spans="1:25" x14ac:dyDescent="0.2">
@@ -15528,64 +15528,64 @@
         <v>1976</v>
       </c>
       <c r="F150">
-        <v>1.9115208315789499E-3</v>
+        <v>7.646974E-3</v>
       </c>
       <c r="G150">
-        <v>3.9099114947368403E-2</v>
+        <v>0.11089765</v>
       </c>
       <c r="H150">
-        <v>0.25925024642105299</v>
+        <v>0.40551350000000003</v>
       </c>
       <c r="I150">
-        <v>0.48668990526315797</v>
+        <v>0.55375730000000001</v>
       </c>
       <c r="J150">
-        <v>0.705135786947368</v>
+        <v>0.72971739999999996</v>
       </c>
       <c r="K150">
-        <v>0.81721421052631604</v>
+        <v>0.82670690000000002</v>
       </c>
       <c r="L150">
-        <v>0.91238344189473697</v>
+        <v>0.91507119999999997</v>
       </c>
       <c r="M150">
-        <v>1.0394708707368401</v>
+        <v>1.0916656</v>
       </c>
       <c r="N150">
-        <v>1.21416692826316</v>
+        <v>1.2143031</v>
       </c>
       <c r="O150">
-        <v>1.25638509647368</v>
+        <v>1.2566105000000001</v>
       </c>
       <c r="P150">
-        <v>1.4032079805789499</v>
+        <v>1.4034188999999999</v>
       </c>
       <c r="Q150">
-        <v>1.64431981278947</v>
+        <v>1.6443179000000001</v>
       </c>
       <c r="R150">
-        <v>1.80193674705263</v>
+        <v>1.8059152999999999</v>
       </c>
       <c r="S150">
-        <v>1.8180695609999999</v>
+        <v>1.8323137</v>
       </c>
       <c r="T150">
-        <v>2.2386874573684201</v>
+        <v>2.2873378</v>
       </c>
       <c r="U150">
-        <v>2.2386874573684201</v>
+        <v>2.2873378</v>
       </c>
       <c r="V150">
-        <v>2.2386874573684201</v>
+        <v>2.2873378</v>
       </c>
       <c r="W150">
-        <v>2.2386874573684201</v>
+        <v>2.2873378</v>
       </c>
       <c r="X150">
-        <v>2.2386874573684201</v>
+        <v>2.2873378</v>
       </c>
       <c r="Y150">
-        <v>2.2386874573684201</v>
+        <v>2.2873378</v>
       </c>
     </row>
     <row r="151" spans="1:25" x14ac:dyDescent="0.2">
@@ -15605,64 +15605,64 @@
         <v>1977</v>
       </c>
       <c r="F151">
-        <v>1.4452827631578999E-3</v>
+        <v>5.7818039999999998E-3</v>
       </c>
       <c r="G151">
-        <v>4.0878150105263203E-2</v>
+        <v>0.11594357</v>
       </c>
       <c r="H151">
-        <v>0.22153829926315799</v>
+        <v>0.34652529999999998</v>
       </c>
       <c r="I151">
-        <v>0.50915665552631595</v>
+        <v>0.57931999999999995</v>
       </c>
       <c r="J151">
-        <v>0.62264494273684201</v>
+        <v>0.64435089999999995</v>
       </c>
       <c r="K151">
-        <v>0.76683888757894703</v>
+        <v>0.77574639999999995</v>
       </c>
       <c r="L151">
-        <v>0.86411045600000003</v>
+        <v>0.86665599999999998</v>
       </c>
       <c r="M151">
-        <v>0.94395794189473703</v>
+        <v>0.99135669999999998</v>
       </c>
       <c r="N151">
-        <v>1.1579748186315799</v>
+        <v>1.1581047</v>
       </c>
       <c r="O151">
-        <v>1.2444248946315799</v>
+        <v>1.2446482000000001</v>
       </c>
       <c r="P151">
-        <v>1.3148806931052599</v>
+        <v>1.3150782999999999</v>
       </c>
       <c r="Q151">
-        <v>1.4736836685789501</v>
+        <v>1.4736819999999999</v>
       </c>
       <c r="R151">
-        <v>1.64657182736842</v>
+        <v>1.6502074</v>
       </c>
       <c r="S151">
-        <v>1.8092157929999999</v>
+        <v>1.8233906</v>
       </c>
       <c r="T151">
-        <v>1.9164317435263201</v>
+        <v>1.9580789000000001</v>
       </c>
       <c r="U151">
-        <v>1.9164317435263201</v>
+        <v>1.9580789000000001</v>
       </c>
       <c r="V151">
-        <v>1.9164317435263201</v>
+        <v>1.9580789000000001</v>
       </c>
       <c r="W151">
-        <v>1.9164317435263201</v>
+        <v>1.9580789000000001</v>
       </c>
       <c r="X151">
-        <v>1.9164317435263201</v>
+        <v>1.9580789000000001</v>
       </c>
       <c r="Y151">
-        <v>1.9164317435263201</v>
+        <v>1.9580789000000001</v>
       </c>
     </row>
     <row r="152" spans="1:25" x14ac:dyDescent="0.2">
@@ -15682,64 +15682,64 @@
         <v>1978</v>
       </c>
       <c r="F152">
-        <v>1.89694299473684E-3</v>
+        <v>7.588656E-3</v>
       </c>
       <c r="G152">
-        <v>2.8487549578947401E-2</v>
+        <v>8.0799839999999998E-2</v>
       </c>
       <c r="H152">
-        <v>0.21348301168421099</v>
+        <v>0.33392539999999998</v>
       </c>
       <c r="I152">
-        <v>0.40102480578947403</v>
+        <v>0.4562872</v>
       </c>
       <c r="J152">
-        <v>0.60038498821052599</v>
+        <v>0.6213149</v>
       </c>
       <c r="K152">
-        <v>0.62411130189473696</v>
+        <v>0.6313609</v>
       </c>
       <c r="L152">
-        <v>0.747356231368421</v>
+        <v>0.7495579</v>
       </c>
       <c r="M152">
-        <v>0.82401417515789499</v>
+        <v>0.86539029999999995</v>
       </c>
       <c r="N152">
-        <v>0.96923630699999996</v>
+        <v>0.96934500000000001</v>
       </c>
       <c r="O152">
-        <v>1.09390505731579</v>
+        <v>1.0941012999999999</v>
       </c>
       <c r="P152">
-        <v>1.20039028294737</v>
+        <v>1.2005707000000001</v>
       </c>
       <c r="Q152">
-        <v>1.2727960545789501</v>
+        <v>1.2727946000000001</v>
       </c>
       <c r="R152">
-        <v>1.36015646221053</v>
+        <v>1.3631595999999999</v>
       </c>
       <c r="S152">
-        <v>1.5237781020000001</v>
+        <v>1.5357166</v>
       </c>
       <c r="T152">
-        <v>1.7577757072631599</v>
+        <v>1.7959750000000001</v>
       </c>
       <c r="U152">
-        <v>1.7577757072631599</v>
+        <v>1.7959750000000001</v>
       </c>
       <c r="V152">
-        <v>1.7577757072631599</v>
+        <v>1.7959750000000001</v>
       </c>
       <c r="W152">
-        <v>1.7577757072631599</v>
+        <v>1.7959750000000001</v>
       </c>
       <c r="X152">
-        <v>1.7577757072631599</v>
+        <v>1.7959750000000001</v>
       </c>
       <c r="Y152">
-        <v>1.7577757072631599</v>
+        <v>1.7959750000000001</v>
       </c>
     </row>
     <row r="153" spans="1:25" x14ac:dyDescent="0.2">
@@ -15759,64 +15759,64 @@
         <v>1979</v>
       </c>
       <c r="F153">
-        <v>1.4826669E-3</v>
+        <v>5.9313580000000003E-3</v>
       </c>
       <c r="G153">
-        <v>4.5216290947368398E-2</v>
+        <v>0.12824793000000001</v>
       </c>
       <c r="H153">
-        <v>0.179914255473684</v>
+        <v>0.2814179</v>
       </c>
       <c r="I153">
-        <v>0.467330382894737</v>
+        <v>0.53172989999999998</v>
       </c>
       <c r="J153">
-        <v>0.57185763536842105</v>
+        <v>0.59179309999999996</v>
       </c>
       <c r="K153">
-        <v>0.727762464</v>
+        <v>0.73621610000000004</v>
       </c>
       <c r="L153">
-        <v>0.73556976842105304</v>
+        <v>0.73773670000000002</v>
       </c>
       <c r="M153">
-        <v>0.86184942989473701</v>
+        <v>0.90512530000000002</v>
       </c>
       <c r="N153">
-        <v>1.02317520315789</v>
+        <v>1.02329</v>
       </c>
       <c r="O153">
-        <v>1.1072569263157901</v>
+        <v>1.1074556</v>
       </c>
       <c r="P153">
-        <v>1.2760617348947401</v>
+        <v>1.2762534999999999</v>
       </c>
       <c r="Q153">
-        <v>1.40518404</v>
+        <v>1.4051823999999999</v>
       </c>
       <c r="R153">
-        <v>1.4206322809473699</v>
+        <v>1.4237690000000001</v>
       </c>
       <c r="S153">
-        <v>1.5221876670000001</v>
+        <v>1.5341137</v>
       </c>
       <c r="T153">
-        <v>1.79032985994737</v>
+        <v>1.8292366</v>
       </c>
       <c r="U153">
-        <v>1.79032985994737</v>
+        <v>1.8292366</v>
       </c>
       <c r="V153">
-        <v>1.79032985994737</v>
+        <v>1.8292366</v>
       </c>
       <c r="W153">
-        <v>1.79032985994737</v>
+        <v>1.8292366</v>
       </c>
       <c r="X153">
-        <v>1.79032985994737</v>
+        <v>1.8292366</v>
       </c>
       <c r="Y153">
-        <v>1.79032985994737</v>
+        <v>1.8292366</v>
       </c>
     </row>
     <row r="154" spans="1:25" x14ac:dyDescent="0.2">
@@ -15836,64 +15836,64 @@
         <v>1980</v>
       </c>
       <c r="F154">
-        <v>1.3986752999999999E-3</v>
+        <v>5.595353E-3</v>
       </c>
       <c r="G154">
-        <v>2.6915963263157899E-2</v>
+        <v>7.6342320000000005E-2</v>
       </c>
       <c r="H154">
-        <v>0.217485895368421</v>
+        <v>0.34018660000000001</v>
       </c>
       <c r="I154">
-        <v>0.299952258157895</v>
+        <v>0.3412866</v>
       </c>
       <c r="J154">
-        <v>0.50753558442105295</v>
+        <v>0.52522869999999999</v>
       </c>
       <c r="K154">
-        <v>0.52792656252631598</v>
+        <v>0.5340589</v>
       </c>
       <c r="L154">
-        <v>0.65324675726315795</v>
+        <v>0.65517119999999995</v>
       </c>
       <c r="M154">
-        <v>0.64603103915789495</v>
+        <v>0.67847009999999996</v>
       </c>
       <c r="N154">
-        <v>0.81502791205263103</v>
+        <v>0.81511929999999999</v>
       </c>
       <c r="O154">
-        <v>0.890214319421052</v>
+        <v>0.890374</v>
       </c>
       <c r="P154">
-        <v>0.98370818621052603</v>
+        <v>0.98385599999999995</v>
       </c>
       <c r="Q154">
-        <v>1.13764882215789</v>
+        <v>1.1376474999999999</v>
       </c>
       <c r="R154">
-        <v>1.1944881825263201</v>
+        <v>1.1971255999999999</v>
       </c>
       <c r="S154">
-        <v>1.210840092</v>
+        <v>1.2203268</v>
       </c>
       <c r="T154">
-        <v>1.3620885227894699</v>
+        <v>1.3916888999999999</v>
       </c>
       <c r="U154">
-        <v>1.3620885227894699</v>
+        <v>1.3916888999999999</v>
       </c>
       <c r="V154">
-        <v>1.3620885227894699</v>
+        <v>1.3916888999999999</v>
       </c>
       <c r="W154">
-        <v>1.3620885227894699</v>
+        <v>1.3916888999999999</v>
       </c>
       <c r="X154">
-        <v>1.3620885227894699</v>
+        <v>1.3916888999999999</v>
       </c>
       <c r="Y154">
-        <v>1.3620885227894699</v>
+        <v>1.3916888999999999</v>
       </c>
     </row>
     <row r="155" spans="1:25" x14ac:dyDescent="0.2">
@@ -15913,64 +15913,64 @@
         <v>1981</v>
       </c>
       <c r="F155">
-        <v>1.55656501578947E-3</v>
+        <v>6.226985E-3</v>
       </c>
       <c r="G155">
-        <v>3.0022731684210501E-2</v>
+        <v>8.5154110000000005E-2</v>
       </c>
       <c r="H155">
-        <v>0.15307809484210499</v>
+        <v>0.2394414</v>
       </c>
       <c r="I155">
-        <v>0.42873054342105199</v>
+        <v>0.48781089999999999</v>
       </c>
       <c r="J155">
-        <v>0.385177901052631</v>
+        <v>0.3986055</v>
       </c>
       <c r="K155">
-        <v>0.55401160168421004</v>
+        <v>0.56044689999999997</v>
       </c>
       <c r="L155">
-        <v>0.56030942694736896</v>
+        <v>0.56196000000000002</v>
       </c>
       <c r="M155">
-        <v>0.67838082189473703</v>
+        <v>0.71244419999999997</v>
       </c>
       <c r="N155">
-        <v>0.72237260368420997</v>
+        <v>0.72245360000000003</v>
       </c>
       <c r="O155">
-        <v>0.83846287136842101</v>
+        <v>0.83861330000000001</v>
       </c>
       <c r="P155">
-        <v>0.93514555894736795</v>
+        <v>0.93528610000000001</v>
       </c>
       <c r="Q155">
-        <v>1.0369781346315801</v>
+        <v>1.0369769</v>
       </c>
       <c r="R155">
-        <v>1.14346711210526</v>
+        <v>1.1459918</v>
       </c>
       <c r="S155">
-        <v>1.20379842</v>
+        <v>1.2132299</v>
       </c>
       <c r="T155">
-        <v>1.28112265310526</v>
+        <v>1.3089634999999999</v>
       </c>
       <c r="U155">
-        <v>1.28112265310526</v>
+        <v>1.3089634999999999</v>
       </c>
       <c r="V155">
-        <v>1.28112265310526</v>
+        <v>1.3089634999999999</v>
       </c>
       <c r="W155">
-        <v>1.28112265310526</v>
+        <v>1.3089634999999999</v>
       </c>
       <c r="X155">
-        <v>1.28112265310526</v>
+        <v>1.3089634999999999</v>
       </c>
       <c r="Y155">
-        <v>1.28112265310526</v>
+        <v>1.3089634999999999</v>
       </c>
     </row>
     <row r="156" spans="1:25" x14ac:dyDescent="0.2">
@@ -15990,64 +15990,64 @@
         <v>1982</v>
       </c>
       <c r="F156">
-        <v>1.0589922315789499E-3</v>
+        <v>4.2364619999999999E-3</v>
       </c>
       <c r="G156">
-        <v>3.0618436947368401E-2</v>
+        <v>8.6843719999999999E-2</v>
       </c>
       <c r="H156">
-        <v>0.156471613368421</v>
+        <v>0.24474940000000001</v>
       </c>
       <c r="I156">
-        <v>0.27653421631578901</v>
+        <v>0.31464150000000002</v>
       </c>
       <c r="J156">
-        <v>0.50451739242105198</v>
+        <v>0.52210529999999999</v>
       </c>
       <c r="K156">
-        <v>0.38529760168421001</v>
+        <v>0.38977319999999999</v>
       </c>
       <c r="L156">
-        <v>0.53883502778947401</v>
+        <v>0.54042239999999997</v>
       </c>
       <c r="M156">
-        <v>0.53322040336842103</v>
+        <v>0.55999489999999996</v>
       </c>
       <c r="N156">
-        <v>0.69512675115789402</v>
+        <v>0.69520470000000001</v>
       </c>
       <c r="O156">
-        <v>0.68101268352631605</v>
+        <v>0.68113489999999999</v>
       </c>
       <c r="P156">
-        <v>0.80714396368421004</v>
+        <v>0.80726529999999996</v>
       </c>
       <c r="Q156">
-        <v>0.903368692421052</v>
+        <v>0.9033677</v>
       </c>
       <c r="R156">
-        <v>0.95514120947368397</v>
+        <v>0.95725009999999999</v>
       </c>
       <c r="S156">
-        <v>1.0560344850000001</v>
+        <v>1.0643083</v>
       </c>
       <c r="T156">
-        <v>1.1671863752631599</v>
+        <v>1.1925512</v>
       </c>
       <c r="U156">
-        <v>1.1671863752631599</v>
+        <v>1.1925512</v>
       </c>
       <c r="V156">
-        <v>1.1671863752631599</v>
+        <v>1.1925512</v>
       </c>
       <c r="W156">
-        <v>1.1671863752631599</v>
+        <v>1.1925512</v>
       </c>
       <c r="X156">
-        <v>1.1671863752631599</v>
+        <v>1.1925512</v>
       </c>
       <c r="Y156">
-        <v>1.1671863752631599</v>
+        <v>1.1925512</v>
       </c>
     </row>
     <row r="157" spans="1:25" x14ac:dyDescent="0.2">
@@ -16067,64 +16067,64 @@
         <v>1983</v>
       </c>
       <c r="F157">
-        <v>1.04636122105263E-3</v>
+        <v>4.1859319999999998E-3</v>
       </c>
       <c r="G157">
-        <v>2.2979744210526301E-2</v>
+        <v>6.5177940000000004E-2</v>
       </c>
       <c r="H157">
-        <v>0.176037479157895</v>
+        <v>0.27535389999999998</v>
       </c>
       <c r="I157">
-        <v>0.31182300368421001</v>
+        <v>0.35479319999999998</v>
       </c>
       <c r="J157">
-        <v>0.35898573305263098</v>
+        <v>0.37150030000000001</v>
       </c>
       <c r="K157">
-        <v>0.55673398231578897</v>
+        <v>0.5632009</v>
       </c>
       <c r="L157">
-        <v>0.41339941094736898</v>
+        <v>0.41461720000000002</v>
       </c>
       <c r="M157">
-        <v>0.56568066442105303</v>
+        <v>0.59408510000000003</v>
       </c>
       <c r="N157">
-        <v>0.60274529857894699</v>
+        <v>0.60281289999999998</v>
       </c>
       <c r="O157">
-        <v>0.72292711168420998</v>
+        <v>0.72305680000000006</v>
       </c>
       <c r="P157">
-        <v>0.72320096747368401</v>
+        <v>0.72330970000000006</v>
       </c>
       <c r="Q157">
-        <v>0.86014855184210504</v>
+        <v>0.86014760000000001</v>
       </c>
       <c r="R157">
-        <v>0.91790905715789495</v>
+        <v>0.91993579999999997</v>
       </c>
       <c r="S157">
-        <v>0.97310258099999902</v>
+        <v>0.9807266</v>
       </c>
       <c r="T157">
-        <v>1.12953887705263</v>
+        <v>1.1540855999999999</v>
       </c>
       <c r="U157">
-        <v>1.12953887705263</v>
+        <v>1.1540855999999999</v>
       </c>
       <c r="V157">
-        <v>1.12953887705263</v>
+        <v>1.1540855999999999</v>
       </c>
       <c r="W157">
-        <v>1.12953887705263</v>
+        <v>1.1540855999999999</v>
       </c>
       <c r="X157">
-        <v>1.12953887705263</v>
+        <v>1.1540855999999999</v>
       </c>
       <c r="Y157">
-        <v>1.12953887705263</v>
+        <v>1.1540855999999999</v>
       </c>
     </row>
     <row r="158" spans="1:25" x14ac:dyDescent="0.2">
@@ -16144,64 +16144,64 @@
         <v>1984</v>
       </c>
       <c r="F158">
-        <v>1.1079341842105299E-3</v>
+        <v>4.4322529999999997E-3</v>
       </c>
       <c r="G158">
-        <v>2.3675312842105299E-2</v>
+        <v>6.7150790000000002E-2</v>
       </c>
       <c r="H158">
-        <v>0.13776184231579</v>
+        <v>0.21548400000000001</v>
       </c>
       <c r="I158">
-        <v>0.36579629263157898</v>
+        <v>0.41620410000000002</v>
       </c>
       <c r="J158">
-        <v>0.422083322105263</v>
+        <v>0.43679750000000001</v>
       </c>
       <c r="K158">
-        <v>0.41305748968421002</v>
+        <v>0.41785549999999999</v>
       </c>
       <c r="L158">
-        <v>0.62284938736842099</v>
+        <v>0.62468420000000002</v>
       </c>
       <c r="M158">
-        <v>0.452529648842105</v>
+        <v>0.47525240000000002</v>
       </c>
       <c r="N158">
-        <v>0.66674539657894705</v>
+        <v>0.66682019999999997</v>
       </c>
       <c r="O158">
-        <v>0.65362110773684201</v>
+        <v>0.65373840000000005</v>
       </c>
       <c r="P158">
-        <v>0.80049756363157898</v>
+        <v>0.80061789999999999</v>
       </c>
       <c r="Q158">
-        <v>0.80360592678947296</v>
+        <v>0.80360500000000001</v>
       </c>
       <c r="R158">
-        <v>0.911317737789474</v>
+        <v>0.91332990000000003</v>
       </c>
       <c r="S158">
-        <v>0.97510733099999902</v>
+        <v>0.98274709999999998</v>
       </c>
       <c r="T158">
-        <v>1.08528407657895</v>
+        <v>1.1088690999999999</v>
       </c>
       <c r="U158">
-        <v>1.08528407657895</v>
+        <v>1.1088690999999999</v>
       </c>
       <c r="V158">
-        <v>1.08528407657895</v>
+        <v>1.1088690999999999</v>
       </c>
       <c r="W158">
-        <v>1.08528407657895</v>
+        <v>1.1088690999999999</v>
       </c>
       <c r="X158">
-        <v>1.08528407657895</v>
+        <v>1.1088690999999999</v>
       </c>
       <c r="Y158">
-        <v>1.08528407657895</v>
+        <v>1.1088690999999999</v>
       </c>
     </row>
     <row r="159" spans="1:25" x14ac:dyDescent="0.2">
@@ -16221,64 +16221,64 @@
         <v>1985</v>
       </c>
       <c r="F159">
-        <v>1.6994084684210499E-3</v>
+        <v>6.7984250000000003E-3</v>
       </c>
       <c r="G159">
-        <v>2.6712968421052599E-2</v>
+        <v>7.5766559999999997E-2</v>
       </c>
       <c r="H159">
-        <v>0.15124241242105299</v>
+        <v>0.23657</v>
       </c>
       <c r="I159">
-        <v>0.30504030815789501</v>
+        <v>0.34707579999999999</v>
       </c>
       <c r="J159">
-        <v>0.52762264715789498</v>
+        <v>0.54601599999999995</v>
       </c>
       <c r="K159">
-        <v>0.51751804547368396</v>
+        <v>0.52352949999999998</v>
       </c>
       <c r="L159">
-        <v>0.49242466610526298</v>
+        <v>0.49387530000000002</v>
       </c>
       <c r="M159">
-        <v>0.72653109726315801</v>
+        <v>0.76301229999999998</v>
       </c>
       <c r="N159">
-        <v>0.56836820131578902</v>
+        <v>0.56843200000000005</v>
       </c>
       <c r="O159">
-        <v>0.770453184789473</v>
+        <v>0.77059140000000004</v>
       </c>
       <c r="P159">
-        <v>0.77123297415789405</v>
+        <v>0.7713489</v>
       </c>
       <c r="Q159">
-        <v>0.94784697047368405</v>
+        <v>0.94784590000000002</v>
       </c>
       <c r="R159">
-        <v>0.90726358094736903</v>
+        <v>0.90926680000000004</v>
       </c>
       <c r="S159">
-        <v>1.0316124719999999</v>
+        <v>1.0396949</v>
       </c>
       <c r="T159">
-        <v>1.1588606825263199</v>
+        <v>1.1840446</v>
       </c>
       <c r="U159">
-        <v>1.1588606825263199</v>
+        <v>1.1840446</v>
       </c>
       <c r="V159">
-        <v>1.1588606825263199</v>
+        <v>1.1840446</v>
       </c>
       <c r="W159">
-        <v>1.1588606825263199</v>
+        <v>1.1840446</v>
       </c>
       <c r="X159">
-        <v>1.1588606825263199</v>
+        <v>1.1840446</v>
       </c>
       <c r="Y159">
-        <v>1.1588606825263199</v>
+        <v>1.1840446</v>
       </c>
     </row>
     <row r="160" spans="1:25" x14ac:dyDescent="0.2">
@@ -16298,64 +16298,64 @@
         <v>1986</v>
       </c>
       <c r="F160">
-        <v>1.3580821736842101E-3</v>
+        <v>5.432961E-3</v>
       </c>
       <c r="G160">
-        <v>3.5899143473684197E-2</v>
+        <v>0.1018215</v>
       </c>
       <c r="H160">
-        <v>0.14951274221052599</v>
+        <v>0.2338645</v>
       </c>
       <c r="I160">
-        <v>0.29341351368420998</v>
+        <v>0.3338468</v>
       </c>
       <c r="J160">
-        <v>0.38549570105263098</v>
+        <v>0.39893440000000002</v>
       </c>
       <c r="K160">
-        <v>0.56679883957894694</v>
+        <v>0.57338270000000002</v>
       </c>
       <c r="L160">
-        <v>0.54054649115789499</v>
+        <v>0.54213889999999998</v>
       </c>
       <c r="M160">
-        <v>0.50325632421052602</v>
+        <v>0.52852619999999995</v>
       </c>
       <c r="N160">
-        <v>0.799494092052631</v>
+        <v>0.79958379999999996</v>
       </c>
       <c r="O160">
-        <v>0.57543238136842101</v>
+        <v>0.57553560000000004</v>
       </c>
       <c r="P160">
-        <v>0.79649687036842098</v>
+        <v>0.79661660000000001</v>
       </c>
       <c r="Q160">
-        <v>0.80009587515789404</v>
+        <v>0.800095</v>
       </c>
       <c r="R160">
-        <v>0.937576652210527</v>
+        <v>0.9396468</v>
       </c>
       <c r="S160">
-        <v>0.89982594899999901</v>
+        <v>0.90687589999999996</v>
       </c>
       <c r="T160">
-        <v>1.0741715524736899</v>
+        <v>1.097515</v>
       </c>
       <c r="U160">
-        <v>1.0741715524736899</v>
+        <v>1.097515</v>
       </c>
       <c r="V160">
-        <v>1.0741715524736899</v>
+        <v>1.097515</v>
       </c>
       <c r="W160">
-        <v>1.0741715524736899</v>
+        <v>1.097515</v>
       </c>
       <c r="X160">
-        <v>1.0741715524736899</v>
+        <v>1.097515</v>
       </c>
       <c r="Y160">
-        <v>1.0741715524736899</v>
+        <v>1.097515</v>
       </c>
     </row>
     <row r="161" spans="1:25" x14ac:dyDescent="0.2">
@@ -16375,64 +16375,64 @@
         <v>1987</v>
       </c>
       <c r="F161">
-        <v>1.3866976894736801E-3</v>
+        <v>5.5474369999999997E-3</v>
       </c>
       <c r="G161">
-        <v>2.6915894315789501E-2</v>
+        <v>7.6342119999999999E-2</v>
       </c>
       <c r="H161">
-        <v>0.18851098452631601</v>
+        <v>0.29486469999999998</v>
       </c>
       <c r="I161">
-        <v>0.27213285578947299</v>
+        <v>0.30963360000000001</v>
       </c>
       <c r="J161">
-        <v>0.34788748800000002</v>
+        <v>0.36001509999999998</v>
       </c>
       <c r="K161">
-        <v>0.38852729431578897</v>
+        <v>0.39304040000000001</v>
       </c>
       <c r="L161">
-        <v>0.55543453957894795</v>
+        <v>0.55707079999999998</v>
       </c>
       <c r="M161">
-        <v>0.51829717136842102</v>
+        <v>0.54432230000000004</v>
       </c>
       <c r="N161">
-        <v>0.51957309647368399</v>
+        <v>0.51963139999999997</v>
       </c>
       <c r="O161">
-        <v>0.75940960026315796</v>
+        <v>0.75954580000000005</v>
       </c>
       <c r="P161">
-        <v>0.55812109736842097</v>
+        <v>0.55820499999999995</v>
       </c>
       <c r="Q161">
-        <v>0.77524126342105204</v>
+        <v>0.77524040000000005</v>
       </c>
       <c r="R161">
-        <v>0.74251797831579003</v>
+        <v>0.74415739999999997</v>
       </c>
       <c r="S161">
-        <v>0.872425223999999</v>
+        <v>0.8792605</v>
       </c>
       <c r="T161">
-        <v>0.87904669563158</v>
+        <v>0.8981498</v>
       </c>
       <c r="U161">
-        <v>0.87904669563158</v>
+        <v>0.8981498</v>
       </c>
       <c r="V161">
-        <v>0.87904669563158</v>
+        <v>0.8981498</v>
       </c>
       <c r="W161">
-        <v>0.87904669563158</v>
+        <v>0.8981498</v>
       </c>
       <c r="X161">
-        <v>0.87904669563158</v>
+        <v>0.8981498</v>
       </c>
       <c r="Y161">
-        <v>0.87904669563158</v>
+        <v>0.8981498</v>
       </c>
     </row>
     <row r="162" spans="1:25" x14ac:dyDescent="0.2">
@@ -16452,64 +16452,64 @@
         <v>1988</v>
       </c>
       <c r="F162">
-        <v>1.61080642105263E-3</v>
+        <v>6.4439759999999997E-3</v>
       </c>
       <c r="G162">
-        <v>3.1529204105263199E-2</v>
+        <v>8.9426950000000005E-2</v>
       </c>
       <c r="H162">
-        <v>0.16214726515789499</v>
+        <v>0.2536272</v>
       </c>
       <c r="I162">
-        <v>0.393629714210526</v>
+        <v>0.44787310000000002</v>
       </c>
       <c r="J162">
-        <v>0.37015881642105197</v>
+        <v>0.38306289999999998</v>
       </c>
       <c r="K162">
-        <v>0.40224353684210501</v>
+        <v>0.4069159</v>
       </c>
       <c r="L162">
-        <v>0.43679110315789499</v>
+        <v>0.43807780000000002</v>
       </c>
       <c r="M162">
-        <v>0.610980199578947</v>
+        <v>0.64165919999999999</v>
       </c>
       <c r="N162">
-        <v>0.613881634263158</v>
+        <v>0.61395049999999995</v>
       </c>
       <c r="O162">
-        <v>0.56618185263157905</v>
+        <v>0.56628339999999999</v>
       </c>
       <c r="P162">
-        <v>0.84500382694736798</v>
+        <v>0.84513079999999996</v>
       </c>
       <c r="Q162">
-        <v>0.62320312563157898</v>
+        <v>0.62320240000000005</v>
       </c>
       <c r="R162">
-        <v>0.82537300199999997</v>
+        <v>0.82719540000000003</v>
       </c>
       <c r="S162">
-        <v>0.79264142099999901</v>
+        <v>0.7988516</v>
       </c>
       <c r="T162">
-        <v>0.97775494452631695</v>
+        <v>0.99900310000000003</v>
       </c>
       <c r="U162">
-        <v>0.97775494452631695</v>
+        <v>0.99900310000000003</v>
       </c>
       <c r="V162">
-        <v>0.97775494452631695</v>
+        <v>0.99900310000000003</v>
       </c>
       <c r="W162">
-        <v>0.97775494452631695</v>
+        <v>0.99900310000000003</v>
       </c>
       <c r="X162">
-        <v>0.97775494452631695</v>
+        <v>0.99900310000000003</v>
       </c>
       <c r="Y162">
-        <v>0.97775494452631695</v>
+        <v>0.99900310000000003</v>
       </c>
     </row>
     <row r="163" spans="1:25" x14ac:dyDescent="0.2">
@@ -16529,64 +16529,64 @@
         <v>1989</v>
       </c>
       <c r="F163">
-        <v>1.57140268421053E-3</v>
+        <v>6.2863429999999998E-3</v>
       </c>
       <c r="G163">
-        <v>3.36103942105263E-2</v>
+        <v>9.5329880000000006E-2</v>
       </c>
       <c r="H163">
-        <v>0.174306219789474</v>
+        <v>0.2726459</v>
       </c>
       <c r="I163">
-        <v>0.31071338736842102</v>
+        <v>0.35353059999999997</v>
       </c>
       <c r="J163">
-        <v>0.49135359073684198</v>
+        <v>0.50848260000000001</v>
       </c>
       <c r="K163">
-        <v>0.39276934484210502</v>
+        <v>0.39733170000000001</v>
       </c>
       <c r="L163">
-        <v>0.414992773684211</v>
+        <v>0.41621530000000001</v>
       </c>
       <c r="M163">
-        <v>0.440927427368421</v>
+        <v>0.46306760000000002</v>
       </c>
       <c r="N163">
-        <v>0.66409779078947295</v>
+        <v>0.66417230000000005</v>
       </c>
       <c r="O163">
-        <v>0.61389352799999997</v>
+        <v>0.61400370000000004</v>
       </c>
       <c r="P163">
-        <v>0.57814605236842098</v>
+        <v>0.57823290000000005</v>
       </c>
       <c r="Q163">
-        <v>0.86588253236842105</v>
+        <v>0.86588149999999997</v>
       </c>
       <c r="R163">
-        <v>0.60889458368421101</v>
+        <v>0.61023899999999998</v>
       </c>
       <c r="S163">
-        <v>0.80857289699999901</v>
+        <v>0.81490790000000002</v>
       </c>
       <c r="T163">
-        <v>0.81522545763158005</v>
+        <v>0.83294159999999995</v>
       </c>
       <c r="U163">
-        <v>0.81522545763158005</v>
+        <v>0.83294159999999995</v>
       </c>
       <c r="V163">
-        <v>0.81522545763158005</v>
+        <v>0.83294159999999995</v>
       </c>
       <c r="W163">
-        <v>0.81522545763158005</v>
+        <v>0.83294159999999995</v>
       </c>
       <c r="X163">
-        <v>0.81522545763158005</v>
+        <v>0.83294159999999995</v>
       </c>
       <c r="Y163">
-        <v>0.81522545763158005</v>
+        <v>0.83294159999999995</v>
       </c>
     </row>
     <row r="164" spans="1:25" x14ac:dyDescent="0.2">
@@ -16606,64 +16606,64 @@
         <v>1990</v>
       </c>
       <c r="F164">
-        <v>1.55079626842105E-3</v>
+        <v>6.2039069999999998E-3</v>
       </c>
       <c r="G164">
-        <v>3.43868932631579E-2</v>
+        <v>9.7532279999999999E-2</v>
       </c>
       <c r="H164">
-        <v>0.194871717157895</v>
+        <v>0.30481399999999997</v>
       </c>
       <c r="I164">
-        <v>0.350298685</v>
+        <v>0.39857090000000001</v>
       </c>
       <c r="J164">
-        <v>0.40676297263157901</v>
+        <v>0.42094310000000001</v>
       </c>
       <c r="K164">
-        <v>0.54678765221052605</v>
+        <v>0.55313909999999999</v>
       </c>
       <c r="L164">
-        <v>0.42497576231578998</v>
+        <v>0.42622769999999999</v>
       </c>
       <c r="M164">
-        <v>0.43934837726315801</v>
+        <v>0.46140930000000002</v>
       </c>
       <c r="N164">
-        <v>0.50262861931578895</v>
+        <v>0.50268500000000005</v>
       </c>
       <c r="O164">
-        <v>0.69649113268421003</v>
+        <v>0.69661609999999996</v>
       </c>
       <c r="P164">
-        <v>0.65743060168420997</v>
+        <v>0.65752940000000004</v>
       </c>
       <c r="Q164">
-        <v>0.62131681894736801</v>
+        <v>0.62131610000000004</v>
       </c>
       <c r="R164">
-        <v>0.88725137757894801</v>
+        <v>0.88921039999999996</v>
       </c>
       <c r="S164">
-        <v>0.62558486099999999</v>
+        <v>0.6304862</v>
       </c>
       <c r="T164">
-        <v>0.87215826052631595</v>
+        <v>0.89111169999999995</v>
       </c>
       <c r="U164">
-        <v>0.87215826052631595</v>
+        <v>0.89111169999999995</v>
       </c>
       <c r="V164">
-        <v>0.87215826052631595</v>
+        <v>0.89111169999999995</v>
       </c>
       <c r="W164">
-        <v>0.87215826052631595</v>
+        <v>0.89111169999999995</v>
       </c>
       <c r="X164">
-        <v>0.87215826052631595</v>
+        <v>0.89111169999999995</v>
       </c>
       <c r="Y164">
-        <v>0.87215826052631595</v>
+        <v>0.89111169999999995</v>
       </c>
     </row>
     <row r="165" spans="1:25" x14ac:dyDescent="0.2">
@@ -16683,64 +16683,64 @@
         <v>1991</v>
       </c>
       <c r="F165">
-        <v>1.6355204684210499E-3</v>
+        <v>6.5428439999999999E-3</v>
       </c>
       <c r="G165">
-        <v>3.3598287052631598E-2</v>
+        <v>9.5295539999999998E-2</v>
       </c>
       <c r="H165">
-        <v>0.19738996852631599</v>
+        <v>0.308753</v>
       </c>
       <c r="I165">
-        <v>0.38773165605263099</v>
+        <v>0.44116230000000001</v>
       </c>
       <c r="J165">
-        <v>0.45402198315789399</v>
+        <v>0.46984959999999998</v>
       </c>
       <c r="K165">
-        <v>0.44814960757894701</v>
+        <v>0.45335530000000002</v>
       </c>
       <c r="L165">
-        <v>0.58573651284210604</v>
+        <v>0.58746200000000004</v>
       </c>
       <c r="M165">
-        <v>0.44544048084210502</v>
+        <v>0.46780729999999998</v>
       </c>
       <c r="N165">
-        <v>0.49584519142105199</v>
+        <v>0.49590079999999997</v>
       </c>
       <c r="O165">
-        <v>0.52190057084210495</v>
+        <v>0.52199419999999996</v>
       </c>
       <c r="P165">
-        <v>0.73846413</v>
+        <v>0.73857510000000004</v>
       </c>
       <c r="Q165">
-        <v>0.69949135278947305</v>
+        <v>0.69949050000000002</v>
       </c>
       <c r="R165">
-        <v>0.63031512557894798</v>
+        <v>0.63170680000000001</v>
       </c>
       <c r="S165">
-        <v>0.90250102799999898</v>
+        <v>0.90957189999999999</v>
       </c>
       <c r="T165">
-        <v>0.66806592705263201</v>
+        <v>0.68258410000000003</v>
       </c>
       <c r="U165">
-        <v>0.66806592705263201</v>
+        <v>0.68258410000000003</v>
       </c>
       <c r="V165">
-        <v>0.66806592705263201</v>
+        <v>0.68258410000000003</v>
       </c>
       <c r="W165">
-        <v>0.66806592705263201</v>
+        <v>0.68258410000000003</v>
       </c>
       <c r="X165">
-        <v>0.66806592705263201</v>
+        <v>0.68258410000000003</v>
       </c>
       <c r="Y165">
-        <v>0.66806592705263201</v>
+        <v>0.68258410000000003</v>
       </c>
     </row>
     <row r="166" spans="1:25" x14ac:dyDescent="0.2">
@@ -16760,64 +16760,64 @@
         <v>1992</v>
       </c>
       <c r="F166">
-        <v>1.7855205789473699E-3</v>
+        <v>7.1429140000000002E-3</v>
       </c>
       <c r="G166">
-        <v>3.5590093789473698E-2</v>
+        <v>0.10094494</v>
       </c>
       <c r="H166">
-        <v>0.193713579894737</v>
+        <v>0.30300250000000001</v>
       </c>
       <c r="I166">
-        <v>0.39447405684210501</v>
+        <v>0.4488338</v>
       </c>
       <c r="J166">
-        <v>0.50475490610526297</v>
+        <v>0.52235109999999996</v>
       </c>
       <c r="K166">
-        <v>0.50242273010526295</v>
+        <v>0.50825880000000001</v>
       </c>
       <c r="L166">
-        <v>0.48218924484210601</v>
+        <v>0.48360969999999998</v>
       </c>
       <c r="M166">
-        <v>0.616649897263158</v>
+        <v>0.64761360000000001</v>
       </c>
       <c r="N166">
-        <v>0.504937403526316</v>
+        <v>0.50499400000000005</v>
       </c>
       <c r="O166">
-        <v>0.51712738436842098</v>
+        <v>0.51722020000000002</v>
       </c>
       <c r="P166">
-        <v>0.55579222373684201</v>
+        <v>0.55587580000000003</v>
       </c>
       <c r="Q166">
-        <v>0.78917392657894703</v>
+        <v>0.78917300000000001</v>
       </c>
       <c r="R166">
-        <v>0.71275097715789504</v>
+        <v>0.71432470000000003</v>
       </c>
       <c r="S166">
-        <v>0.64397589300000002</v>
+        <v>0.64902130000000002</v>
       </c>
       <c r="T166">
-        <v>0.96803632215789504</v>
+        <v>0.98907330000000004</v>
       </c>
       <c r="U166">
-        <v>0.96803632215789504</v>
+        <v>0.98907330000000004</v>
       </c>
       <c r="V166">
-        <v>0.96803632215789504</v>
+        <v>0.98907330000000004</v>
       </c>
       <c r="W166">
-        <v>0.96803632215789504</v>
+        <v>0.98907330000000004</v>
       </c>
       <c r="X166">
-        <v>0.96803632215789504</v>
+        <v>0.98907330000000004</v>
       </c>
       <c r="Y166">
-        <v>0.96803632215789504</v>
+        <v>0.98907330000000004</v>
       </c>
     </row>
     <row r="167" spans="1:25" x14ac:dyDescent="0.2">
@@ -16837,64 +16837,64 @@
         <v>1993</v>
       </c>
       <c r="F167">
-        <v>1.3877081842105299E-3</v>
+        <v>5.5514789999999998E-3</v>
       </c>
       <c r="G167">
-        <v>3.2840045263157903E-2</v>
+        <v>9.3144920000000006E-2</v>
       </c>
       <c r="H167">
-        <v>0.173435463789474</v>
+        <v>0.27128390000000002</v>
       </c>
       <c r="I167">
-        <v>0.32720442815789402</v>
+        <v>0.37229420000000002</v>
       </c>
       <c r="J167">
-        <v>0.43404359368421003</v>
+        <v>0.44917469999999998</v>
       </c>
       <c r="K167">
-        <v>0.47210500042105202</v>
+        <v>0.47758889999999998</v>
       </c>
       <c r="L167">
-        <v>0.45690873915789498</v>
+        <v>0.45825470000000001</v>
       </c>
       <c r="M167">
-        <v>0.42906142821052601</v>
+        <v>0.4506058</v>
       </c>
       <c r="N167">
-        <v>0.590815980473684</v>
+        <v>0.59088229999999997</v>
       </c>
       <c r="O167">
-        <v>0.445096915105263</v>
+        <v>0.44517679999999998</v>
       </c>
       <c r="P167">
-        <v>0.46546588894736801</v>
+        <v>0.4655358</v>
       </c>
       <c r="Q167">
-        <v>0.50202043957894704</v>
+        <v>0.50201989999999996</v>
       </c>
       <c r="R167">
-        <v>0.679663395263158</v>
+        <v>0.68116410000000005</v>
       </c>
       <c r="S167">
-        <v>0.615482109</v>
+        <v>0.62030430000000003</v>
       </c>
       <c r="T167">
-        <v>0.58382036863157905</v>
+        <v>0.59650769999999997</v>
       </c>
       <c r="U167">
-        <v>0.58382036863157905</v>
+        <v>0.59650769999999997</v>
       </c>
       <c r="V167">
-        <v>0.58382036863157905</v>
+        <v>0.59650769999999997</v>
       </c>
       <c r="W167">
-        <v>0.58382036863157905</v>
+        <v>0.59650769999999997</v>
       </c>
       <c r="X167">
-        <v>0.58382036863157905</v>
+        <v>0.59650769999999997</v>
       </c>
       <c r="Y167">
-        <v>0.58382036863157905</v>
+        <v>0.59650769999999997</v>
       </c>
     </row>
     <row r="168" spans="1:25" x14ac:dyDescent="0.2">
@@ -16914,64 +16914,64 @@
         <v>1994</v>
       </c>
       <c r="F168">
-        <v>1.6215467052631599E-3</v>
+        <v>6.4869419999999999E-3</v>
       </c>
       <c r="G168">
-        <v>3.27156917894737E-2</v>
+        <v>9.279221E-2</v>
       </c>
       <c r="H168">
-        <v>0.20513106421052599</v>
+        <v>0.32086150000000002</v>
       </c>
       <c r="I168">
-        <v>0.37550514157894699</v>
+        <v>0.42725089999999999</v>
       </c>
       <c r="J168">
-        <v>0.46148019957894698</v>
+        <v>0.47756779999999999</v>
       </c>
       <c r="K168">
-        <v>0.52036782063157805</v>
+        <v>0.52641230000000006</v>
       </c>
       <c r="L168">
-        <v>0.55032315221052697</v>
+        <v>0.5519444</v>
       </c>
       <c r="M168">
-        <v>0.52113525557894702</v>
+        <v>0.54730290000000004</v>
       </c>
       <c r="N168">
-        <v>0.52692892294736804</v>
+        <v>0.52698800000000001</v>
       </c>
       <c r="O168">
-        <v>0.66755686926315805</v>
+        <v>0.66767659999999995</v>
       </c>
       <c r="P168">
-        <v>0.51352787984210502</v>
+        <v>0.51360510000000004</v>
       </c>
       <c r="Q168">
-        <v>0.53890951405263099</v>
+        <v>0.53890890000000002</v>
       </c>
       <c r="R168">
-        <v>0.55419377031578998</v>
+        <v>0.55541739999999995</v>
       </c>
       <c r="S168">
-        <v>0.75229902000000004</v>
+        <v>0.75819309999999995</v>
       </c>
       <c r="T168">
-        <v>0.71522732226315799</v>
+        <v>0.73077040000000004</v>
       </c>
       <c r="U168">
-        <v>0.71522732226315799</v>
+        <v>0.73077040000000004</v>
       </c>
       <c r="V168">
-        <v>0.71522732226315799</v>
+        <v>0.73077040000000004</v>
       </c>
       <c r="W168">
-        <v>0.71522732226315799</v>
+        <v>0.73077040000000004</v>
       </c>
       <c r="X168">
-        <v>0.71522732226315799</v>
+        <v>0.73077040000000004</v>
       </c>
       <c r="Y168">
-        <v>0.71522732226315799</v>
+        <v>0.73077040000000004</v>
       </c>
     </row>
     <row r="169" spans="1:25" x14ac:dyDescent="0.2">
@@ -16991,64 +16991,64 @@
         <v>1995</v>
       </c>
       <c r="F169">
-        <v>1.8659506105263199E-3</v>
+        <v>7.4646720000000003E-3</v>
       </c>
       <c r="G169">
-        <v>3.7527666526315798E-2</v>
+        <v>0.10644052</v>
       </c>
       <c r="H169">
-        <v>0.20060785947368401</v>
+        <v>0.31378640000000002</v>
       </c>
       <c r="I169">
-        <v>0.43598712184210497</v>
+        <v>0.49606749999999999</v>
       </c>
       <c r="J169">
-        <v>0.51989308210526297</v>
+        <v>0.53801699999999997</v>
       </c>
       <c r="K169">
-        <v>0.54311823663157899</v>
+        <v>0.549427</v>
       </c>
       <c r="L169">
-        <v>0.59546159200000004</v>
+        <v>0.59721579999999996</v>
       </c>
       <c r="M169">
-        <v>0.61617344168420995</v>
+        <v>0.6471133</v>
       </c>
       <c r="N169">
-        <v>0.62827125678947404</v>
+        <v>0.6283417</v>
       </c>
       <c r="O169">
-        <v>0.584456629263158</v>
+        <v>0.58456149999999996</v>
       </c>
       <c r="P169">
-        <v>0.75606965905263102</v>
+        <v>0.7561833</v>
       </c>
       <c r="Q169">
-        <v>0.58365495142105295</v>
+        <v>0.58365429999999996</v>
       </c>
       <c r="R169">
-        <v>0.58400991578947403</v>
+        <v>0.58529940000000003</v>
       </c>
       <c r="S169">
-        <v>0.60217452900000001</v>
+        <v>0.6068924</v>
       </c>
       <c r="T169">
-        <v>0.85818969115789501</v>
+        <v>0.87683949999999999</v>
       </c>
       <c r="U169">
-        <v>0.85818969115789501</v>
+        <v>0.87683949999999999</v>
       </c>
       <c r="V169">
-        <v>0.85818969115789501</v>
+        <v>0.87683949999999999</v>
       </c>
       <c r="W169">
-        <v>0.85818969115789501</v>
+        <v>0.87683949999999999</v>
       </c>
       <c r="X169">
-        <v>0.85818969115789501</v>
+        <v>0.87683949999999999</v>
       </c>
       <c r="Y169">
-        <v>0.85818969115789501</v>
+        <v>0.87683949999999999</v>
       </c>
     </row>
     <row r="170" spans="1:25" x14ac:dyDescent="0.2">
@@ -17068,64 +17068,64 @@
         <v>1996</v>
       </c>
       <c r="F170">
-        <v>1.6108232684210501E-3</v>
+        <v>6.444043E-3</v>
       </c>
       <c r="G170">
-        <v>3.8615407789473699E-2</v>
+        <v>0.1095257</v>
       </c>
       <c r="H170">
-        <v>0.20576990568421</v>
+        <v>0.3218607</v>
       </c>
       <c r="I170">
-        <v>0.38126636552631499</v>
+        <v>0.43380600000000002</v>
       </c>
       <c r="J170">
-        <v>0.53977168715789503</v>
+        <v>0.55858859999999999</v>
       </c>
       <c r="K170">
-        <v>0.54713397221052595</v>
+        <v>0.55348940000000002</v>
       </c>
       <c r="L170">
-        <v>0.55574562421052698</v>
+        <v>0.55738279999999996</v>
       </c>
       <c r="M170">
-        <v>0.59617991157894701</v>
+        <v>0.6261158</v>
       </c>
       <c r="N170">
-        <v>0.664260005368421</v>
+        <v>0.66433450000000005</v>
       </c>
       <c r="O170">
-        <v>0.62314025873684198</v>
+        <v>0.62325209999999998</v>
       </c>
       <c r="P170">
-        <v>0.59192159826315804</v>
+        <v>0.59201060000000005</v>
       </c>
       <c r="Q170">
-        <v>0.76840896126315805</v>
+        <v>0.76840810000000004</v>
       </c>
       <c r="R170">
-        <v>0.56558628</v>
+        <v>0.56683510000000004</v>
       </c>
       <c r="S170">
-        <v>0.56743919099999995</v>
+        <v>0.57188490000000003</v>
       </c>
       <c r="T170">
-        <v>0.61426194215789498</v>
+        <v>0.62761080000000002</v>
       </c>
       <c r="U170">
-        <v>0.61426194215789498</v>
+        <v>0.62761080000000002</v>
       </c>
       <c r="V170">
-        <v>0.61426194215789498</v>
+        <v>0.62761080000000002</v>
       </c>
       <c r="W170">
-        <v>0.61426194215789498</v>
+        <v>0.62761080000000002</v>
       </c>
       <c r="X170">
-        <v>0.61426194215789498</v>
+        <v>0.62761080000000002</v>
       </c>
       <c r="Y170">
-        <v>0.61426194215789498</v>
+        <v>0.62761080000000002</v>
       </c>
     </row>
     <row r="171" spans="1:25" x14ac:dyDescent="0.2">
@@ -17145,64 +17145,64 @@
         <v>1997</v>
       </c>
       <c r="F171">
-        <v>1.58213306842105E-3</v>
+        <v>6.3292690000000002E-3</v>
       </c>
       <c r="G171">
-        <v>3.5286380631578997E-2</v>
+        <v>0.10008351</v>
       </c>
       <c r="H171">
-        <v>0.22412462810526301</v>
+        <v>0.35057080000000002</v>
       </c>
       <c r="I171">
-        <v>0.41396260631578902</v>
+        <v>0.47100789999999998</v>
       </c>
       <c r="J171">
-        <v>0.49964754947368401</v>
+        <v>0.51706569999999996</v>
       </c>
       <c r="K171">
-        <v>0.60129635115789404</v>
+        <v>0.60828090000000001</v>
       </c>
       <c r="L171">
-        <v>0.59261701978947401</v>
+        <v>0.59436279999999997</v>
       </c>
       <c r="M171">
-        <v>0.58897702989473599</v>
+        <v>0.61855119999999997</v>
       </c>
       <c r="N171">
-        <v>0.68031684994736796</v>
+        <v>0.68039320000000003</v>
       </c>
       <c r="O171">
-        <v>0.69738955957894699</v>
+        <v>0.69751470000000004</v>
       </c>
       <c r="P171">
-        <v>0.66803071973684203</v>
+        <v>0.66813109999999998</v>
       </c>
       <c r="Q171">
-        <v>0.63678597299999995</v>
+        <v>0.63678520000000005</v>
       </c>
       <c r="R171">
-        <v>0.78819527726315797</v>
+        <v>0.78993559999999996</v>
       </c>
       <c r="S171">
-        <v>0.58169697300000001</v>
+        <v>0.58625439999999995</v>
       </c>
       <c r="T171">
-        <v>0.61270200484210502</v>
+        <v>0.62601700000000005</v>
       </c>
       <c r="U171">
-        <v>0.61270200484210502</v>
+        <v>0.62601700000000005</v>
       </c>
       <c r="V171">
-        <v>0.61270200484210502</v>
+        <v>0.62601700000000005</v>
       </c>
       <c r="W171">
-        <v>0.61270200484210502</v>
+        <v>0.62601700000000005</v>
       </c>
       <c r="X171">
-        <v>0.61270200484210502</v>
+        <v>0.62601700000000005</v>
       </c>
       <c r="Y171">
-        <v>0.61270200484210502</v>
+        <v>0.62601700000000005</v>
       </c>
     </row>
     <row r="172" spans="1:25" x14ac:dyDescent="0.2">
@@ -17222,64 +17222,64 @@
         <v>1998</v>
       </c>
       <c r="F172">
-        <v>1.6454510368421099E-3</v>
+        <v>6.5825709999999997E-3</v>
       </c>
       <c r="G172">
-        <v>3.1875471578947399E-2</v>
+        <v>9.0409080000000003E-2</v>
       </c>
       <c r="H172">
-        <v>0.18836078347368401</v>
+        <v>0.2946298</v>
       </c>
       <c r="I172">
-        <v>0.41468984236842099</v>
+        <v>0.47183540000000002</v>
       </c>
       <c r="J172">
-        <v>0.49894284589473697</v>
+        <v>0.51633640000000003</v>
       </c>
       <c r="K172">
-        <v>0.51191347452631497</v>
+        <v>0.51785979999999998</v>
       </c>
       <c r="L172">
-        <v>0.59899535010526395</v>
+        <v>0.60075990000000001</v>
       </c>
       <c r="M172">
-        <v>0.57763154442105202</v>
+        <v>0.60663610000000001</v>
       </c>
       <c r="N172">
-        <v>0.61813979194736801</v>
+        <v>0.61820909999999996</v>
       </c>
       <c r="O172">
-        <v>0.65690567810526301</v>
+        <v>0.65702349999999998</v>
       </c>
       <c r="P172">
-        <v>0.68760741078947396</v>
+        <v>0.68771070000000001</v>
       </c>
       <c r="Q172">
-        <v>0.66096763910526302</v>
+        <v>0.66096690000000002</v>
       </c>
       <c r="R172">
-        <v>0.60074400389473703</v>
+        <v>0.60207040000000001</v>
       </c>
       <c r="S172">
-        <v>0.74556622800000005</v>
+        <v>0.75140759999999995</v>
       </c>
       <c r="T172">
-        <v>0.57767180284210495</v>
+        <v>0.59022549999999996</v>
       </c>
       <c r="U172">
-        <v>0.57767180284210495</v>
+        <v>0.59022549999999996</v>
       </c>
       <c r="V172">
-        <v>0.57767180284210495</v>
+        <v>0.59022549999999996</v>
       </c>
       <c r="W172">
-        <v>0.57767180284210495</v>
+        <v>0.59022549999999996</v>
       </c>
       <c r="X172">
-        <v>0.57767180284210495</v>
+        <v>0.59022549999999996</v>
       </c>
       <c r="Y172">
-        <v>0.57767180284210495</v>
+        <v>0.59022549999999996</v>
       </c>
     </row>
     <row r="173" spans="1:25" x14ac:dyDescent="0.2">
@@ -17299,64 +17299,64 @@
         <v>1999</v>
       </c>
       <c r="F173">
-        <v>1.48831580526316E-3</v>
+        <v>5.9539570000000002E-3</v>
       </c>
       <c r="G173">
-        <v>3.5012990526315797E-2</v>
+        <v>9.9308090000000002E-2</v>
       </c>
       <c r="H173">
-        <v>0.179709305368421</v>
+        <v>0.28109729999999999</v>
       </c>
       <c r="I173">
-        <v>0.36809065815789399</v>
+        <v>0.41881469999999998</v>
       </c>
       <c r="J173">
-        <v>0.527890172631579</v>
+        <v>0.54629289999999997</v>
       </c>
       <c r="K173">
-        <v>0.53990105684210499</v>
+        <v>0.54617249999999995</v>
       </c>
       <c r="L173">
-        <v>0.53859464421052705</v>
+        <v>0.54018129999999998</v>
       </c>
       <c r="M173">
-        <v>0.616638573473684</v>
+        <v>0.64760169999999995</v>
       </c>
       <c r="N173">
-        <v>0.640279733210526</v>
+        <v>0.64035160000000002</v>
       </c>
       <c r="O173">
-        <v>0.63038954131578995</v>
+        <v>0.63050260000000002</v>
       </c>
       <c r="P173">
-        <v>0.68406697515789505</v>
+        <v>0.68416980000000005</v>
       </c>
       <c r="Q173">
-        <v>0.71854641852631596</v>
+        <v>0.71854560000000001</v>
       </c>
       <c r="R173">
-        <v>0.65857719421052596</v>
+        <v>0.66003129999999999</v>
       </c>
       <c r="S173">
-        <v>0.60016720499999998</v>
+        <v>0.6048694</v>
       </c>
       <c r="T173">
-        <v>0.78198985915789498</v>
+        <v>0.79898380000000002</v>
       </c>
       <c r="U173">
-        <v>0.78198985915789498</v>
+        <v>0.79898380000000002</v>
       </c>
       <c r="V173">
-        <v>0.78198985915789498</v>
+        <v>0.79898380000000002</v>
       </c>
       <c r="W173">
-        <v>0.78198985915789498</v>
+        <v>0.79898380000000002</v>
       </c>
       <c r="X173">
-        <v>0.78198985915789498</v>
+        <v>0.79898380000000002</v>
       </c>
       <c r="Y173">
-        <v>0.78198985915789498</v>
+        <v>0.79898380000000002</v>
       </c>
     </row>
     <row r="174" spans="1:25" x14ac:dyDescent="0.2">
@@ -17376,64 +17376,64 @@
         <v>2000</v>
       </c>
       <c r="F174">
-        <v>1.8794979789473699E-3</v>
+        <v>7.5188670000000003E-3</v>
       </c>
       <c r="G174">
-        <v>4.1796253263157897E-2</v>
+        <v>0.1185476</v>
       </c>
       <c r="H174">
-        <v>0.260520086105263</v>
+        <v>0.40749980000000002</v>
       </c>
       <c r="I174">
-        <v>0.46348215157894701</v>
+        <v>0.52735140000000003</v>
       </c>
       <c r="J174">
-        <v>0.61840515621052605</v>
+        <v>0.63996330000000001</v>
       </c>
       <c r="K174">
-        <v>0.75388484463157801</v>
+        <v>0.76264189999999998</v>
       </c>
       <c r="L174">
-        <v>0.74968309263157995</v>
+        <v>0.75189159999999999</v>
       </c>
       <c r="M174">
-        <v>0.73175783494736801</v>
+        <v>0.76850149999999995</v>
       </c>
       <c r="N174">
-        <v>0.90208536821052598</v>
+        <v>0.90218659999999995</v>
       </c>
       <c r="O174">
-        <v>0.86176759926315805</v>
+        <v>0.86192219999999997</v>
       </c>
       <c r="P174">
-        <v>0.86636867636842096</v>
+        <v>0.86649889999999996</v>
       </c>
       <c r="Q174">
-        <v>0.94343289489473703</v>
+        <v>0.94343180000000004</v>
       </c>
       <c r="R174">
-        <v>0.94488589726315797</v>
+        <v>0.94697220000000004</v>
       </c>
       <c r="S174">
-        <v>0.86833563300000005</v>
+        <v>0.87513879999999999</v>
       </c>
       <c r="T174">
-        <v>0.830778558578947</v>
+        <v>0.8488327</v>
       </c>
       <c r="U174">
-        <v>0.830778558578947</v>
+        <v>0.8488327</v>
       </c>
       <c r="V174">
-        <v>0.830778558578947</v>
+        <v>0.8488327</v>
       </c>
       <c r="W174">
-        <v>0.830778558578947</v>
+        <v>0.8488327</v>
       </c>
       <c r="X174">
-        <v>0.830778558578947</v>
+        <v>0.8488327</v>
       </c>
       <c r="Y174">
-        <v>0.830778558578947</v>
+        <v>0.8488327</v>
       </c>
     </row>
     <row r="175" spans="1:25" x14ac:dyDescent="0.2">
@@ -17453,64 +17453,64 @@
         <v>2001</v>
       </c>
       <c r="F175">
-        <v>2.0401405894736801E-3</v>
+        <v>8.1615130000000004E-3</v>
       </c>
       <c r="G175">
-        <v>4.2166307578947397E-2</v>
+        <v>0.11959719000000001</v>
       </c>
       <c r="H175">
-        <v>0.24844530557894701</v>
+        <v>0.38861269999999998</v>
       </c>
       <c r="I175">
-        <v>0.53676602157894704</v>
+        <v>0.610734</v>
       </c>
       <c r="J175">
-        <v>0.62206066863157905</v>
+        <v>0.64374620000000005</v>
       </c>
       <c r="K175">
-        <v>0.705530887578947</v>
+        <v>0.71372619999999998</v>
       </c>
       <c r="L175">
-        <v>0.83627664652631595</v>
+        <v>0.83874020000000005</v>
       </c>
       <c r="M175">
-        <v>0.81370029642105202</v>
+        <v>0.8545585</v>
       </c>
       <c r="N175">
-        <v>0.85519615973684204</v>
+        <v>0.8552921</v>
       </c>
       <c r="O175">
-        <v>0.96995033100000005</v>
+        <v>0.9701244</v>
       </c>
       <c r="P175">
-        <v>0.94616155800000001</v>
+        <v>0.94630380000000003</v>
       </c>
       <c r="Q175">
-        <v>0.95454534315789497</v>
+        <v>0.95454419999999995</v>
       </c>
       <c r="R175">
-        <v>0.99109879947368396</v>
+        <v>0.99328709999999998</v>
       </c>
       <c r="S175">
-        <v>0.99527194799999996</v>
+        <v>1.0030697</v>
       </c>
       <c r="T175">
-        <v>0.96024499568420996</v>
+        <v>0.98111269999999995</v>
       </c>
       <c r="U175">
-        <v>0.96024499568420996</v>
+        <v>0.98111269999999995</v>
       </c>
       <c r="V175">
-        <v>0.96024499568420996</v>
+        <v>0.98111269999999995</v>
       </c>
       <c r="W175">
-        <v>0.96024499568420996</v>
+        <v>0.98111269999999995</v>
       </c>
       <c r="X175">
-        <v>0.96024499568420996</v>
+        <v>0.98111269999999995</v>
       </c>
       <c r="Y175">
-        <v>0.96024499568420996</v>
+        <v>0.98111269999999995</v>
       </c>
     </row>
     <row r="176" spans="1:25" x14ac:dyDescent="0.2">
@@ -17530,64 +17530,64 @@
         <v>2002</v>
       </c>
       <c r="F176">
-        <v>2.17160216842105E-3</v>
+        <v>8.6874199999999995E-3</v>
       </c>
       <c r="G176">
-        <v>4.5099632000000098E-2</v>
+        <v>0.12791704000000001</v>
       </c>
       <c r="H176">
-        <v>0.24697231</v>
+        <v>0.3863086</v>
       </c>
       <c r="I176">
-        <v>0.50438701789473595</v>
+        <v>0.57389310000000004</v>
       </c>
       <c r="J176">
-        <v>0.70986207031578996</v>
+        <v>0.7346085</v>
       </c>
       <c r="K176">
-        <v>0.69930215242105198</v>
+        <v>0.70742519999999998</v>
       </c>
       <c r="L176">
-        <v>0.77117013831578995</v>
+        <v>0.77344190000000002</v>
       </c>
       <c r="M176">
-        <v>0.894388101052631</v>
+        <v>0.93929790000000002</v>
       </c>
       <c r="N176">
-        <v>0.937026968210526</v>
+        <v>0.93713210000000002</v>
       </c>
       <c r="O176">
-        <v>0.90605977531578996</v>
+        <v>0.90622230000000004</v>
       </c>
       <c r="P176">
-        <v>1.0493343279473699</v>
+        <v>1.0494920000000001</v>
       </c>
       <c r="Q176">
-        <v>1.0271841920526299</v>
+        <v>1.027183</v>
       </c>
       <c r="R176">
-        <v>0.988079165368421</v>
+        <v>0.99026080000000005</v>
       </c>
       <c r="S176">
-        <v>1.0286522730000001</v>
+        <v>1.0367115</v>
       </c>
       <c r="T176">
-        <v>1.0844896721578901</v>
+        <v>1.1080574000000001</v>
       </c>
       <c r="U176">
-        <v>1.0844896721578901</v>
+        <v>1.1080574000000001</v>
       </c>
       <c r="V176">
-        <v>1.0844896721578901</v>
+        <v>1.1080574000000001</v>
       </c>
       <c r="W176">
-        <v>1.0844896721578901</v>
+        <v>1.1080574000000001</v>
       </c>
       <c r="X176">
-        <v>1.0844896721578901</v>
+        <v>1.1080574000000001</v>
       </c>
       <c r="Y176">
-        <v>1.0844896721578901</v>
+        <v>1.1080574000000001</v>
       </c>
     </row>
     <row r="177" spans="1:25" x14ac:dyDescent="0.2">
@@ -17607,64 +17607,64 @@
         <v>2003</v>
       </c>
       <c r="F177">
-        <v>1.94888308421053E-3</v>
+        <v>7.79644E-3</v>
       </c>
       <c r="G177">
-        <v>4.1992904947368501E-2</v>
+        <v>0.11910537</v>
       </c>
       <c r="H177">
-        <v>0.231067300105263</v>
+        <v>0.36143039999999999</v>
       </c>
       <c r="I177">
-        <v>0.43859545052631499</v>
+        <v>0.49903520000000001</v>
       </c>
       <c r="J177">
-        <v>0.58349293852631601</v>
+        <v>0.60383399999999998</v>
       </c>
       <c r="K177">
-        <v>0.69805372547368305</v>
+        <v>0.70616219999999996</v>
       </c>
       <c r="L177">
-        <v>0.66862373831579003</v>
+        <v>0.67059340000000001</v>
       </c>
       <c r="M177">
-        <v>0.72145451873684197</v>
+        <v>0.75768080000000004</v>
       </c>
       <c r="N177">
-        <v>0.90094107078947405</v>
+        <v>0.90104209999999996</v>
       </c>
       <c r="O177">
-        <v>0.86841220026315802</v>
+        <v>0.86856800000000001</v>
       </c>
       <c r="P177">
-        <v>0.85744047789473699</v>
+        <v>0.85756929999999998</v>
       </c>
       <c r="Q177">
-        <v>0.99650544726315804</v>
+        <v>0.99650430000000001</v>
       </c>
       <c r="R177">
-        <v>0.93009276042105204</v>
+        <v>0.93214640000000004</v>
       </c>
       <c r="S177">
-        <v>0.89706949199999997</v>
+        <v>0.90409779999999995</v>
       </c>
       <c r="T177">
-        <v>0.98047149268420997</v>
+        <v>1.0017787</v>
       </c>
       <c r="U177">
-        <v>0.98047149268420997</v>
+        <v>1.0017787</v>
       </c>
       <c r="V177">
-        <v>0.98047149268420997</v>
+        <v>1.0017787</v>
       </c>
       <c r="W177">
-        <v>0.98047149268420997</v>
+        <v>1.0017787</v>
       </c>
       <c r="X177">
-        <v>0.98047149268420997</v>
+        <v>1.0017787</v>
       </c>
       <c r="Y177">
-        <v>0.98047149268420997</v>
+        <v>1.0017787</v>
       </c>
     </row>
     <row r="178" spans="1:25" x14ac:dyDescent="0.2">
@@ -17684,64 +17684,64 @@
         <v>2004</v>
       </c>
       <c r="F178">
-        <v>1.86415610526316E-3</v>
+        <v>7.4574929999999999E-3</v>
       </c>
       <c r="G178">
-        <v>3.8838231894736903E-2</v>
+        <v>0.1101577</v>
       </c>
       <c r="H178">
-        <v>0.221727409052631</v>
+        <v>0.34682109999999999</v>
       </c>
       <c r="I178">
-        <v>0.42289477421052601</v>
+        <v>0.48117100000000002</v>
       </c>
       <c r="J178">
-        <v>0.52289416547368395</v>
+        <v>0.54112269999999996</v>
       </c>
       <c r="K178">
-        <v>0.59132804968421004</v>
+        <v>0.59819679999999997</v>
       </c>
       <c r="L178">
-        <v>0.68783421010526402</v>
+        <v>0.68986049999999999</v>
       </c>
       <c r="M178">
-        <v>0.64464192421052602</v>
+        <v>0.67701120000000004</v>
       </c>
       <c r="N178">
-        <v>0.74895770415789498</v>
+        <v>0.74904170000000003</v>
       </c>
       <c r="O178">
-        <v>0.86049466957894805</v>
+        <v>0.86064909999999994</v>
       </c>
       <c r="P178">
-        <v>0.84693690899999996</v>
+        <v>0.84706420000000004</v>
       </c>
       <c r="Q178">
-        <v>0.83916570126315804</v>
+        <v>0.83916469999999999</v>
       </c>
       <c r="R178">
-        <v>0.92989857557894695</v>
+        <v>0.9319518</v>
       </c>
       <c r="S178">
-        <v>0.87023920499999996</v>
+        <v>0.87705730000000004</v>
       </c>
       <c r="T178">
-        <v>0.88119193752631597</v>
+        <v>0.90034170000000002</v>
       </c>
       <c r="U178">
-        <v>0.88119193752631597</v>
+        <v>0.90034170000000002</v>
       </c>
       <c r="V178">
-        <v>0.88119193752631597</v>
+        <v>0.90034170000000002</v>
       </c>
       <c r="W178">
-        <v>0.88119193752631597</v>
+        <v>0.90034170000000002</v>
       </c>
       <c r="X178">
-        <v>0.88119193752631597</v>
+        <v>0.90034170000000002</v>
       </c>
       <c r="Y178">
-        <v>0.88119193752631597</v>
+        <v>0.90034170000000002</v>
       </c>
     </row>
     <row r="179" spans="1:25" x14ac:dyDescent="0.2">
@@ -17761,64 +17761,64 @@
         <v>2005</v>
       </c>
       <c r="F179">
-        <v>1.7212461315789501E-3</v>
+        <v>6.8857859999999996E-3</v>
       </c>
       <c r="G179">
-        <v>3.9603506315789502E-2</v>
+        <v>0.11232826999999999</v>
       </c>
       <c r="H179">
-        <v>0.218615274</v>
+        <v>0.34195320000000001</v>
       </c>
       <c r="I179">
-        <v>0.43260421078947298</v>
+        <v>0.4922184</v>
       </c>
       <c r="J179">
-        <v>0.53747664547368401</v>
+        <v>0.55621350000000003</v>
       </c>
       <c r="K179">
-        <v>0.56491649431578905</v>
+        <v>0.5714785</v>
       </c>
       <c r="L179">
-        <v>0.62115634610526405</v>
+        <v>0.62298620000000005</v>
       </c>
       <c r="M179">
-        <v>0.70696530189473605</v>
+        <v>0.74246400000000001</v>
       </c>
       <c r="N179">
-        <v>0.71341871873684204</v>
+        <v>0.71349870000000004</v>
       </c>
       <c r="O179">
-        <v>0.76258232952631599</v>
+        <v>0.76271909999999998</v>
       </c>
       <c r="P179">
-        <v>0.89464528610526295</v>
+        <v>0.89477969999999996</v>
       </c>
       <c r="Q179">
-        <v>0.88363398457894804</v>
+        <v>0.883633</v>
       </c>
       <c r="R179">
-        <v>0.834797745368421</v>
+        <v>0.83664090000000002</v>
       </c>
       <c r="S179">
-        <v>0.92752486199999995</v>
+        <v>0.93479179999999995</v>
       </c>
       <c r="T179">
-        <v>0.91129842636842096</v>
+        <v>0.9311024</v>
       </c>
       <c r="U179">
-        <v>0.91129842636842096</v>
+        <v>0.9311024</v>
       </c>
       <c r="V179">
-        <v>0.91129842636842096</v>
+        <v>0.9311024</v>
       </c>
       <c r="W179">
-        <v>0.91129842636842096</v>
+        <v>0.9311024</v>
       </c>
       <c r="X179">
-        <v>0.91129842636842096</v>
+        <v>0.9311024</v>
       </c>
       <c r="Y179">
-        <v>0.91129842636842096</v>
+        <v>0.9311024</v>
       </c>
     </row>
     <row r="180" spans="1:25" x14ac:dyDescent="0.2">
@@ -17838,64 +17838,64 @@
         <v>2006</v>
       </c>
       <c r="F180">
-        <v>1.54031842105263E-3</v>
+        <v>6.1619910000000003E-3</v>
       </c>
       <c r="G180">
-        <v>3.7841377052631603E-2</v>
+        <v>0.1073303</v>
       </c>
       <c r="H180">
-        <v>0.230689183052631</v>
+        <v>0.36083890000000002</v>
       </c>
       <c r="I180">
-        <v>0.44139207315789403</v>
+        <v>0.50221720000000003</v>
       </c>
       <c r="J180">
-        <v>0.56897172463157897</v>
+        <v>0.58880659999999996</v>
       </c>
       <c r="K180">
-        <v>0.60090066947368403</v>
+        <v>0.60788070000000005</v>
       </c>
       <c r="L180">
-        <v>0.61408634042105303</v>
+        <v>0.61589539999999998</v>
       </c>
       <c r="M180">
-        <v>0.66067517305263102</v>
+        <v>0.69384950000000001</v>
       </c>
       <c r="N180">
-        <v>0.80964884463157905</v>
+        <v>0.80973969999999995</v>
       </c>
       <c r="O180">
-        <v>0.75170345826315799</v>
+        <v>0.75183829999999996</v>
       </c>
       <c r="P180">
-        <v>0.82046884689473698</v>
+        <v>0.82059210000000005</v>
       </c>
       <c r="Q180">
-        <v>0.96592834894736901</v>
+        <v>0.96592719999999999</v>
       </c>
       <c r="R180">
-        <v>0.90965899252631499</v>
+        <v>0.91166749999999996</v>
       </c>
       <c r="S180">
-        <v>0.86167570500000001</v>
+        <v>0.8684267</v>
       </c>
       <c r="T180">
-        <v>1.0051252486842099</v>
+        <v>1.0269682</v>
       </c>
       <c r="U180">
-        <v>1.0051252486842099</v>
+        <v>1.0269682</v>
       </c>
       <c r="V180">
-        <v>1.0051252486842099</v>
+        <v>1.0269682</v>
       </c>
       <c r="W180">
-        <v>1.0051252486842099</v>
+        <v>1.0269682</v>
       </c>
       <c r="X180">
-        <v>1.0051252486842099</v>
+        <v>1.0269682</v>
       </c>
       <c r="Y180">
-        <v>1.0051252486842099</v>
+        <v>1.0269682</v>
       </c>
     </row>
     <row r="181" spans="1:25" x14ac:dyDescent="0.2">
@@ -17915,64 +17915,64 @@
         <v>2007</v>
       </c>
       <c r="F181">
-        <v>1.27272784736842E-3</v>
+        <v>5.0915040000000002E-3</v>
       </c>
       <c r="G181">
-        <v>3.1375823789473699E-2</v>
+        <v>8.8991920000000002E-2</v>
       </c>
       <c r="H181">
-        <v>0.20423083189473701</v>
+        <v>0.3194534</v>
       </c>
       <c r="I181">
-        <v>0.431550839210526</v>
+        <v>0.49101990000000001</v>
       </c>
       <c r="J181">
-        <v>0.53787960631579002</v>
+        <v>0.55663050000000003</v>
       </c>
       <c r="K181">
-        <v>0.58937880505263096</v>
+        <v>0.596225</v>
       </c>
       <c r="L181">
-        <v>0.60521335831579004</v>
+        <v>0.60699630000000004</v>
       </c>
       <c r="M181">
-        <v>0.60516957305263097</v>
+        <v>0.63555680000000003</v>
       </c>
       <c r="N181">
-        <v>0.70104713352631598</v>
+        <v>0.70112580000000002</v>
       </c>
       <c r="O181">
-        <v>0.79042276894736896</v>
+        <v>0.79056459999999995</v>
       </c>
       <c r="P181">
-        <v>0.74934629952631604</v>
+        <v>0.74945890000000004</v>
       </c>
       <c r="Q181">
-        <v>0.820761093</v>
+        <v>0.82076020000000005</v>
       </c>
       <c r="R181">
-        <v>0.92132264326315705</v>
+        <v>0.92335690000000004</v>
       </c>
       <c r="S181">
-        <v>0.86996517299999998</v>
+        <v>0.87678120000000004</v>
       </c>
       <c r="T181">
-        <v>0.865165421315789</v>
+        <v>0.8839669</v>
       </c>
       <c r="U181">
-        <v>0.865165421315789</v>
+        <v>0.8839669</v>
       </c>
       <c r="V181">
-        <v>0.865165421315789</v>
+        <v>0.8839669</v>
       </c>
       <c r="W181">
-        <v>0.865165421315789</v>
+        <v>0.8839669</v>
       </c>
       <c r="X181">
-        <v>0.865165421315789</v>
+        <v>0.8839669</v>
       </c>
       <c r="Y181">
-        <v>0.865165421315789</v>
+        <v>0.8839669</v>
       </c>
     </row>
     <row r="182" spans="1:25" x14ac:dyDescent="0.2">
@@ -17992,64 +17992,64 @@
         <v>2008</v>
       </c>
       <c r="F182">
-        <v>1.3908608999999999E-3</v>
+        <v>5.5640910000000002E-3</v>
       </c>
       <c r="G182">
-        <v>3.12846477894737E-2</v>
+        <v>8.8733309999999996E-2</v>
       </c>
       <c r="H182">
-        <v>0.20434340578947399</v>
+        <v>0.31962940000000001</v>
       </c>
       <c r="I182">
-        <v>0.46103844368420999</v>
+        <v>0.52457089999999995</v>
       </c>
       <c r="J182">
-        <v>0.63460540547368505</v>
+        <v>0.65672830000000004</v>
       </c>
       <c r="K182">
-        <v>0.67235727410526203</v>
+        <v>0.68016730000000003</v>
       </c>
       <c r="L182">
-        <v>0.71632733178947405</v>
+        <v>0.71843760000000001</v>
       </c>
       <c r="M182">
-        <v>0.71972626105263104</v>
+        <v>0.75586580000000003</v>
       </c>
       <c r="N182">
-        <v>0.77490334136842098</v>
+        <v>0.77499030000000002</v>
       </c>
       <c r="O182">
-        <v>0.82588799321052697</v>
+        <v>0.8260362</v>
       </c>
       <c r="P182">
-        <v>0.950838295263158</v>
+        <v>0.95098119999999997</v>
       </c>
       <c r="Q182">
-        <v>0.90458305294736896</v>
+        <v>0.904582</v>
       </c>
       <c r="R182">
-        <v>0.94470188021052603</v>
+        <v>0.94678770000000001</v>
       </c>
       <c r="S182">
-        <v>1.063276533</v>
+        <v>1.0716071</v>
       </c>
       <c r="T182">
-        <v>1.0540673463157899</v>
+        <v>1.0769739</v>
       </c>
       <c r="U182">
-        <v>1.0540673463157899</v>
+        <v>1.0769739</v>
       </c>
       <c r="V182">
-        <v>1.0540673463157899</v>
+        <v>1.0769739</v>
       </c>
       <c r="W182">
-        <v>1.0540673463157899</v>
+        <v>1.0769739</v>
       </c>
       <c r="X182">
-        <v>1.0540673463157899</v>
+        <v>1.0769739</v>
       </c>
       <c r="Y182">
-        <v>1.0540673463157899</v>
+        <v>1.0769739</v>
       </c>
     </row>
     <row r="183" spans="1:25" x14ac:dyDescent="0.2">
@@ -18069,64 +18069,64 @@
         <v>2009</v>
       </c>
       <c r="F183">
-        <v>7.6919680000000004E-4</v>
+        <v>3.8785540000000002E-3</v>
       </c>
       <c r="G183">
-        <v>2.1458270000000002E-2</v>
+        <v>7.0524950000000003E-2</v>
       </c>
       <c r="H183">
-        <v>0.15135859199999999</v>
+        <v>0.26735789999999998</v>
       </c>
       <c r="I183">
-        <v>0.38522757600000002</v>
+        <v>0.45206170000000001</v>
       </c>
       <c r="J183">
-        <v>0.58322105499999999</v>
+        <v>0.60650190000000004</v>
       </c>
       <c r="K183">
-        <v>0.68289732000000003</v>
+        <v>0.69425440000000005</v>
       </c>
       <c r="L183">
-        <v>0.70314938100000002</v>
+        <v>0.7092157</v>
       </c>
       <c r="M183">
-        <v>0.77479779999999998</v>
+        <v>0.77422230000000003</v>
       </c>
       <c r="N183">
-        <v>0.79804850000000005</v>
+        <v>0.79765830000000004</v>
       </c>
       <c r="O183">
-        <v>0.79052020000000001</v>
+        <v>0.79019099999999998</v>
       </c>
       <c r="P183">
-        <v>0.86031970000000002</v>
+        <v>0.85992500000000005</v>
       </c>
       <c r="Q183">
-        <v>0.99394879999999997</v>
+        <v>0.99329880000000004</v>
       </c>
       <c r="R183">
-        <v>0.89494871399999998</v>
+        <v>0.90289900000000001</v>
       </c>
       <c r="S183">
-        <v>0.94360909500000001</v>
+        <v>0.95040380000000002</v>
       </c>
       <c r="T183">
-        <v>1.1011171200000001</v>
+        <v>1.1368906999999999</v>
       </c>
       <c r="U183">
-        <v>1.1011171200000001</v>
+        <v>1.1368906999999999</v>
       </c>
       <c r="V183">
-        <v>1.1011171200000001</v>
+        <v>1.1368906999999999</v>
       </c>
       <c r="W183">
-        <v>1.1011171200000001</v>
+        <v>1.1368906999999999</v>
       </c>
       <c r="X183">
-        <v>1.1011171200000001</v>
+        <v>1.1368906999999999</v>
       </c>
       <c r="Y183">
-        <v>1.1011171200000001</v>
+        <v>1.1368906999999999</v>
       </c>
     </row>
     <row r="184" spans="1:25" x14ac:dyDescent="0.2">
@@ -18146,64 +18146,64 @@
         <v>2010</v>
       </c>
       <c r="F184">
-        <v>2.6063843999999999E-3</v>
+        <v>1.0298441E-2</v>
       </c>
       <c r="G184">
-        <v>4.9060022000000002E-2</v>
+        <v>0.12302265</v>
       </c>
       <c r="H184">
-        <v>0.23233016400000001</v>
+        <v>0.3157394</v>
       </c>
       <c r="I184">
-        <v>0.40408158700000002</v>
+        <v>0.4349073</v>
       </c>
       <c r="J184">
-        <v>0.56368188799999996</v>
+        <v>0.57234039999999997</v>
       </c>
       <c r="K184">
-        <v>0.690126723</v>
+        <v>0.69603870000000001</v>
       </c>
       <c r="L184">
-        <v>0.78467560000000003</v>
+        <v>0.78420319999999999</v>
       </c>
       <c r="M184">
-        <v>0.82766220000000001</v>
+        <v>0.82740689999999995</v>
       </c>
       <c r="N184">
-        <v>0.88448689999999996</v>
+        <v>0.88430609999999998</v>
       </c>
       <c r="O184">
-        <v>0.88036409999999998</v>
+        <v>0.88020989999999999</v>
       </c>
       <c r="P184">
-        <v>0.89046990000000004</v>
+        <v>0.89029700000000001</v>
       </c>
       <c r="Q184">
-        <v>0.9724893</v>
+        <v>0.97221840000000004</v>
       </c>
       <c r="R184">
-        <v>1.0741035000000001</v>
+        <v>1.0735486000000001</v>
       </c>
       <c r="S184">
-        <v>0.97382943899999996</v>
+        <v>0.98244719999999996</v>
       </c>
       <c r="T184">
-        <v>1.0792709620000001</v>
+        <v>1.0970707</v>
       </c>
       <c r="U184">
-        <v>1.0792709620000001</v>
+        <v>1.0970707</v>
       </c>
       <c r="V184">
-        <v>1.0792709620000001</v>
+        <v>1.0970707</v>
       </c>
       <c r="W184">
-        <v>1.0792709620000001</v>
+        <v>1.0970707</v>
       </c>
       <c r="X184">
-        <v>1.0792709620000001</v>
+        <v>1.0970707</v>
       </c>
       <c r="Y184">
-        <v>1.0792709620000001</v>
+        <v>1.0970707</v>
       </c>
     </row>
     <row r="185" spans="1:25" x14ac:dyDescent="0.2">
@@ -18223,64 +18223,64 @@
         <v>2011</v>
       </c>
       <c r="F185">
-        <v>8.2272669999999999E-4</v>
+        <v>3.2506409999999999E-3</v>
       </c>
       <c r="G185">
-        <v>1.8579792000000001E-2</v>
+        <v>6.4705410000000005E-2</v>
       </c>
       <c r="H185">
-        <v>0.131553591</v>
+        <v>0.2486226</v>
       </c>
       <c r="I185">
-        <v>0.32681017200000001</v>
+        <v>0.39394200000000001</v>
       </c>
       <c r="J185">
-        <v>0.46547596800000002</v>
+        <v>0.48803469999999999</v>
       </c>
       <c r="K185">
-        <v>0.59017971599999997</v>
+        <v>0.59960389999999997</v>
       </c>
       <c r="L185">
-        <v>0.71656516800000003</v>
+        <v>0.72258529999999999</v>
       </c>
       <c r="M185">
-        <v>0.84313450000000001</v>
+        <v>0.84242609999999996</v>
       </c>
       <c r="N185">
-        <v>0.8712086</v>
+        <v>0.87073610000000001</v>
       </c>
       <c r="O185">
-        <v>0.89968499999999996</v>
+        <v>0.89927760000000001</v>
       </c>
       <c r="P185">
-        <v>0.91439680000000001</v>
+        <v>0.91394980000000003</v>
       </c>
       <c r="Q185">
-        <v>0.92813319999999999</v>
+        <v>0.92749959999999998</v>
       </c>
       <c r="R185">
-        <v>0.95933039399999998</v>
+        <v>0.96782619999999997</v>
       </c>
       <c r="S185">
-        <v>1.066920723</v>
+        <v>1.0745988</v>
       </c>
       <c r="T185">
-        <v>1.0060800000000001</v>
+        <v>1.0389438</v>
       </c>
       <c r="U185">
-        <v>1.0060800000000001</v>
+        <v>1.0389438</v>
       </c>
       <c r="V185">
-        <v>1.0060800000000001</v>
+        <v>1.0389438</v>
       </c>
       <c r="W185">
-        <v>1.0060800000000001</v>
+        <v>1.0389438</v>
       </c>
       <c r="X185">
-        <v>1.0060800000000001</v>
+        <v>1.0389438</v>
       </c>
       <c r="Y185">
-        <v>1.0060800000000001</v>
+        <v>1.0389438</v>
       </c>
     </row>
     <row r="186" spans="1:25" x14ac:dyDescent="0.2">
@@ -18300,64 +18300,64 @@
         <v>2012</v>
       </c>
       <c r="F186">
-        <v>9.2730380000000004E-4</v>
+        <v>2.6911610000000001E-3</v>
       </c>
       <c r="G186">
-        <v>1.3662911999999999E-2</v>
+        <v>4.9674410000000002E-2</v>
       </c>
       <c r="H186">
-        <v>0.112758284</v>
+        <v>0.243142</v>
       </c>
       <c r="I186">
-        <v>0.29930414399999999</v>
+        <v>0.3818454</v>
       </c>
       <c r="J186">
-        <v>0.44507530000000001</v>
+        <v>0.47407179999999999</v>
       </c>
       <c r="K186">
-        <v>0.52070793100000001</v>
+        <v>0.53355390000000003</v>
       </c>
       <c r="L186">
-        <v>0.64094847300000002</v>
+        <v>0.6459028</v>
       </c>
       <c r="M186">
-        <v>7.2472401000000006E-2</v>
+        <v>0.80430690000000005</v>
       </c>
       <c r="N186">
-        <v>0.91890130000000003</v>
+        <v>0.91820979999999996</v>
       </c>
       <c r="O186">
-        <v>0.91753819999999997</v>
+        <v>0.91696460000000002</v>
       </c>
       <c r="P186">
-        <v>0.96753290000000003</v>
+        <v>0.96688399999999997</v>
       </c>
       <c r="Q186">
-        <v>0.98679879999999998</v>
+        <v>0.98588180000000003</v>
       </c>
       <c r="R186">
-        <v>0.94797430199999999</v>
+        <v>0.95595790000000003</v>
       </c>
       <c r="S186">
-        <v>0.98653561999999995</v>
+        <v>1.002807</v>
       </c>
       <c r="T186">
-        <v>1.12937197</v>
+        <v>1.1752904</v>
       </c>
       <c r="U186">
-        <v>1.12937197</v>
+        <v>1.1752904</v>
       </c>
       <c r="V186">
-        <v>1.12937197</v>
+        <v>1.1752904</v>
       </c>
       <c r="W186">
-        <v>1.12937197</v>
+        <v>1.1752904</v>
       </c>
       <c r="X186">
-        <v>1.12937197</v>
+        <v>1.1752904</v>
       </c>
       <c r="Y186">
-        <v>1.12937197</v>
+        <v>1.1752904</v>
       </c>
     </row>
     <row r="187" spans="1:25" x14ac:dyDescent="0.2">
@@ -18377,64 +18377,64 @@
         <v>2013</v>
       </c>
       <c r="F187">
-        <v>1.0471896E-3</v>
+        <v>4.1869860000000002E-3</v>
       </c>
       <c r="G187">
-        <v>2.1698783999999999E-2</v>
+        <v>7.6274939999999999E-2</v>
       </c>
       <c r="H187">
-        <v>0.146987217</v>
+        <v>0.2789605</v>
       </c>
       <c r="I187">
-        <v>0.36949668600000002</v>
+        <v>0.44597179999999997</v>
       </c>
       <c r="J187">
-        <v>0.47680381399999999</v>
+        <v>0.50012570000000001</v>
       </c>
       <c r="K187">
-        <v>0.543139912</v>
+        <v>0.55190939999999999</v>
       </c>
       <c r="L187">
-        <v>0.60377397300000002</v>
+        <v>0.60890080000000002</v>
       </c>
       <c r="M187">
-        <v>0.76117500000000005</v>
+        <v>0.76057889999999995</v>
       </c>
       <c r="N187">
-        <v>0.92744689999999996</v>
+        <v>0.92698670000000005</v>
       </c>
       <c r="O187">
-        <v>1.0227223999999999</v>
+        <v>1.0223077</v>
       </c>
       <c r="P187">
-        <v>1.0427648</v>
+        <v>1.042319</v>
       </c>
       <c r="Q187">
-        <v>1.1034347</v>
+        <v>1.1027929999999999</v>
       </c>
       <c r="R187">
-        <v>1.075887</v>
+        <v>1.0747894</v>
       </c>
       <c r="S187">
-        <v>1.040727897</v>
+        <v>1.0488150000000001</v>
       </c>
       <c r="T187">
-        <v>1.1383133329999999</v>
+        <v>1.1656446</v>
       </c>
       <c r="U187">
-        <v>1.1383133329999999</v>
+        <v>1.1656446</v>
       </c>
       <c r="V187">
-        <v>1.1383133329999999</v>
+        <v>1.1656446</v>
       </c>
       <c r="W187">
-        <v>1.1383133329999999</v>
+        <v>1.1656446</v>
       </c>
       <c r="X187">
-        <v>1.1383133329999999</v>
+        <v>1.1656446</v>
       </c>
       <c r="Y187">
-        <v>1.1383133329999999</v>
+        <v>1.1656446</v>
       </c>
     </row>
     <row r="188" spans="1:25" x14ac:dyDescent="0.2">
@@ -18454,64 +18454,64 @@
         <v>2014</v>
       </c>
       <c r="F188">
-        <v>2.1849365999999999E-3</v>
+        <v>1.0199866E-2</v>
       </c>
       <c r="G188">
-        <v>5.5906272E-2</v>
+        <v>0.15257232000000001</v>
       </c>
       <c r="H188">
-        <v>0.27767541600000001</v>
+        <v>0.39839160000000001</v>
       </c>
       <c r="I188">
-        <v>0.44794629000000002</v>
+        <v>0.48541250000000002</v>
       </c>
       <c r="J188">
-        <v>0.56853678799999996</v>
+        <v>0.58273010000000003</v>
       </c>
       <c r="K188">
-        <v>0.58334621399999997</v>
+        <v>0.58822470000000004</v>
       </c>
       <c r="L188">
-        <v>0.63847160000000003</v>
+        <v>0.63805089999999998</v>
       </c>
       <c r="M188">
-        <v>0.72706800000000005</v>
+        <v>0.72683140000000002</v>
       </c>
       <c r="N188">
-        <v>0.888961</v>
+        <v>0.88877649999999997</v>
       </c>
       <c r="O188">
-        <v>1.0466880000000001</v>
+        <v>1.0465092</v>
       </c>
       <c r="P188">
-        <v>1.1785805</v>
+        <v>1.1783665999999999</v>
       </c>
       <c r="Q188">
-        <v>1.2058867</v>
+        <v>1.2055864999999999</v>
       </c>
       <c r="R188">
-        <v>1.2198992</v>
+        <v>1.2193613999999999</v>
       </c>
       <c r="S188">
-        <v>1.1976959</v>
+        <v>1.1964895</v>
       </c>
       <c r="T188">
-        <v>1.2302118179999999</v>
+        <v>1.2389507</v>
       </c>
       <c r="U188">
-        <v>1.2302118179999999</v>
+        <v>1.2389507</v>
       </c>
       <c r="V188">
-        <v>1.2302118179999999</v>
+        <v>1.2389507</v>
       </c>
       <c r="W188">
-        <v>1.2302118179999999</v>
+        <v>1.2389507</v>
       </c>
       <c r="X188">
-        <v>1.2302118179999999</v>
+        <v>1.2389507</v>
       </c>
       <c r="Y188">
-        <v>1.2302118179999999</v>
+        <v>1.2389507</v>
       </c>
     </row>
     <row r="189" spans="1:25" x14ac:dyDescent="0.2">
@@ -18531,64 +18531,64 @@
         <v>2015</v>
       </c>
       <c r="F189">
-        <v>2.6566008000000001E-3</v>
+        <v>9.5879759999999998E-3</v>
       </c>
       <c r="G189">
-        <v>4.8363200000000002E-2</v>
+        <v>0.12804359000000001</v>
       </c>
       <c r="H189">
-        <v>0.24896806399999999</v>
+        <v>0.34606239999999999</v>
       </c>
       <c r="I189">
-        <v>0.408254483</v>
+        <v>0.43878309999999998</v>
       </c>
       <c r="J189">
-        <v>0.45039535800000002</v>
+        <v>0.4571847</v>
       </c>
       <c r="K189">
-        <v>0.50305414500000001</v>
+        <v>0.50732739999999998</v>
       </c>
       <c r="L189">
-        <v>0.50659469999999995</v>
+        <v>0.50627820000000001</v>
       </c>
       <c r="M189">
-        <v>0.56805570000000005</v>
+        <v>0.56787529999999997</v>
       </c>
       <c r="N189">
-        <v>0.63370439999999995</v>
+        <v>0.63357200000000002</v>
       </c>
       <c r="O189">
-        <v>0.74872859999999997</v>
+        <v>0.74859540000000002</v>
       </c>
       <c r="P189">
-        <v>0.90018600000000004</v>
+        <v>0.90000939999999996</v>
       </c>
       <c r="Q189">
-        <v>1.0171684999999999</v>
+        <v>1.0168836999999999</v>
       </c>
       <c r="R189">
-        <v>0.99494090000000002</v>
+        <v>0.99442609999999998</v>
       </c>
       <c r="S189">
-        <v>1.0033501499999999</v>
+        <v>1.0122310999999999</v>
       </c>
       <c r="T189">
-        <v>1.0354492820000001</v>
+        <v>1.0525416999999999</v>
       </c>
       <c r="U189">
-        <v>1.0354492820000001</v>
+        <v>1.0525416999999999</v>
       </c>
       <c r="V189">
-        <v>1.0354492820000001</v>
+        <v>1.0525416999999999</v>
       </c>
       <c r="W189">
-        <v>1.0354492820000001</v>
+        <v>1.0525416999999999</v>
       </c>
       <c r="X189">
-        <v>1.0354492820000001</v>
+        <v>1.0525416999999999</v>
       </c>
       <c r="Y189">
-        <v>1.0354492820000001</v>
+        <v>1.0525416999999999</v>
       </c>
     </row>
     <row r="190" spans="1:25" x14ac:dyDescent="0.2">
@@ -18608,64 +18608,64 @@
         <v>2016</v>
       </c>
       <c r="F190">
-        <v>0</v>
+        <v>1.9762349999999998E-3</v>
       </c>
       <c r="G190">
-        <v>9.6841960000000008E-3</v>
+        <v>3.766974E-2</v>
       </c>
       <c r="H190">
-        <v>8.6042057000000005E-2</v>
+        <v>0.21236840000000001</v>
       </c>
       <c r="I190">
-        <v>0.293602364</v>
+        <v>0.41594389999999998</v>
       </c>
       <c r="J190">
-        <v>0.44515933800000002</v>
+        <v>0.49550119999999997</v>
       </c>
       <c r="K190">
-        <v>0.472448064</v>
+        <v>0.48727369999999998</v>
       </c>
       <c r="L190">
-        <v>0.52880721600000002</v>
+        <v>0.53747679999999998</v>
       </c>
       <c r="M190">
-        <v>0.55114695899999999</v>
+        <v>0.55558819999999998</v>
       </c>
       <c r="N190">
-        <v>0.60542459999999998</v>
+        <v>0.61071690000000001</v>
       </c>
       <c r="O190">
-        <v>0.65265829200000003</v>
+        <v>0.65848580000000001</v>
       </c>
       <c r="P190">
-        <v>0.78740263799999999</v>
+        <v>0.79432519999999995</v>
       </c>
       <c r="Q190">
-        <v>0.94999944599999997</v>
+        <v>0.95779530000000002</v>
       </c>
       <c r="R190">
-        <v>1.0158557500000001</v>
+        <v>1.0329444000000001</v>
       </c>
       <c r="S190">
-        <v>0.98013119999999998</v>
+        <v>1.0122861999999999</v>
       </c>
       <c r="T190">
-        <v>0.98284666899999995</v>
+        <v>1.0752451000000001</v>
       </c>
       <c r="U190">
-        <v>0.98284666899999995</v>
+        <v>1.0752451000000001</v>
       </c>
       <c r="V190">
-        <v>0.98284666899999995</v>
+        <v>1.0752451000000001</v>
       </c>
       <c r="W190">
-        <v>0.98284666899999995</v>
+        <v>1.0752451000000001</v>
       </c>
       <c r="X190">
-        <v>0.98284666899999995</v>
+        <v>1.0752451000000001</v>
       </c>
       <c r="Y190">
-        <v>0.98284666899999995</v>
+        <v>1.0752451000000001</v>
       </c>
     </row>
     <row r="191" spans="1:25" x14ac:dyDescent="0.2">
@@ -18685,64 +18685,64 @@
         <v>2017</v>
       </c>
       <c r="F191">
-        <v>2.2601484000000002E-3</v>
+        <v>1.0046115E-2</v>
       </c>
       <c r="G191">
-        <v>5.1402100999999999E-2</v>
+        <v>0.14438635</v>
       </c>
       <c r="H191">
-        <v>0.24598655999999999</v>
+        <v>0.35613489999999998</v>
       </c>
       <c r="I191">
-        <v>0.44364533099999998</v>
+        <v>0.48535430000000002</v>
       </c>
       <c r="J191">
-        <v>0.57346254500000005</v>
+        <v>0.58752110000000002</v>
       </c>
       <c r="K191">
-        <v>0.593752104</v>
+        <v>0.59862700000000002</v>
       </c>
       <c r="L191">
-        <v>0.57204909999999998</v>
+        <v>0.57163339999999996</v>
       </c>
       <c r="M191">
-        <v>0.64908520000000003</v>
+        <v>0.64884830000000004</v>
       </c>
       <c r="N191">
-        <v>0.6560319</v>
+        <v>0.65587640000000003</v>
       </c>
       <c r="O191">
-        <v>0.6963821</v>
+        <v>0.69624330000000001</v>
       </c>
       <c r="P191">
-        <v>0.76656089999999999</v>
+        <v>0.76639460000000004</v>
       </c>
       <c r="Q191">
-        <v>0.92806060000000001</v>
+        <v>0.92777690000000002</v>
       </c>
       <c r="R191">
-        <v>1.0704342</v>
+        <v>1.0698377999999999</v>
       </c>
       <c r="S191">
-        <v>1.1526980849999999</v>
+        <v>1.1628118000000001</v>
       </c>
       <c r="T191">
-        <v>1.1933731460000001</v>
+        <v>1.2128540000000001</v>
       </c>
       <c r="U191">
-        <v>1.1933731460000001</v>
+        <v>1.2128540000000001</v>
       </c>
       <c r="V191">
-        <v>1.1933731460000001</v>
+        <v>1.2128540000000001</v>
       </c>
       <c r="W191">
-        <v>1.1933731460000001</v>
+        <v>1.2128540000000001</v>
       </c>
       <c r="X191">
-        <v>1.1933731460000001</v>
+        <v>1.2128540000000001</v>
       </c>
       <c r="Y191">
-        <v>1.1933731460000001</v>
+        <v>1.2128540000000001</v>
       </c>
     </row>
     <row r="192" spans="1:25" x14ac:dyDescent="0.2">
@@ -18762,64 +18762,64 @@
         <v>2018</v>
       </c>
       <c r="F192">
-        <v>2.5957141999999999E-3</v>
+        <v>1.3015041E-2</v>
       </c>
       <c r="G192">
-        <v>6.2154965999999999E-2</v>
+        <v>0.16967412000000001</v>
       </c>
       <c r="H192">
-        <v>0.31697612800000002</v>
+        <v>0.44048720000000002</v>
       </c>
       <c r="I192">
-        <v>0.480864293</v>
+        <v>0.51724840000000005</v>
       </c>
       <c r="J192">
-        <v>0.58992315200000001</v>
+        <v>0.59904990000000002</v>
       </c>
       <c r="K192">
-        <v>0.663590664</v>
+        <v>0.66934450000000001</v>
       </c>
       <c r="L192">
-        <v>0.67433940000000003</v>
+        <v>0.67397830000000003</v>
       </c>
       <c r="M192">
-        <v>0.6656128</v>
+        <v>0.66543819999999998</v>
       </c>
       <c r="N192">
-        <v>0.73986490000000005</v>
+        <v>0.73974169999999995</v>
       </c>
       <c r="O192">
-        <v>0.7226129</v>
+        <v>0.72251399999999999</v>
       </c>
       <c r="P192">
-        <v>0.78325219999999995</v>
+        <v>0.78313790000000005</v>
       </c>
       <c r="Q192">
-        <v>0.86520569999999997</v>
+        <v>0.86503140000000001</v>
       </c>
       <c r="R192">
-        <v>1.0013966999999999</v>
+        <v>1.0010359</v>
       </c>
       <c r="S192">
-        <v>1.1630339999999999</v>
+        <v>1.1620628</v>
       </c>
       <c r="T192">
-        <v>1.32987492</v>
+        <v>1.3399433999999999</v>
       </c>
       <c r="U192">
-        <v>1.32987492</v>
+        <v>1.3399433999999999</v>
       </c>
       <c r="V192">
-        <v>1.32987492</v>
+        <v>1.3399433999999999</v>
       </c>
       <c r="W192">
-        <v>1.32987492</v>
+        <v>1.3399433999999999</v>
       </c>
       <c r="X192">
-        <v>1.32987492</v>
+        <v>1.3399433999999999</v>
       </c>
       <c r="Y192">
-        <v>1.32987492</v>
+        <v>1.3399433999999999</v>
       </c>
     </row>
     <row r="193" spans="1:25" x14ac:dyDescent="0.2">
@@ -18839,64 +18839,64 @@
         <v>2019</v>
       </c>
       <c r="F193">
-        <v>8.9370669999999999E-4</v>
+        <v>3.0589089999999998E-3</v>
       </c>
       <c r="G193">
-        <v>2.2110444999999999E-2</v>
+        <v>7.9635209999999998E-2</v>
       </c>
       <c r="H193">
-        <v>0.16217974800000001</v>
+        <v>0.32100869999999998</v>
       </c>
       <c r="I193">
-        <v>0.40788569200000002</v>
+        <v>0.50113339999999995</v>
       </c>
       <c r="J193">
-        <v>0.49893597899999997</v>
+        <v>0.52796650000000001</v>
       </c>
       <c r="K193">
-        <v>0.56232125600000005</v>
+        <v>0.57108369999999997</v>
       </c>
       <c r="L193">
-        <v>0.62728667100000002</v>
+        <v>0.63247880000000001</v>
       </c>
       <c r="M193">
-        <v>0.65966610000000003</v>
+        <v>0.65907899999999997</v>
       </c>
       <c r="N193">
-        <v>0.6378663</v>
+        <v>0.63750459999999998</v>
       </c>
       <c r="O193">
-        <v>0.68515749999999997</v>
+        <v>0.68483729999999998</v>
       </c>
       <c r="P193">
-        <v>0.68330869999999999</v>
+        <v>0.68296840000000003</v>
       </c>
       <c r="Q193">
-        <v>0.74324429999999997</v>
+        <v>0.74273409999999995</v>
       </c>
       <c r="R193">
-        <v>0.77703694199999995</v>
+        <v>0.7839256</v>
       </c>
       <c r="S193">
-        <v>0.90558883800000001</v>
+        <v>0.91215900000000005</v>
       </c>
       <c r="T193">
-        <v>1.082969184</v>
+        <v>1.1186624999999999</v>
       </c>
       <c r="U193">
-        <v>1.082969184</v>
+        <v>1.1186624999999999</v>
       </c>
       <c r="V193">
-        <v>1.082969184</v>
+        <v>1.1186624999999999</v>
       </c>
       <c r="W193">
-        <v>1.082969184</v>
+        <v>1.1186624999999999</v>
       </c>
       <c r="X193">
-        <v>1.082969184</v>
+        <v>1.1186624999999999</v>
       </c>
       <c r="Y193">
-        <v>1.082969184</v>
+        <v>1.1186624999999999</v>
       </c>
     </row>
     <row r="194" spans="1:25" x14ac:dyDescent="0.2">
@@ -18916,64 +18916,64 @@
         <v>2020</v>
       </c>
       <c r="F194">
-        <v>3.2245005000000001E-3</v>
+        <v>1.1292649E-2</v>
       </c>
       <c r="G194">
-        <v>4.9564499999999997E-2</v>
+        <v>0.13051212000000001</v>
       </c>
       <c r="H194">
-        <v>0.32214981500000001</v>
+        <v>0.44146279999999999</v>
       </c>
       <c r="I194">
-        <v>0.50615910799999997</v>
+        <v>0.54443209999999997</v>
       </c>
       <c r="J194">
-        <v>0.608421926</v>
+        <v>0.6177859</v>
       </c>
       <c r="K194">
-        <v>0.57684528000000002</v>
+        <v>0.58182330000000004</v>
       </c>
       <c r="L194">
-        <v>0.61801269999999997</v>
+        <v>0.61766869999999996</v>
       </c>
       <c r="M194">
-        <v>0.70623579999999997</v>
+        <v>0.70604169999999999</v>
       </c>
       <c r="N194">
-        <v>0.72028669999999995</v>
+        <v>0.72016029999999998</v>
       </c>
       <c r="O194">
-        <v>0.67303999999999997</v>
+        <v>0.67294240000000005</v>
       </c>
       <c r="P194">
-        <v>0.73820149999999995</v>
+        <v>0.73808720000000005</v>
       </c>
       <c r="Q194">
-        <v>0.73878849999999996</v>
+        <v>0.73863060000000003</v>
       </c>
       <c r="R194">
-        <v>0.76823109999999994</v>
+        <v>0.7679378</v>
       </c>
       <c r="S194">
-        <v>0.81690090000000004</v>
+        <v>0.81618080000000004</v>
       </c>
       <c r="T194">
-        <v>1.000821789</v>
+        <v>1.0082736000000001</v>
       </c>
       <c r="U194">
-        <v>1.000821789</v>
+        <v>1.0082736000000001</v>
       </c>
       <c r="V194">
-        <v>1.000821789</v>
+        <v>1.0082736000000001</v>
       </c>
       <c r="W194">
-        <v>1.000821789</v>
+        <v>1.0082736000000001</v>
       </c>
       <c r="X194">
-        <v>1.000821789</v>
+        <v>1.0082736000000001</v>
       </c>
       <c r="Y194">
-        <v>1.000821789</v>
+        <v>1.0082736000000001</v>
       </c>
     </row>
     <row r="195" spans="1:25" x14ac:dyDescent="0.2">
@@ -18993,64 +18993,64 @@
         <v>2021</v>
       </c>
       <c r="F195">
-        <v>2.4606393999999998E-3</v>
+        <v>1.0674196E-2</v>
       </c>
       <c r="G195">
-        <v>5.2077919E-2</v>
+        <v>0.14626861999999999</v>
       </c>
       <c r="H195">
-        <v>0.23980314</v>
+        <v>0.34844839999999999</v>
       </c>
       <c r="I195">
-        <v>0.56605185000000002</v>
+        <v>0.61329920000000004</v>
       </c>
       <c r="J195">
-        <v>0.64810193000000005</v>
+        <v>0.6575666</v>
       </c>
       <c r="K195">
-        <v>0.68611029300000004</v>
+        <v>0.69189389999999995</v>
       </c>
       <c r="L195">
-        <v>0.64503140000000003</v>
+        <v>0.64463150000000002</v>
       </c>
       <c r="M195">
-        <v>0.7080012</v>
+        <v>0.7077888</v>
       </c>
       <c r="N195">
-        <v>0.79259009999999996</v>
+        <v>0.79244150000000002</v>
       </c>
       <c r="O195">
-        <v>0.78114980000000001</v>
+        <v>0.78103160000000005</v>
       </c>
       <c r="P195">
-        <v>0.7453206</v>
+        <v>0.7452029</v>
       </c>
       <c r="Q195">
-        <v>0.82034359999999995</v>
+        <v>0.82016909999999998</v>
       </c>
       <c r="R195">
-        <v>0.78487079999999998</v>
+        <v>0.7845801</v>
       </c>
       <c r="S195">
-        <v>0.82181210000000005</v>
+        <v>0.82112759999999996</v>
       </c>
       <c r="T195">
-        <v>0.91864555199999998</v>
+        <v>0.9256818</v>
       </c>
       <c r="U195">
-        <v>0.91864555199999998</v>
+        <v>0.9256818</v>
       </c>
       <c r="V195">
-        <v>0.91864555199999998</v>
+        <v>0.9256818</v>
       </c>
       <c r="W195">
-        <v>0.91864555199999998</v>
+        <v>0.9256818</v>
       </c>
       <c r="X195">
-        <v>0.91864555199999998</v>
+        <v>0.9256818</v>
       </c>
       <c r="Y195">
-        <v>0.91864555199999998</v>
+        <v>0.9256818</v>
       </c>
     </row>
     <row r="196" spans="1:25" x14ac:dyDescent="0.2">
@@ -19070,64 +19070,64 @@
         <v>2022</v>
       </c>
       <c r="F196">
-        <v>2.0431441999999998E-3</v>
+        <v>7.6449420000000001E-3</v>
       </c>
       <c r="G196">
-        <v>5.2805535000000001E-2</v>
+        <v>0.15238477</v>
       </c>
       <c r="H196">
-        <v>0.27775524000000001</v>
+        <v>0.42055809999999999</v>
       </c>
       <c r="I196">
-        <v>0.44808693599999999</v>
+        <v>0.4935349</v>
       </c>
       <c r="J196">
-        <v>0.728222068</v>
+        <v>0.74534350000000005</v>
       </c>
       <c r="K196">
-        <v>0.73373493599999995</v>
+        <v>0.73956500000000003</v>
       </c>
       <c r="L196">
-        <v>0.77023319999999995</v>
+        <v>0.76960589999999995</v>
       </c>
       <c r="M196">
-        <v>0.74186379999999996</v>
+        <v>0.74156610000000001</v>
       </c>
       <c r="N196">
-        <v>0.79770010000000002</v>
+        <v>0.79749650000000005</v>
       </c>
       <c r="O196">
-        <v>0.86294740000000003</v>
+        <v>0.86276640000000004</v>
       </c>
       <c r="P196">
-        <v>0.86844690000000002</v>
+        <v>0.86825350000000001</v>
       </c>
       <c r="Q196">
-        <v>0.83151629999999999</v>
+        <v>0.83126250000000002</v>
       </c>
       <c r="R196">
-        <v>0.87494459999999996</v>
+        <v>0.87447160000000002</v>
       </c>
       <c r="S196">
-        <v>0.83448931500000001</v>
+        <v>0.84187670000000003</v>
       </c>
       <c r="T196">
-        <v>0.91843571400000001</v>
+        <v>0.93376400000000004</v>
       </c>
       <c r="U196">
-        <v>0.91843571400000001</v>
+        <v>0.93376400000000004</v>
       </c>
       <c r="V196">
-        <v>0.91843571400000001</v>
+        <v>0.93376400000000004</v>
       </c>
       <c r="W196">
-        <v>0.91843571400000001</v>
+        <v>0.93376400000000004</v>
       </c>
       <c r="X196">
-        <v>0.91843571400000001</v>
+        <v>0.93376400000000004</v>
       </c>
       <c r="Y196">
-        <v>0.91843571400000001</v>
+        <v>0.93376400000000004</v>
       </c>
     </row>
     <row r="197" spans="1:25" x14ac:dyDescent="0.2">
@@ -19147,64 +19147,64 @@
         <v>2023</v>
       </c>
       <c r="F197">
-        <v>8.7544019999999997E-4</v>
+        <v>4.6825310000000002E-3</v>
       </c>
       <c r="G197">
-        <v>2.9231136000000001E-2</v>
+        <v>9.2155760000000003E-2</v>
       </c>
       <c r="H197">
-        <v>0.23835783199999999</v>
+        <v>0.41158400000000001</v>
       </c>
       <c r="I197">
-        <v>0.47680644799999999</v>
+        <v>0.54920869999999999</v>
       </c>
       <c r="J197">
-        <v>0.53044819200000004</v>
+        <v>0.5467824</v>
       </c>
       <c r="K197">
-        <v>0.75723011100000004</v>
+        <v>0.7624959</v>
       </c>
       <c r="L197">
-        <v>0.74133843300000002</v>
+        <v>0.74793220000000005</v>
       </c>
       <c r="M197">
-        <v>0.80534019999999995</v>
+        <v>0.80486440000000004</v>
       </c>
       <c r="N197">
-        <v>0.75987769999999999</v>
+        <v>0.75959100000000002</v>
       </c>
       <c r="O197">
-        <v>0.78956729999999997</v>
+        <v>0.78932159999999996</v>
       </c>
       <c r="P197">
-        <v>0.87218209999999996</v>
+        <v>0.87189300000000003</v>
       </c>
       <c r="Q197">
-        <v>0.88081509999999996</v>
+        <v>0.88041340000000001</v>
       </c>
       <c r="R197">
-        <v>0.80624929999999995</v>
+        <v>0.80559619999999998</v>
       </c>
       <c r="S197">
-        <v>0.84570126300000004</v>
+        <v>0.85265679999999999</v>
       </c>
       <c r="T197">
-        <v>0.85639799000000005</v>
+        <v>0.86907979999999996</v>
       </c>
       <c r="U197">
-        <v>0.85639799000000005</v>
+        <v>0.86907979999999996</v>
       </c>
       <c r="V197">
-        <v>0.85639799000000005</v>
+        <v>0.86907979999999996</v>
       </c>
       <c r="W197">
-        <v>0.85639799000000005</v>
+        <v>0.86907979999999996</v>
       </c>
       <c r="X197">
-        <v>0.85639799000000005</v>
+        <v>0.86907979999999996</v>
       </c>
       <c r="Y197">
-        <v>0.85639799000000005</v>
+        <v>0.86907979999999996</v>
       </c>
     </row>
     <row r="198" spans="1:25" x14ac:dyDescent="0.2">
@@ -28330,7 +28330,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScale="186" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28453,7 +28453,7 @@
         <v>61</v>
       </c>
       <c r="B15">
-        <v>1.24</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -31454,8 +31454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31680,12 +31680,6 @@
       <c r="Q3">
         <v>3</v>
       </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
       <c r="T3">
         <v>0</v>
       </c>

</xml_diff>